<commit_message>
[ADD] bioapis; still unstable
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1275" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4220C988-5BA0-40A0-A17D-FB6313B8CF63}"/>
   <bookViews>
-    <workbookView xWindow="-17772" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -728,6 +728,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -736,15 +745,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,9 +1062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:BD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BC31" sqref="BC31"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2331,14 +2331,14 @@
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
-      <c r="M13" s="26" t="s">
+      <c r="M13" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="N13" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="O13" s="27"/>
-      <c r="P13" s="28" t="s">
+      <c r="N13" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="24"/>
+      <c r="P13" s="25" t="s">
         <v>76</v>
       </c>
       <c r="Y13" s="8" t="s">
@@ -2364,14 +2364,14 @@
       </c>
     </row>
     <row r="14" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="M14" s="26" t="s">
+      <c r="M14" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="O14" s="27"/>
-      <c r="P14" s="28" t="s">
+      <c r="N14" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" s="24"/>
+      <c r="P14" s="25" t="s">
         <v>76</v>
       </c>
       <c r="Y14" s="8" t="s">
@@ -2500,90 +2500,90 @@
       <c r="AB20" s="20"/>
     </row>
     <row r="21" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="23" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="23" t="s">
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="23" t="s">
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="23" t="s">
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="23" t="s">
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="23" t="s">
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="25"/>
-      <c r="AC21" s="23" t="s">
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AD21" s="24"/>
-      <c r="AE21" s="24"/>
-      <c r="AF21" s="25"/>
-      <c r="AG21" s="23" t="s">
+      <c r="AD21" s="27"/>
+      <c r="AE21" s="27"/>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AH21" s="24"/>
-      <c r="AI21" s="24"/>
-      <c r="AJ21" s="25"/>
-      <c r="AK21" s="23" t="s">
+      <c r="AH21" s="27"/>
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="28"/>
+      <c r="AK21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AL21" s="24"/>
-      <c r="AM21" s="24"/>
-      <c r="AN21" s="25"/>
-      <c r="AO21" s="23" t="s">
+      <c r="AL21" s="27"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="28"/>
+      <c r="AO21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AP21" s="24"/>
-      <c r="AQ21" s="24"/>
-      <c r="AR21" s="25"/>
-      <c r="AS21" s="23" t="s">
+      <c r="AP21" s="27"/>
+      <c r="AQ21" s="27"/>
+      <c r="AR21" s="28"/>
+      <c r="AS21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AT21" s="24"/>
-      <c r="AU21" s="24"/>
-      <c r="AV21" s="25"/>
-      <c r="AW21" s="23" t="s">
+      <c r="AT21" s="27"/>
+      <c r="AU21" s="27"/>
+      <c r="AV21" s="28"/>
+      <c r="AW21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AX21" s="24"/>
-      <c r="AY21" s="24"/>
-      <c r="AZ21" s="25"/>
-      <c r="BA21" s="23" t="s">
+      <c r="AX21" s="27"/>
+      <c r="AY21" s="27"/>
+      <c r="AZ21" s="28"/>
+      <c r="BA21" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="BB21" s="24"/>
-      <c r="BC21" s="24"/>
-      <c r="BD21" s="25"/>
+      <c r="BB21" s="27"/>
+      <c r="BC21" s="27"/>
+      <c r="BD21" s="28"/>
     </row>
     <row r="22" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
@@ -2755,7 +2755,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
[FIX] debugging organism transformer and model
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1275" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4220C988-5BA0-40A0-A17D-FB6313B8CF63}"/>
+  <xr:revisionPtr revIDLastSave="1276" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C95EF9E2-9C04-4D8C-90DB-278F61D685D6}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -462,9 +462,6 @@
     <t>PRT.REG.0.000.000</t>
   </si>
   <si>
-    <t>PRT.RON.0.000.001</t>
-  </si>
-  <si>
     <t>Regulatory Interaction Properties</t>
   </si>
   <si>
@@ -550,6 +547,9 @@
   </si>
   <si>
     <t>regulatory_effect</t>
+  </si>
+  <si>
+    <t>PRT.REN.0.000.001</t>
   </si>
 </sst>
 </file>
@@ -1062,9 +1062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:BD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BC5" sqref="BC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,16 +1286,16 @@
         <v>39</v>
       </c>
       <c r="BA1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB1" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="BB1" s="11" t="s">
+      <c r="BC1" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="BC1" s="11" t="s">
+      <c r="BD1" s="12" t="s">
         <v>145</v>
-      </c>
-      <c r="BD1" s="12" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1528,7 +1528,7 @@
     </row>
     <row r="4" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>60</v>
@@ -1536,7 +1536,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>60</v>
@@ -1544,7 +1544,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
       <c r="I4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>60</v>
@@ -1552,7 +1552,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="6"/>
       <c r="M4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>60</v>
@@ -1560,7 +1560,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>60</v>
@@ -1568,7 +1568,7 @@
       <c r="S4" s="5"/>
       <c r="T4" s="6"/>
       <c r="U4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>60</v>
@@ -1576,7 +1576,7 @@
       <c r="W4" s="5"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>60</v>
@@ -1584,7 +1584,7 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>60</v>
@@ -1592,7 +1592,7 @@
       <c r="AE4" s="5"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AH4" s="5" t="s">
         <v>60</v>
@@ -1600,7 +1600,7 @@
       <c r="AI4" s="5"/>
       <c r="AJ4" s="6"/>
       <c r="AK4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AL4" s="5" t="s">
         <v>60</v>
@@ -1608,7 +1608,7 @@
       <c r="AM4" s="5"/>
       <c r="AN4" s="6"/>
       <c r="AO4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AP4" s="5" t="s">
         <v>60</v>
@@ -1616,7 +1616,7 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="6"/>
       <c r="AS4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AT4" s="5" t="s">
         <v>60</v>
@@ -1624,7 +1624,7 @@
       <c r="AU4" s="5"/>
       <c r="AV4" s="6"/>
       <c r="AW4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AX4" s="5" t="s">
         <v>60</v>
@@ -1632,7 +1632,7 @@
       <c r="AY4" s="5"/>
       <c r="AZ4" s="6"/>
       <c r="BA4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BB4" s="5" t="s">
         <v>60</v>
@@ -1768,7 +1768,7 @@
         <v>56</v>
       </c>
       <c r="AY5" s="5" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="AZ5" s="6"/>
       <c r="BA5" s="4" t="s">
@@ -1778,7 +1778,7 @@
         <v>56</v>
       </c>
       <c r="BC5" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="BD5" s="6"/>
     </row>
@@ -1835,7 +1835,7 @@
         <v>56</v>
       </c>
       <c r="AB6" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AC6" s="7" t="s">
         <v>1</v>
@@ -1917,7 +1917,7 @@
         <v>72</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>56</v>
@@ -1941,7 +1941,7 @@
         <v>91</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AD7" s="13" t="s">
         <v>9</v>
@@ -1981,10 +1981,10 @@
         <v>56</v>
       </c>
       <c r="AU7" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AW7" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AX7" s="8" t="s">
         <v>9</v>
@@ -2065,7 +2065,7 @@
         <v>74</v>
       </c>
       <c r="AS8" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AT8" s="8" t="s">
         <v>56</v>
@@ -2127,7 +2127,7 @@
         <v>114</v>
       </c>
       <c r="AC9" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD9" s="13" t="s">
         <v>9</v>
@@ -2155,13 +2155,13 @@
         <v>74</v>
       </c>
       <c r="AW9" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AX9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="BA9" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BB9" s="8" t="s">
         <v>9</v>
@@ -2229,7 +2229,7 @@
         <v>140</v>
       </c>
       <c r="BA10" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="BB10" s="8" t="s">
         <v>9</v>
@@ -2243,7 +2243,7 @@
         <v>56</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>74</v>
@@ -2264,7 +2264,7 @@
         <v>74</v>
       </c>
       <c r="AK11" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AL11" s="8" t="s">
         <v>74</v>
@@ -2274,7 +2274,7 @@
         <v>97</v>
       </c>
       <c r="BA11" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="BB11" s="8" t="s">
         <v>56</v>
@@ -2289,7 +2289,7 @@
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="M12" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>56</v>
@@ -2316,7 +2316,7 @@
         <v>74</v>
       </c>
       <c r="AK12" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AL12" s="8" t="s">
         <v>74</v>
@@ -2342,7 +2342,7 @@
         <v>76</v>
       </c>
       <c r="Y13" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Z13" s="8" t="s">
         <v>74</v>
@@ -2351,7 +2351,7 @@
         <v>97</v>
       </c>
       <c r="AK13" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AL13" s="8" t="s">
         <v>56</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="15" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="Y15" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z15" s="8" t="s">
         <v>56</v>
@@ -2501,85 +2501,85 @@
     </row>
     <row r="21" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
       <c r="D21" s="28"/>
       <c r="E21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="28"/>
       <c r="I21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
       <c r="L21" s="28"/>
       <c r="M21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N21" s="27"/>
       <c r="O21" s="27"/>
       <c r="P21" s="28"/>
       <c r="Q21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="28"/>
       <c r="U21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="V21" s="27"/>
       <c r="W21" s="27"/>
       <c r="X21" s="28"/>
       <c r="Y21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Z21" s="27"/>
       <c r="AA21" s="27"/>
       <c r="AB21" s="28"/>
       <c r="AC21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AD21" s="27"/>
       <c r="AE21" s="27"/>
       <c r="AF21" s="28"/>
       <c r="AG21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AH21" s="27"/>
       <c r="AI21" s="27"/>
       <c r="AJ21" s="28"/>
       <c r="AK21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL21" s="27"/>
       <c r="AM21" s="27"/>
       <c r="AN21" s="28"/>
       <c r="AO21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AP21" s="27"/>
       <c r="AQ21" s="27"/>
       <c r="AR21" s="28"/>
       <c r="AS21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AT21" s="27"/>
       <c r="AU21" s="27"/>
       <c r="AV21" s="28"/>
       <c r="AW21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AX21" s="27"/>
       <c r="AY21" s="27"/>
       <c r="AZ21" s="28"/>
       <c r="BA21" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BB21" s="27"/>
       <c r="BC21" s="27"/>
@@ -2587,172 +2587,172 @@
     </row>
     <row r="22" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="D22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="G22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="G22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="H22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="J22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="K22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="K22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="L22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="N22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="N22" s="17" t="s">
+      <c r="O22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="O22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="P22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="R22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="R22" s="17" t="s">
+      <c r="S22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="S22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="T22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="V22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="V22" s="17" t="s">
+      <c r="W22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="W22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="X22" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y22" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="Z22" s="17" t="s">
+      <c r="AA22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AA22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="AB22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AC22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AD22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="AD22" s="17" t="s">
+      <c r="AE22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AE22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="AF22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AG22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="AH22" s="17" t="s">
+      <c r="AI22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AI22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="AJ22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AK22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="AL22" s="17" t="s">
+      <c r="AM22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AM22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="AN22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AO22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="AP22" s="17" t="s">
+      <c r="AQ22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AQ22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="AR22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AS22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AT22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="AT22" s="17" t="s">
+      <c r="AU22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AU22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="AV22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AW22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AX22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="AX22" s="17" t="s">
+      <c r="AY22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AY22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="AZ22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BA22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="BB22" s="17" t="s">
+      <c r="BC22" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="BC22" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="BD22" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
@@ -2760,160 +2760,160 @@
         <v>0</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="R23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="V23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Y23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="Z23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AC23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="AD23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="AH23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AK23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="AL23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AO23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="AP23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AS23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="AT23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AU23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AV23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="AX23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AZ23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BA23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="BB23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC23" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD23" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.3">
@@ -2921,129 +2921,129 @@
         <v>20</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="R24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T24" s="9"/>
       <c r="U24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="V24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y24" s="7" t="s">
         <v>126</v>
       </c>
       <c r="Z24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC24" s="7" t="s">
         <v>126</v>
       </c>
       <c r="AD24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG24" s="7" t="s">
         <v>126</v>
       </c>
       <c r="AH24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK24" s="7" t="s">
         <v>126</v>
       </c>
       <c r="AL24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN24" s="9"/>
       <c r="AO24" s="7" t="s">
         <v>126</v>
       </c>
       <c r="AP24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AT24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AU24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW24" s="7" t="s">
         <v>126</v>
       </c>
       <c r="AX24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BA24" s="7" t="s">
         <v>126</v>
       </c>
       <c r="BB24" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
@@ -3051,128 +3051,128 @@
         <v>44</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>44</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M25" s="7" t="s">
         <v>12</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q25" s="7" t="s">
         <v>12</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U25" s="7" t="s">
         <v>12</v>
       </c>
       <c r="V25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="Z25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AD25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AH25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AL25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN25" s="9"/>
       <c r="AO25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AP25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS25" s="7" t="s">
         <v>0</v>
       </c>
       <c r="AT25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AU25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="AX25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BA25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BB25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC25" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.3">
@@ -3180,52 +3180,52 @@
         <v>12</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>10</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q26" s="7" t="s">
         <v>17</v>
       </c>
       <c r="R26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y26" s="8" t="s">
         <v>0</v>
       </c>
       <c r="Z26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA26" s="8">
         <v>1</v>
@@ -3234,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="AD26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE26" s="8">
         <v>1</v>
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="AH26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI26" s="8">
         <v>1</v>
@@ -3252,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="AL26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM26" s="8">
         <v>1</v>
@@ -3262,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="AP26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ26" s="8">
         <v>1</v>
@@ -3271,16 +3271,16 @@
         <v>12</v>
       </c>
       <c r="AT26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AU26" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AW26" s="8" t="s">
         <v>0</v>
       </c>
       <c r="AX26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY26" s="8">
         <v>1</v>
@@ -3289,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="BB26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC26" s="8">
         <v>1</v>
@@ -3300,61 +3300,61 @@
         <v>10</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>10</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>11</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y27" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Z27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA27" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC27" s="7" t="s">
         <v>12</v>
       </c>
       <c r="AD27" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE27" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG27" s="7" t="s">
         <v>10</v>
       </c>
       <c r="AH27" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI27" s="8">
         <v>1</v>
@@ -3363,19 +3363,19 @@
         <v>20</v>
       </c>
       <c r="AL27" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM27" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO27" s="7" t="s">
         <v>12</v>
       </c>
       <c r="AP27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ27" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR27" s="9" t="s">
         <v>54</v>
@@ -3384,27 +3384,27 @@
         <v>19</v>
       </c>
       <c r="AT27" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AU27" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AV27" s="20"/>
       <c r="AW27" s="7" t="s">
         <v>12</v>
       </c>
       <c r="AX27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY27" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AZ27" s="20"/>
       <c r="BA27" s="7" t="s">
         <v>12</v>
       </c>
       <c r="BB27" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC27" s="8">
         <v>1</v>
@@ -3416,43 +3416,43 @@
         <v>11</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M28" s="7" t="s">
         <v>17</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y28" s="8" t="s">
         <v>44</v>
       </c>
       <c r="Z28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA28" s="8">
         <v>1</v>
@@ -3461,19 +3461,19 @@
         <v>11</v>
       </c>
       <c r="AD28" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE28" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG28" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AH28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI28" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AJ28" s="9" t="s">
         <v>54</v>
@@ -3482,10 +3482,10 @@
         <v>12</v>
       </c>
       <c r="AL28" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM28" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN28" s="16" t="s">
         <v>54</v>
@@ -3494,7 +3494,7 @@
         <v>10</v>
       </c>
       <c r="AP28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ28" s="8">
         <v>1</v>
@@ -3503,17 +3503,17 @@
         <v>10</v>
       </c>
       <c r="AX28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY28" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AZ28" s="20"/>
       <c r="BA28" s="7" t="s">
         <v>10</v>
       </c>
       <c r="BB28" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC28" s="8">
         <v>1</v>
@@ -3525,61 +3525,61 @@
         <v>17</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M29" s="7" t="s">
         <v>16</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y29" s="8" t="s">
         <v>10</v>
       </c>
       <c r="Z29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA29" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC29" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AD29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE29" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AK29" s="7" t="s">
         <v>10</v>
       </c>
       <c r="AL29" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM29" s="8">
         <v>1</v>
@@ -3589,10 +3589,10 @@
         <v>17</v>
       </c>
       <c r="AP29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ29" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AR29" s="9" t="s">
         <v>54</v>
@@ -3601,10 +3601,10 @@
         <v>17</v>
       </c>
       <c r="AX29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY29" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AZ29" s="20" t="s">
         <v>54</v>
@@ -3613,10 +3613,10 @@
         <v>17</v>
       </c>
       <c r="BB29" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC29" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BD29" s="20" t="s">
         <v>54</v>
@@ -3627,37 +3627,37 @@
         <v>16</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M30" s="7" t="s">
         <v>18</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y30" s="8" t="s">
         <v>17</v>
       </c>
       <c r="Z30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB30" s="9" t="s">
         <v>54</v>
@@ -3666,19 +3666,19 @@
         <v>16</v>
       </c>
       <c r="AD30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK30" s="8" t="s">
         <v>11</v>
       </c>
       <c r="AL30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN30" s="9" t="s">
         <v>54</v>
@@ -3687,10 +3687,10 @@
         <v>15</v>
       </c>
       <c r="AP30" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ30" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR30" s="20" t="s">
         <v>54</v>
@@ -3699,10 +3699,10 @@
         <v>16</v>
       </c>
       <c r="AX30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AY30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AZ30" s="20" t="s">
         <v>54</v>
@@ -3711,10 +3711,10 @@
         <v>16</v>
       </c>
       <c r="BB30" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC30" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD30" s="20" t="s">
         <v>54</v>
@@ -3725,37 +3725,37 @@
         <v>18</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>18</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M31" s="7" t="s">
         <v>15</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y31" s="8" t="s">
         <v>16</v>
       </c>
       <c r="Z31" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB31" s="9" t="s">
         <v>54</v>
@@ -3764,20 +3764,20 @@
         <v>15</v>
       </c>
       <c r="AD31" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF31" s="20"/>
       <c r="AK31" s="15" t="s">
         <v>16</v>
       </c>
       <c r="AL31" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM31" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN31" s="16" t="s">
         <v>54</v>
@@ -3786,10 +3786,10 @@
         <v>19</v>
       </c>
       <c r="AP31" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AQ31" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR31" s="20" t="s">
         <v>54</v>
@@ -3798,10 +3798,10 @@
         <v>18</v>
       </c>
       <c r="BB31" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BC31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD31" s="20"/>
     </row>
@@ -3810,56 +3810,56 @@
         <v>15</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M32" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y32" s="8" t="s">
         <v>18</v>
       </c>
       <c r="Z32" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA32" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC32" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AD32" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE32" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF32" s="20"/>
       <c r="AK32" s="15" t="s">
         <v>15</v>
       </c>
       <c r="AL32" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM32" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN32" s="20" t="s">
         <v>54</v>
@@ -3870,38 +3870,38 @@
         <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y33" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Z33" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA33" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB33" s="20"/>
       <c r="AK33" s="15" t="s">
         <v>19</v>
       </c>
       <c r="AL33" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AM33" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN33" s="20" t="s">
         <v>54</v>
@@ -3912,10 +3912,10 @@
         <v>19</v>
       </c>
       <c r="Z34" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB34" s="20"/>
     </row>

</xml_diff>

<commit_message>
[ADD] stack csv, source transformer
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1276" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C95EF9E2-9C04-4D8C-90DB-278F61D685D6}"/>
+  <xr:revisionPtr revIDLastSave="1278" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD790535-5876-497D-8956-124B5E34CDFA}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="173">
   <si>
     <t>Organism</t>
   </si>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t>PRT.REN.0.000.001</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
 </sst>
 </file>
@@ -1062,9 +1065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:BD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BC5" sqref="BC5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2284,8 +2287,12 @@
       </c>
     </row>
     <row r="12" spans="1:56" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="M12" s="7" t="s">

</xml_diff>

<commit_message>
[REFACTOR] major transform refactoring and simplification; [ADD] transform settings
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -1065,9 +1065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:BD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[ADD] annotation color scheme
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1436" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D56A3FCC-0EEC-4821-AC2A-CDAE0D4194CB}"/>
+  <xr:revisionPtr revIDLastSave="1507" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84069A16-61A3-4568-8016-35BC59F724E9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="173">
   <si>
     <t>Organism</t>
   </si>
@@ -549,35 +549,17 @@
     <t>kegg_compounds</t>
   </si>
   <si>
-    <t>using operon to connect regulator to gene and tfbs</t>
-  </si>
-  <si>
-    <t>using regulator to connect operon to organism</t>
-  </si>
-  <si>
-    <t>using operon to connect regulator to gene</t>
-  </si>
-  <si>
-    <t>using operon to connect regulator to tfbs</t>
-  </si>
-  <si>
-    <t>using operon to connect gene to tfbs</t>
-  </si>
-  <si>
-    <t>using operon to connect tfbs to gene</t>
-  </si>
-  <si>
-    <t>using regulator to connect gene to organism</t>
-  </si>
-  <si>
-    <t>using regulator to connect tfbs to organism</t>
+    <t>Color scheme</t>
+  </si>
+  <si>
+    <t>red - identifier; yellow - implemented; green - ready</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,9 +582,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -689,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -760,14 +754,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,13 +1090,13 @@
   <dimension ref="A1:BD40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" style="7" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" style="8" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="9" customWidth="1"/>
@@ -1135,7 +1140,7 @@
     <col min="42" max="42" width="11.77734375" style="8" customWidth="1"/>
     <col min="43" max="43" width="12.44140625" style="8" customWidth="1"/>
     <col min="44" max="44" width="11.21875" style="9" customWidth="1"/>
-    <col min="45" max="45" width="11.88671875" style="7" customWidth="1"/>
+    <col min="45" max="45" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="12.44140625" style="8" customWidth="1"/>
     <col min="47" max="47" width="14.33203125" style="8" customWidth="1"/>
     <col min="48" max="48" width="13.21875" style="9" customWidth="1"/>
@@ -2795,7 +2800,7 @@
       </c>
     </row>
     <row r="24" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -2804,7 +2809,7 @@
       <c r="C24" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2813,7 +2818,7 @@
       <c r="G24" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I24" s="26" t="s">
+      <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="8" t="s">
@@ -2822,7 +2827,7 @@
       <c r="K24" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M24" s="21" t="s">
+      <c r="M24" s="27" t="s">
         <v>21</v>
       </c>
       <c r="N24" s="8" t="s">
@@ -2834,7 +2839,7 @@
       <c r="P24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q24" s="21" t="s">
+      <c r="Q24" s="27" t="s">
         <v>21</v>
       </c>
       <c r="R24" s="8" t="s">
@@ -2846,7 +2851,7 @@
       <c r="T24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="U24" s="21" t="s">
+      <c r="U24" s="27" t="s">
         <v>21</v>
       </c>
       <c r="V24" s="8" t="s">
@@ -2858,7 +2863,7 @@
       <c r="X24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Y24" s="21" t="s">
+      <c r="Y24" s="27" t="s">
         <v>21</v>
       </c>
       <c r="Z24" s="8" t="s">
@@ -2870,7 +2875,7 @@
       <c r="AB24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="AC24" s="21" t="s">
+      <c r="AC24" s="27" t="s">
         <v>21</v>
       </c>
       <c r="AD24" s="8" t="s">
@@ -2885,78 +2890,78 @@
       <c r="AG24" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="AH24" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI24" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ24" s="9" t="s">
+      <c r="AH24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AK24" s="21" t="s">
+      <c r="AK24" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="AL24" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM24" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN24" s="9" t="s">
+      <c r="AL24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AO24" s="21" t="s">
+      <c r="AO24" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="AP24" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ24" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AR24" s="9" t="s">
+      <c r="AP24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AS24" s="21" t="s">
+      <c r="AS24" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="AT24" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU24" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AV24" s="9" t="s">
+      <c r="AT24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AW24" s="26" t="s">
+      <c r="AW24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AX24" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY24" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AZ24" s="9" t="s">
+      <c r="AX24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AZ24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="BA24" s="26" t="s">
+      <c r="BA24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="BB24" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC24" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="BD24" s="9" t="s">
+      <c r="BB24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD24" s="6" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -2965,7 +2970,7 @@
       <c r="C25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -2974,7 +2979,7 @@
       <c r="G25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J25" s="8" t="s">
@@ -2983,7 +2988,7 @@
       <c r="K25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M25" s="26" t="s">
+      <c r="M25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="N25" s="8" t="s">
@@ -2992,7 +2997,7 @@
       <c r="O25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Q25" s="26" t="s">
+      <c r="Q25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="R25" s="8" t="s">
@@ -3002,7 +3007,7 @@
         <v>147</v>
       </c>
       <c r="T25" s="9"/>
-      <c r="U25" s="21" t="s">
+      <c r="U25" s="28" t="s">
         <v>22</v>
       </c>
       <c r="V25" s="8" t="s">
@@ -3011,7 +3016,7 @@
       <c r="W25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y25" s="26" t="s">
+      <c r="Y25" s="4" t="s">
         <v>120</v>
       </c>
       <c r="Z25" s="8" t="s">
@@ -3020,7 +3025,7 @@
       <c r="AA25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AC25" s="26" t="s">
+      <c r="AC25" s="4" t="s">
         <v>120</v>
       </c>
       <c r="AD25" s="8" t="s">
@@ -3029,64 +3034,69 @@
       <c r="AE25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AG25" s="26" t="s">
+      <c r="AG25" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AH25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK25" s="26" t="s">
+      <c r="AH25" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AL25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN25" s="9"/>
-      <c r="AO25" s="26" t="s">
+      <c r="AL25" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AP25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AS25" s="26" t="s">
+      <c r="AP25" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR25" s="6"/>
+      <c r="AS25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AT25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AW25" s="26" t="s">
+      <c r="AT25" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV25" s="6"/>
+      <c r="AW25" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AX25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="BA25" s="26" t="s">
+      <c r="AX25" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AZ25" s="6"/>
+      <c r="BA25" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="BB25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC25" s="8" t="s">
-        <v>147</v>
-      </c>
+      <c r="BB25" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD25" s="6"/>
     </row>
     <row r="26" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -3095,7 +3105,7 @@
       <c r="C26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="8" t="s">
@@ -3104,7 +3114,7 @@
       <c r="G26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="28" t="s">
         <v>42</v>
       </c>
       <c r="J26" s="8" t="s">
@@ -3113,7 +3123,7 @@
       <c r="K26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M26" s="21" t="s">
+      <c r="M26" s="28" t="s">
         <v>12</v>
       </c>
       <c r="N26" s="8" t="s">
@@ -3122,7 +3132,7 @@
       <c r="O26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Q26" s="21" t="s">
+      <c r="Q26" s="28" t="s">
         <v>12</v>
       </c>
       <c r="R26" s="8" t="s">
@@ -3131,7 +3141,7 @@
       <c r="S26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="U26" s="21" t="s">
+      <c r="U26" s="28" t="s">
         <v>12</v>
       </c>
       <c r="V26" s="8" t="s">
@@ -3140,7 +3150,7 @@
       <c r="W26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y26" s="26" t="s">
+      <c r="Y26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="Z26" s="8" t="s">
@@ -3149,7 +3159,7 @@
       <c r="AA26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AC26" s="26" t="s">
+      <c r="AC26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="AD26" s="8" t="s">
@@ -3158,64 +3168,69 @@
       <c r="AE26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AG26" s="26" t="s">
+      <c r="AG26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AH26" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI26" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK26" s="26" t="s">
+      <c r="AH26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AL26" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM26" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="26" t="s">
+      <c r="AL26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AP26" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ26" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AS26" s="26" t="s">
+      <c r="AP26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR26" s="6"/>
+      <c r="AS26" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AT26" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU26" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AW26" s="26" t="s">
+      <c r="AT26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV26" s="6"/>
+      <c r="AW26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AX26" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY26" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="BA26" s="26" t="s">
+      <c r="AX26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AZ26" s="6"/>
+      <c r="BA26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="BB26" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC26" s="8" t="s">
-        <v>147</v>
-      </c>
+      <c r="BB26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD26" s="6"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="27" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3224,7 +3239,7 @@
       <c r="C27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -3233,7 +3248,7 @@
       <c r="G27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I27" s="26" t="s">
+      <c r="I27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J27" s="8" t="s">
@@ -3242,7 +3257,7 @@
       <c r="K27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M27" s="21" t="s">
+      <c r="M27" s="28" t="s">
         <v>10</v>
       </c>
       <c r="N27" s="8" t="s">
@@ -3251,7 +3266,7 @@
       <c r="O27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Q27" s="26" t="s">
+      <c r="Q27" s="28" t="s">
         <v>17</v>
       </c>
       <c r="R27" s="8" t="s">
@@ -3260,7 +3275,7 @@
       <c r="S27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y27" s="17" t="s">
+      <c r="Y27" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Z27" s="8" t="s">
@@ -3269,7 +3284,7 @@
       <c r="AA27" s="8">
         <v>1</v>
       </c>
-      <c r="AC27" s="17" t="s">
+      <c r="AC27" s="29" t="s">
         <v>0</v>
       </c>
       <c r="AD27" s="8" t="s">
@@ -3278,64 +3293,69 @@
       <c r="AE27" s="8">
         <v>1</v>
       </c>
-      <c r="AG27" s="27" t="s">
+      <c r="AG27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AH27" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI27" s="8">
+      <c r="AH27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI27" s="5">
         <v>1</v>
       </c>
-      <c r="AK27" s="17" t="s">
+      <c r="AJ27" s="6"/>
+      <c r="AK27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AL27" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM27" s="8">
+      <c r="AL27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM27" s="5">
         <v>1</v>
       </c>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="17" t="s">
+      <c r="AN27" s="6"/>
+      <c r="AO27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AP27" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ27" s="8">
+      <c r="AP27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ27" s="5">
         <v>1</v>
       </c>
-      <c r="AS27" s="21" t="s">
+      <c r="AR27" s="6"/>
+      <c r="AS27" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AT27" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU27" s="8" t="s">
+      <c r="AT27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU27" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AW27" s="27" t="s">
+      <c r="AV27" s="6"/>
+      <c r="AW27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AX27" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY27" s="8">
+      <c r="AX27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY27" s="5">
         <v>1</v>
       </c>
-      <c r="BA27" s="26" t="s">
+      <c r="AZ27" s="6"/>
+      <c r="BA27" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BB27" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC27" s="8">
+      <c r="BB27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC27" s="5">
         <v>1</v>
       </c>
+      <c r="BD27" s="6"/>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -3344,7 +3364,7 @@
       <c r="C28" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -3353,7 +3373,7 @@
       <c r="G28" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I28" s="26" t="s">
+      <c r="I28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="8" t="s">
@@ -3362,7 +3382,7 @@
       <c r="K28" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M28" s="26" t="s">
+      <c r="M28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="N28" s="8" t="s">
@@ -3371,7 +3391,7 @@
       <c r="O28" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y28" s="17" t="s">
+      <c r="Y28" s="29" t="s">
         <v>20</v>
       </c>
       <c r="Z28" s="8" t="s">
@@ -3380,7 +3400,7 @@
       <c r="AA28" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AC28" s="21" t="s">
+      <c r="AC28" s="28" t="s">
         <v>12</v>
       </c>
       <c r="AD28" s="19" t="s">
@@ -3389,66 +3409,68 @@
       <c r="AE28" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AG28" s="26" t="s">
+      <c r="AG28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AH28" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI28" s="8">
+      <c r="AH28" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI28" s="5">
         <v>1</v>
       </c>
-      <c r="AK28" s="28" t="s">
+      <c r="AJ28" s="6"/>
+      <c r="AK28" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="AL28" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM28" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AO28" s="21" t="s">
+      <c r="AL28" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM28" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN28" s="30"/>
+      <c r="AO28" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AP28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AR28" s="9" t="s">
+      <c r="AP28" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ28" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AS28" s="28" t="s">
+      <c r="AS28" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AT28" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU28" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AV28" s="20"/>
-      <c r="AW28" s="26" t="s">
+      <c r="AT28" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU28" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV28" s="31"/>
+      <c r="AW28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AX28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY28" s="8" t="s">
+      <c r="AX28" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY28" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AZ28" s="20"/>
-      <c r="BA28" s="26" t="s">
+      <c r="AZ28" s="31"/>
+      <c r="BA28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="BB28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC28" s="8">
+      <c r="BB28" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC28" s="5">
         <v>1</v>
       </c>
-      <c r="BD28" s="20"/>
+      <c r="BD28" s="31"/>
     </row>
     <row r="29" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
@@ -3460,7 +3482,7 @@
       <c r="C29" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="8" t="s">
@@ -3469,7 +3491,7 @@
       <c r="G29" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I29" s="26" t="s">
+      <c r="I29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J29" s="8" t="s">
@@ -3478,7 +3500,7 @@
       <c r="K29" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M29" s="21" t="s">
+      <c r="M29" s="28" t="s">
         <v>17</v>
       </c>
       <c r="N29" s="8" t="s">
@@ -3487,7 +3509,7 @@
       <c r="O29" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y29" s="17" t="s">
+      <c r="Y29" s="29" t="s">
         <v>42</v>
       </c>
       <c r="Z29" s="8" t="s">
@@ -3496,7 +3518,7 @@
       <c r="AA29" s="8">
         <v>1</v>
       </c>
-      <c r="AC29" s="26" t="s">
+      <c r="AC29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD29" s="19" t="s">
@@ -3505,62 +3527,67 @@
       <c r="AE29" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AG29" s="27" t="s">
+      <c r="AG29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AH29" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI29" s="8" t="s">
+      <c r="AH29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI29" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AJ29" s="9" t="s">
+      <c r="AJ29" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AK29" s="29" t="s">
+      <c r="AK29" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="AL29" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM29" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN29" s="16" t="s">
+      <c r="AL29" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM29" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN29" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="AO29" s="21" t="s">
+      <c r="AO29" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="AP29" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ29" s="8">
+      <c r="AP29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ29" s="5">
         <v>1</v>
       </c>
-      <c r="AW29" s="26" t="s">
+      <c r="AR29" s="6"/>
+      <c r="AS29" s="4"/>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="5"/>
+      <c r="AV29" s="6"/>
+      <c r="AW29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AX29" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY29" s="8" t="s">
+      <c r="AX29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY29" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AZ29" s="20"/>
-      <c r="BA29" s="26" t="s">
+      <c r="AZ29" s="31"/>
+      <c r="BA29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="BB29" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC29" s="8">
+      <c r="BB29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC29" s="5">
         <v>1</v>
       </c>
-      <c r="BD29" s="20"/>
+      <c r="BD29" s="31"/>
     </row>
     <row r="30" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -3569,7 +3596,7 @@
       <c r="C30" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F30" s="8" t="s">
@@ -3578,7 +3605,7 @@
       <c r="G30" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="I30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J30" s="8" t="s">
@@ -3587,7 +3614,7 @@
       <c r="K30" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M30" s="21" t="s">
+      <c r="M30" s="28" t="s">
         <v>16</v>
       </c>
       <c r="N30" s="8" t="s">
@@ -3596,7 +3623,7 @@
       <c r="O30" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y30" s="17" t="s">
+      <c r="Y30" s="29" t="s">
         <v>10</v>
       </c>
       <c r="Z30" s="8" t="s">
@@ -3605,7 +3632,7 @@
       <c r="AA30" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AC30" s="17" t="s">
+      <c r="AC30" s="29" t="s">
         <v>17</v>
       </c>
       <c r="AD30" s="8" t="s">
@@ -3614,55 +3641,63 @@
       <c r="AE30" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="AK30" s="21" t="s">
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="33"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="6"/>
+      <c r="AK30" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="AL30" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM30" s="8">
+      <c r="AL30" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM30" s="5">
         <v>1</v>
       </c>
-      <c r="AN30" s="9"/>
-      <c r="AO30" s="21" t="s">
+      <c r="AN30" s="6"/>
+      <c r="AO30" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="AP30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ30" s="8" t="s">
+      <c r="AP30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ30" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AR30" s="9" t="s">
+      <c r="AR30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AW30" s="26" t="s">
+      <c r="AS30" s="4"/>
+      <c r="AT30" s="5"/>
+      <c r="AU30" s="5"/>
+      <c r="AV30" s="6"/>
+      <c r="AW30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AX30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY30" s="8" t="s">
+      <c r="AX30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY30" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AZ30" s="20" t="s">
+      <c r="AZ30" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="BA30" s="26" t="s">
+      <c r="BA30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="BB30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC30" s="8" t="s">
+      <c r="BB30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC30" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="BD30" s="20" t="s">
+      <c r="BD30" s="31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3671,7 +3706,7 @@
       <c r="C31" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I31" s="26" t="s">
+      <c r="I31" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J31" s="8" t="s">
@@ -3680,7 +3715,7 @@
       <c r="K31" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M31" s="26" t="s">
+      <c r="M31" s="28" t="s">
         <v>18</v>
       </c>
       <c r="N31" s="8" t="s">
@@ -3689,7 +3724,7 @@
       <c r="O31" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y31" s="17" t="s">
+      <c r="Y31" s="29" t="s">
         <v>17</v>
       </c>
       <c r="Z31" s="8" t="s">
@@ -3701,7 +3736,7 @@
       <c r="AB31" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AC31" s="17" t="s">
+      <c r="AC31" s="29" t="s">
         <v>16</v>
       </c>
       <c r="AD31" s="8" t="s">
@@ -3710,57 +3745,65 @@
       <c r="AE31" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AK31" s="27" t="s">
+      <c r="AG31" s="4"/>
+      <c r="AH31" s="33"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="6"/>
+      <c r="AK31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AL31" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM31" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN31" s="9" t="s">
+      <c r="AL31" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AO31" s="28" t="s">
+      <c r="AO31" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="AP31" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ31" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AR31" s="20" t="s">
+      <c r="AP31" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ31" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR31" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="AW31" s="26" t="s">
+      <c r="AS31" s="4"/>
+      <c r="AT31" s="5"/>
+      <c r="AU31" s="5"/>
+      <c r="AV31" s="6"/>
+      <c r="AW31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AX31" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY31" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AZ31" s="20" t="s">
+      <c r="AX31" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AZ31" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="BA31" s="26" t="s">
+      <c r="BA31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="BB31" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC31" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="BD31" s="20" t="s">
+      <c r="BB31" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD31" s="31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="27" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -3769,7 +3812,7 @@
       <c r="C32" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I32" s="26" t="s">
+      <c r="I32" s="4" t="s">
         <v>18</v>
       </c>
       <c r="J32" s="8" t="s">
@@ -3778,7 +3821,7 @@
       <c r="K32" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M32" s="26" t="s">
+      <c r="M32" s="4" t="s">
         <v>15</v>
       </c>
       <c r="N32" s="8" t="s">
@@ -3787,7 +3830,7 @@
       <c r="O32" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y32" s="17" t="s">
+      <c r="Y32" s="29" t="s">
         <v>16</v>
       </c>
       <c r="Z32" s="8" t="s">
@@ -3799,7 +3842,7 @@
       <c r="AB32" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AC32" s="27" t="s">
+      <c r="AC32" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AD32" s="8" t="s">
@@ -3809,42 +3852,54 @@
         <v>147</v>
       </c>
       <c r="AF32" s="20"/>
-      <c r="AK32" s="29" t="s">
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="33"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="6"/>
+      <c r="AK32" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AL32" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM32" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN32" s="16" t="s">
+      <c r="AL32" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM32" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN32" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="AO32" s="28" t="s">
+      <c r="AO32" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AP32" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ32" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AR32" s="20" t="s">
+      <c r="AP32" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ32" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR32" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="BA32" s="26" t="s">
+      <c r="AS32" s="4"/>
+      <c r="AT32" s="5"/>
+      <c r="AU32" s="5"/>
+      <c r="AV32" s="6"/>
+      <c r="AW32" s="4"/>
+      <c r="AX32" s="5"/>
+      <c r="AY32" s="5"/>
+      <c r="AZ32" s="6"/>
+      <c r="BA32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="BB32" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC32" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="BD32" s="20"/>
+      <c r="BB32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC32" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD32" s="31"/>
     </row>
-    <row r="33" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -3854,7 +3909,7 @@
       <c r="C33" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I33" s="26" t="s">
+      <c r="I33" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J33" s="8" t="s">
@@ -3863,7 +3918,7 @@
       <c r="K33" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M33" s="26" t="s">
+      <c r="M33" s="4" t="s">
         <v>19</v>
       </c>
       <c r="N33" s="8" t="s">
@@ -3872,7 +3927,7 @@
       <c r="O33" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y33" s="17" t="s">
+      <c r="Y33" s="29" t="s">
         <v>18</v>
       </c>
       <c r="Z33" s="8" t="s">
@@ -3881,7 +3936,7 @@
       <c r="AA33" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AC33" s="27" t="s">
+      <c r="AC33" s="5" t="s">
         <v>19</v>
       </c>
       <c r="AD33" s="8" t="s">
@@ -3891,20 +3946,40 @@
         <v>147</v>
       </c>
       <c r="AF33" s="20"/>
-      <c r="AK33" s="28" t="s">
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="33"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="6"/>
+      <c r="AK33" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="AL33" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM33" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN33" s="20" t="s">
+      <c r="AL33" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM33" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN33" s="31" t="s">
         <v>52</v>
       </c>
+      <c r="AO33" s="4"/>
+      <c r="AP33" s="5"/>
+      <c r="AQ33" s="5"/>
+      <c r="AR33" s="6"/>
+      <c r="AS33" s="4"/>
+      <c r="AT33" s="5"/>
+      <c r="AU33" s="5"/>
+      <c r="AV33" s="6"/>
+      <c r="AW33" s="4"/>
+      <c r="AX33" s="5"/>
+      <c r="AY33" s="5"/>
+      <c r="AZ33" s="6"/>
+      <c r="BA33" s="4"/>
+      <c r="BB33" s="5"/>
+      <c r="BC33" s="5"/>
+      <c r="BD33" s="6"/>
     </row>
-    <row r="34" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
         <v>19</v>
       </c>
@@ -3914,7 +3989,7 @@
       <c r="C34" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="I34" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J34" s="8" t="s">
@@ -3923,7 +3998,7 @@
       <c r="K34" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Y34" s="27" t="s">
+      <c r="Y34" s="5" t="s">
         <v>15</v>
       </c>
       <c r="Z34" s="8" t="s">
@@ -3933,21 +4008,41 @@
         <v>147</v>
       </c>
       <c r="AB34" s="20"/>
-      <c r="AK34" s="28" t="s">
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="33"/>
+      <c r="AI34" s="5"/>
+      <c r="AJ34" s="6"/>
+      <c r="AK34" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AL34" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM34" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="AN34" s="20" t="s">
+      <c r="AL34" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM34" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN34" s="31" t="s">
         <v>52</v>
       </c>
+      <c r="AO34" s="4"/>
+      <c r="AP34" s="5"/>
+      <c r="AQ34" s="5"/>
+      <c r="AR34" s="6"/>
+      <c r="AS34" s="4"/>
+      <c r="AT34" s="5"/>
+      <c r="AU34" s="5"/>
+      <c r="AV34" s="6"/>
+      <c r="AW34" s="4"/>
+      <c r="AX34" s="5"/>
+      <c r="AY34" s="5"/>
+      <c r="AZ34" s="6"/>
+      <c r="BA34" s="4"/>
+      <c r="BB34" s="5"/>
+      <c r="BC34" s="5"/>
+      <c r="BD34" s="6"/>
     </row>
-    <row r="35" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y35" s="27" t="s">
+    <row r="35" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Y35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="Z35" s="8" t="s">
@@ -3957,36 +4052,122 @@
         <v>147</v>
       </c>
       <c r="AB35" s="20"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="33"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="6"/>
+      <c r="AK35" s="32"/>
+      <c r="AL35" s="33"/>
+      <c r="AM35" s="33"/>
+      <c r="AN35" s="30"/>
+      <c r="AO35" s="4"/>
+      <c r="AP35" s="5"/>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="6"/>
+      <c r="AS35" s="4"/>
+      <c r="AT35" s="5"/>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="6"/>
+      <c r="AW35" s="4"/>
+      <c r="AX35" s="5"/>
+      <c r="AY35" s="5"/>
+      <c r="AZ35" s="6"/>
+      <c r="BA35" s="4"/>
+      <c r="BB35" s="5"/>
+      <c r="BC35" s="5"/>
+      <c r="BD35" s="6"/>
     </row>
-    <row r="38" spans="1:41" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="Y38" s="8" t="s">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="AG36" s="4"/>
+      <c r="AH36" s="33"/>
+      <c r="AI36" s="5"/>
+      <c r="AJ36" s="6"/>
+      <c r="AK36" s="32"/>
+      <c r="AL36" s="33"/>
+      <c r="AM36" s="33"/>
+      <c r="AN36" s="30"/>
+      <c r="AO36" s="4"/>
+      <c r="AP36" s="5"/>
+      <c r="AQ36" s="5"/>
+      <c r="AR36" s="6"/>
+      <c r="AS36" s="4"/>
+      <c r="AT36" s="5"/>
+      <c r="AU36" s="5"/>
+      <c r="AV36" s="6"/>
+      <c r="AW36" s="4"/>
+      <c r="AX36" s="5"/>
+      <c r="AY36" s="5"/>
+      <c r="AZ36" s="6"/>
+      <c r="BA36" s="4"/>
+      <c r="BB36" s="5"/>
+      <c r="BC36" s="5"/>
+      <c r="BD36" s="6"/>
+    </row>
+    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="AG37" s="4"/>
+      <c r="AH37" s="33"/>
+      <c r="AI37" s="5"/>
+      <c r="AJ37" s="6"/>
+      <c r="AK37" s="32"/>
+      <c r="AL37" s="33"/>
+      <c r="AM37" s="33"/>
+      <c r="AN37" s="30"/>
+      <c r="AO37" s="4"/>
+      <c r="AP37" s="5"/>
+      <c r="AQ37" s="5"/>
+      <c r="AR37" s="6"/>
+      <c r="AS37" s="4"/>
+      <c r="AT37" s="5"/>
+      <c r="AU37" s="5"/>
+      <c r="AV37" s="6"/>
+      <c r="AW37" s="4"/>
+      <c r="AX37" s="5"/>
+      <c r="AY37" s="5"/>
+      <c r="AZ37" s="6"/>
+      <c r="BA37" s="4"/>
+      <c r="BB37" s="5"/>
+      <c r="BC37" s="5"/>
+      <c r="BD37" s="6"/>
+    </row>
+    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="AC38" s="8" t="s">
+      <c r="AC38" s="8"/>
+      <c r="AG38" s="4"/>
+      <c r="AH38" s="33"/>
+      <c r="AI38" s="5"/>
+      <c r="AJ38" s="6"/>
+      <c r="AK38" s="5"/>
+      <c r="AL38" s="33"/>
+      <c r="AM38" s="33"/>
+      <c r="AN38" s="30"/>
+      <c r="AO38" s="5"/>
+      <c r="AP38" s="5"/>
+      <c r="AQ38" s="5"/>
+      <c r="AR38" s="6"/>
+      <c r="AS38" s="4"/>
+      <c r="AT38" s="5"/>
+      <c r="AU38" s="5"/>
+      <c r="AV38" s="6"/>
+      <c r="AW38" s="4"/>
+      <c r="AX38" s="5"/>
+      <c r="AY38" s="5"/>
+      <c r="AZ38" s="6"/>
+      <c r="BA38" s="4"/>
+      <c r="BB38" s="5"/>
+      <c r="BC38" s="5"/>
+      <c r="BD38" s="6"/>
+    </row>
+    <row r="39" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="AK38" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="AO38" s="8" t="s">
-        <v>174</v>
-      </c>
+      <c r="AO39" s="15"/>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="AK39" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="AO39" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" spans="1:41" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="AK40" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="AO40" s="8" t="s">
-        <v>178</v>
-      </c>
+    <row r="40" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="AK40" s="8"/>
+      <c r="AO40" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
[ADD] annotation regprecise yellow level
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1507" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84069A16-61A3-4568-8016-35BC59F724E9}"/>
+  <xr:revisionPtr revIDLastSave="1554" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CEBBB25-6689-4703-9CEE-FC3787BD6AE2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="179">
   <si>
     <t>Organism</t>
   </si>
@@ -549,17 +549,35 @@
     <t>kegg_compounds</t>
   </si>
   <si>
-    <t>Color scheme</t>
-  </si>
-  <si>
-    <t>red - identifier; yellow - implemented; green - ready</t>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>identified</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>working</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,13 +595,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -616,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -679,11 +690,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -745,6 +778,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -754,25 +815,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,17 +1129,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
-  <dimension ref="A1:BD40"/>
+  <dimension ref="A1:BD41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomLeft" activeCell="AO28" sqref="AO28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.21875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="8" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="9" customWidth="1"/>
     <col min="5" max="5" width="13" style="7" customWidth="1"/>
@@ -2544,90 +2586,90 @@
       <c r="AB21" s="20"/>
     </row>
     <row r="22" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="23" t="s">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="23" t="s">
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="23" t="s">
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="23" t="s">
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="25"/>
-      <c r="U22" s="23" t="s">
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="25"/>
-      <c r="Y22" s="23" t="s">
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="25"/>
-      <c r="AC22" s="23" t="s">
+      <c r="Z22" s="36"/>
+      <c r="AA22" s="36"/>
+      <c r="AB22" s="37"/>
+      <c r="AC22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="AD22" s="24"/>
-      <c r="AE22" s="24"/>
-      <c r="AF22" s="25"/>
-      <c r="AG22" s="23" t="s">
+      <c r="AD22" s="36"/>
+      <c r="AE22" s="36"/>
+      <c r="AF22" s="37"/>
+      <c r="AG22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="AH22" s="24"/>
-      <c r="AI22" s="24"/>
-      <c r="AJ22" s="25"/>
-      <c r="AK22" s="23" t="s">
+      <c r="AH22" s="36"/>
+      <c r="AI22" s="36"/>
+      <c r="AJ22" s="37"/>
+      <c r="AK22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="AL22" s="24"/>
-      <c r="AM22" s="24"/>
-      <c r="AN22" s="25"/>
-      <c r="AO22" s="23" t="s">
+      <c r="AL22" s="36"/>
+      <c r="AM22" s="36"/>
+      <c r="AN22" s="37"/>
+      <c r="AO22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="AP22" s="24"/>
-      <c r="AQ22" s="24"/>
-      <c r="AR22" s="25"/>
-      <c r="AS22" s="23" t="s">
+      <c r="AP22" s="36"/>
+      <c r="AQ22" s="36"/>
+      <c r="AR22" s="37"/>
+      <c r="AS22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="AT22" s="24"/>
-      <c r="AU22" s="24"/>
-      <c r="AV22" s="25"/>
-      <c r="AW22" s="23" t="s">
+      <c r="AT22" s="36"/>
+      <c r="AU22" s="36"/>
+      <c r="AV22" s="37"/>
+      <c r="AW22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="AX22" s="24"/>
-      <c r="AY22" s="24"/>
-      <c r="AZ22" s="25"/>
-      <c r="BA22" s="23" t="s">
+      <c r="AX22" s="36"/>
+      <c r="AY22" s="36"/>
+      <c r="AZ22" s="37"/>
+      <c r="BA22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="BB22" s="24"/>
-      <c r="BC22" s="24"/>
-      <c r="BD22" s="25"/>
+      <c r="BB22" s="36"/>
+      <c r="BC22" s="36"/>
+      <c r="BD22" s="37"/>
     </row>
     <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
@@ -2800,7 +2842,7 @@
       </c>
     </row>
     <row r="24" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -2827,7 +2869,7 @@
       <c r="K24" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M24" s="27" t="s">
+      <c r="M24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="N24" s="8" t="s">
@@ -2839,7 +2881,7 @@
       <c r="P24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q24" s="27" t="s">
+      <c r="Q24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="R24" s="8" t="s">
@@ -2851,7 +2893,7 @@
       <c r="T24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="U24" s="27" t="s">
+      <c r="U24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="V24" s="8" t="s">
@@ -2863,7 +2905,7 @@
       <c r="X24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Y24" s="27" t="s">
+      <c r="Y24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="Z24" s="8" t="s">
@@ -2875,7 +2917,7 @@
       <c r="AB24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="AC24" s="27" t="s">
+      <c r="AC24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="AD24" s="8" t="s">
@@ -2887,7 +2929,7 @@
       <c r="AF24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="AG24" s="26" t="s">
+      <c r="AG24" s="23" t="s">
         <v>21</v>
       </c>
       <c r="AH24" s="5" t="s">
@@ -2899,7 +2941,7 @@
       <c r="AJ24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AK24" s="27" t="s">
+      <c r="AK24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="AL24" s="5" t="s">
@@ -2911,7 +2953,7 @@
       <c r="AN24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AO24" s="27" t="s">
+      <c r="AO24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="AP24" s="5" t="s">
@@ -2923,7 +2965,7 @@
       <c r="AR24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AS24" s="27" t="s">
+      <c r="AS24" s="24" t="s">
         <v>21</v>
       </c>
       <c r="AT24" s="5" t="s">
@@ -2961,7 +3003,7 @@
       </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="24" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -3007,7 +3049,7 @@
         <v>147</v>
       </c>
       <c r="T25" s="9"/>
-      <c r="U25" s="28" t="s">
+      <c r="U25" s="24" t="s">
         <v>22</v>
       </c>
       <c r="V25" s="8" t="s">
@@ -3096,7 +3138,7 @@
       <c r="BD25" s="6"/>
     </row>
     <row r="26" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -3114,7 +3156,7 @@
       <c r="G26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="I26" s="24" t="s">
         <v>42</v>
       </c>
       <c r="J26" s="8" t="s">
@@ -3123,7 +3165,7 @@
       <c r="K26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M26" s="28" t="s">
+      <c r="M26" s="24" t="s">
         <v>12</v>
       </c>
       <c r="N26" s="8" t="s">
@@ -3132,7 +3174,7 @@
       <c r="O26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Q26" s="28" t="s">
+      <c r="Q26" s="24" t="s">
         <v>12</v>
       </c>
       <c r="R26" s="8" t="s">
@@ -3141,7 +3183,7 @@
       <c r="S26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="U26" s="28" t="s">
+      <c r="U26" s="24" t="s">
         <v>12</v>
       </c>
       <c r="V26" s="8" t="s">
@@ -3198,7 +3240,7 @@
         <v>147</v>
       </c>
       <c r="AR26" s="6"/>
-      <c r="AS26" s="28" t="s">
+      <c r="AS26" s="24" t="s">
         <v>0</v>
       </c>
       <c r="AT26" s="5" t="s">
@@ -3230,7 +3272,7 @@
       <c r="BD26" s="6"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="24" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3257,7 +3299,7 @@
       <c r="K27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M27" s="28" t="s">
+      <c r="M27" s="24" t="s">
         <v>10</v>
       </c>
       <c r="N27" s="8" t="s">
@@ -3266,7 +3308,7 @@
       <c r="O27" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Q27" s="28" t="s">
+      <c r="Q27" s="24" t="s">
         <v>17</v>
       </c>
       <c r="R27" s="8" t="s">
@@ -3323,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="AR27" s="6"/>
-      <c r="AS27" s="28" t="s">
+      <c r="AS27" s="24" t="s">
         <v>12</v>
       </c>
       <c r="AT27" s="5" t="s">
@@ -3355,7 +3397,7 @@
       <c r="BD27" s="6"/>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="24" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -3400,7 +3442,7 @@
       <c r="AA28" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="AC28" s="28" t="s">
+      <c r="AC28" s="24" t="s">
         <v>12</v>
       </c>
       <c r="AD28" s="19" t="s">
@@ -3428,8 +3470,8 @@
       <c r="AM28" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AN28" s="30"/>
-      <c r="AO28" s="28" t="s">
+      <c r="AN28" s="25"/>
+      <c r="AO28" s="24" t="s">
         <v>12</v>
       </c>
       <c r="AP28" s="5" t="s">
@@ -3441,7 +3483,7 @@
       <c r="AR28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AS28" s="32" t="s">
+      <c r="AS28" s="27" t="s">
         <v>19</v>
       </c>
       <c r="AT28" s="13" t="s">
@@ -3450,7 +3492,7 @@
       <c r="AU28" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AV28" s="31"/>
+      <c r="AV28" s="26"/>
       <c r="AW28" s="4" t="s">
         <v>12</v>
       </c>
@@ -3460,7 +3502,7 @@
       <c r="AY28" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AZ28" s="31"/>
+      <c r="AZ28" s="26"/>
       <c r="BA28" s="4" t="s">
         <v>12</v>
       </c>
@@ -3470,10 +3512,10 @@
       <c r="BC28" s="5">
         <v>1</v>
       </c>
-      <c r="BD28" s="31"/>
+      <c r="BD28" s="26"/>
     </row>
     <row r="29" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="8" t="s">
@@ -3500,7 +3542,7 @@
       <c r="K29" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M29" s="28" t="s">
+      <c r="M29" s="24" t="s">
         <v>17</v>
       </c>
       <c r="N29" s="8" t="s">
@@ -3548,10 +3590,10 @@
       <c r="AM29" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AN29" s="30" t="s">
+      <c r="AN29" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="AO29" s="28" t="s">
+      <c r="AO29" s="24" t="s">
         <v>10</v>
       </c>
       <c r="AP29" s="5" t="s">
@@ -3574,7 +3616,7 @@
       <c r="AY29" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AZ29" s="31"/>
+      <c r="AZ29" s="26"/>
       <c r="BA29" s="4" t="s">
         <v>10</v>
       </c>
@@ -3584,10 +3626,10 @@
       <c r="BC29" s="5">
         <v>1</v>
       </c>
-      <c r="BD29" s="31"/>
+      <c r="BD29" s="26"/>
     </row>
     <row r="30" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -3614,7 +3656,7 @@
       <c r="K30" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M30" s="28" t="s">
+      <c r="M30" s="24" t="s">
         <v>16</v>
       </c>
       <c r="N30" s="8" t="s">
@@ -3642,10 +3684,10 @@
         <v>149</v>
       </c>
       <c r="AG30" s="4"/>
-      <c r="AH30" s="33"/>
+      <c r="AH30" s="28"/>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="6"/>
-      <c r="AK30" s="28" t="s">
+      <c r="AK30" s="24" t="s">
         <v>10</v>
       </c>
       <c r="AL30" s="13" t="s">
@@ -3655,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="AN30" s="6"/>
-      <c r="AO30" s="28" t="s">
+      <c r="AO30" s="24" t="s">
         <v>17</v>
       </c>
       <c r="AP30" s="5" t="s">
@@ -3680,7 +3722,7 @@
       <c r="AY30" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AZ30" s="31" t="s">
+      <c r="AZ30" s="26" t="s">
         <v>52</v>
       </c>
       <c r="BA30" s="4" t="s">
@@ -3692,12 +3734,12 @@
       <c r="BC30" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="BD30" s="31" t="s">
+      <c r="BD30" s="26" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3715,7 +3757,7 @@
       <c r="K31" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="M31" s="28" t="s">
+      <c r="M31" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N31" s="8" t="s">
@@ -3746,7 +3788,7 @@
         <v>147</v>
       </c>
       <c r="AG31" s="4"/>
-      <c r="AH31" s="33"/>
+      <c r="AH31" s="28"/>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="6"/>
       <c r="AK31" s="5" t="s">
@@ -3761,7 +3803,7 @@
       <c r="AN31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AO31" s="32" t="s">
+      <c r="AO31" s="27" t="s">
         <v>15</v>
       </c>
       <c r="AP31" s="13" t="s">
@@ -3770,7 +3812,7 @@
       <c r="AQ31" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AR31" s="31" t="s">
+      <c r="AR31" s="26" t="s">
         <v>52</v>
       </c>
       <c r="AS31" s="4"/>
@@ -3786,7 +3828,7 @@
       <c r="AY31" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="AZ31" s="31" t="s">
+      <c r="AZ31" s="26" t="s">
         <v>52</v>
       </c>
       <c r="BA31" s="4" t="s">
@@ -3798,12 +3840,12 @@
       <c r="BC31" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="BD31" s="31" t="s">
+      <c r="BD31" s="26" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -3853,7 +3895,7 @@
       </c>
       <c r="AF32" s="20"/>
       <c r="AG32" s="4"/>
-      <c r="AH32" s="33"/>
+      <c r="AH32" s="28"/>
       <c r="AI32" s="5"/>
       <c r="AJ32" s="6"/>
       <c r="AK32" s="34" t="s">
@@ -3865,10 +3907,10 @@
       <c r="AM32" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AN32" s="30" t="s">
+      <c r="AN32" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="AO32" s="32" t="s">
+      <c r="AO32" s="27" t="s">
         <v>19</v>
       </c>
       <c r="AP32" s="13" t="s">
@@ -3877,7 +3919,7 @@
       <c r="AQ32" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AR32" s="31" t="s">
+      <c r="AR32" s="26" t="s">
         <v>52</v>
       </c>
       <c r="AS32" s="4"/>
@@ -3897,10 +3939,10 @@
       <c r="BC32" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="BD32" s="31"/>
+      <c r="BD32" s="26"/>
     </row>
     <row r="33" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -3947,10 +3989,10 @@
       </c>
       <c r="AF33" s="20"/>
       <c r="AG33" s="4"/>
-      <c r="AH33" s="33"/>
+      <c r="AH33" s="28"/>
       <c r="AI33" s="5"/>
       <c r="AJ33" s="6"/>
-      <c r="AK33" s="32" t="s">
+      <c r="AK33" s="27" t="s">
         <v>15</v>
       </c>
       <c r="AL33" s="13" t="s">
@@ -3959,7 +4001,7 @@
       <c r="AM33" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AN33" s="31" t="s">
+      <c r="AN33" s="26" t="s">
         <v>52</v>
       </c>
       <c r="AO33" s="4"/>
@@ -3980,7 +4022,7 @@
       <c r="BD33" s="6"/>
     </row>
     <row r="34" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -4009,10 +4051,10 @@
       </c>
       <c r="AB34" s="20"/>
       <c r="AG34" s="4"/>
-      <c r="AH34" s="33"/>
+      <c r="AH34" s="28"/>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="6"/>
-      <c r="AK34" s="32" t="s">
+      <c r="AK34" s="27" t="s">
         <v>19</v>
       </c>
       <c r="AL34" s="13" t="s">
@@ -4021,7 +4063,7 @@
       <c r="AM34" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AN34" s="31" t="s">
+      <c r="AN34" s="26" t="s">
         <v>52</v>
       </c>
       <c r="AO34" s="4"/>
@@ -4053,13 +4095,13 @@
       </c>
       <c r="AB35" s="20"/>
       <c r="AG35" s="4"/>
-      <c r="AH35" s="33"/>
+      <c r="AH35" s="28"/>
       <c r="AI35" s="5"/>
       <c r="AJ35" s="6"/>
-      <c r="AK35" s="32"/>
-      <c r="AL35" s="33"/>
-      <c r="AM35" s="33"/>
-      <c r="AN35" s="30"/>
+      <c r="AK35" s="27"/>
+      <c r="AL35" s="28"/>
+      <c r="AM35" s="28"/>
+      <c r="AN35" s="25"/>
       <c r="AO35" s="4"/>
       <c r="AP35" s="5"/>
       <c r="AQ35" s="5"/>
@@ -4079,13 +4121,13 @@
     </row>
     <row r="36" spans="1:56" x14ac:dyDescent="0.3">
       <c r="AG36" s="4"/>
-      <c r="AH36" s="33"/>
+      <c r="AH36" s="28"/>
       <c r="AI36" s="5"/>
       <c r="AJ36" s="6"/>
-      <c r="AK36" s="32"/>
-      <c r="AL36" s="33"/>
-      <c r="AM36" s="33"/>
-      <c r="AN36" s="30"/>
+      <c r="AK36" s="27"/>
+      <c r="AL36" s="28"/>
+      <c r="AM36" s="28"/>
+      <c r="AN36" s="25"/>
       <c r="AO36" s="4"/>
       <c r="AP36" s="5"/>
       <c r="AQ36" s="5"/>
@@ -4103,15 +4145,15 @@
       <c r="BC36" s="5"/>
       <c r="BD36" s="6"/>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AG37" s="4"/>
-      <c r="AH37" s="33"/>
+      <c r="AH37" s="28"/>
       <c r="AI37" s="5"/>
       <c r="AJ37" s="6"/>
-      <c r="AK37" s="32"/>
-      <c r="AL37" s="33"/>
-      <c r="AM37" s="33"/>
-      <c r="AN37" s="30"/>
+      <c r="AK37" s="27"/>
+      <c r="AL37" s="28"/>
+      <c r="AM37" s="28"/>
+      <c r="AN37" s="25"/>
       <c r="AO37" s="4"/>
       <c r="AP37" s="5"/>
       <c r="AQ37" s="5"/>
@@ -4129,19 +4171,22 @@
       <c r="BC37" s="5"/>
       <c r="BD37" s="6"/>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="32" t="s">
         <v>171</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>172</v>
       </c>
       <c r="AC38" s="8"/>
       <c r="AG38" s="4"/>
-      <c r="AH38" s="33"/>
+      <c r="AH38" s="28"/>
       <c r="AI38" s="5"/>
       <c r="AJ38" s="6"/>
       <c r="AK38" s="5"/>
-      <c r="AL38" s="33"/>
-      <c r="AM38" s="33"/>
-      <c r="AN38" s="30"/>
+      <c r="AL38" s="28"/>
+      <c r="AM38" s="28"/>
+      <c r="AN38" s="25"/>
       <c r="AO38" s="5"/>
       <c r="AP38" s="5"/>
       <c r="AQ38" s="5"/>
@@ -4159,15 +4204,32 @@
       <c r="BC38" s="5"/>
       <c r="BD38" s="6"/>
     </row>
-    <row r="39" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>172</v>
+    <row r="39" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="AO39" s="15"/>
     </row>
     <row r="40" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="B40" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="AK40" s="8"/>
       <c r="AO40" s="8"/>
+    </row>
+    <row r="41" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
[FIX] debugging regprecise transformers [ADD] bioapi cache using diskcache package and cache memoize
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1554" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CEBBB25-6689-4703-9CEE-FC3787BD6AE2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -1131,9 +1131,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO28" sqref="AO28"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[FIX] strand possible values
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1554" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CEBBB25-6689-4703-9CEE-FC3787BD6AE2}"/>
+  <xr:revisionPtr revIDLastSave="1561" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0650C2EE-A550-4BC2-8318-534D152DD94A}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="179">
   <si>
     <t>Organism</t>
   </si>
@@ -42,12 +42,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>phylum</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
     <t>Organism Comments</t>
   </si>
   <si>
@@ -571,6 +565,12 @@
   </si>
   <si>
     <t>working</t>
+  </si>
+  <si>
+    <t>loaded</t>
+  </si>
+  <si>
+    <t>blue</t>
   </si>
 </sst>
 </file>
@@ -1129,11 +1129,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
-  <dimension ref="A1:BD41"/>
+  <dimension ref="A1:BD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO7" sqref="AO7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,7 +1150,7 @@
     <col min="10" max="10" width="10.88671875" style="8" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" style="8" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" style="7" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" style="7" customWidth="1"/>
     <col min="14" max="14" width="9.77734375" style="8" customWidth="1"/>
     <col min="15" max="15" width="12" style="8" customWidth="1"/>
     <col min="16" max="16" width="12.44140625" style="9" customWidth="1"/>
@@ -1199,655 +1199,655 @@
   <sheetData>
     <row r="1" spans="1:56" s="2" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>127</v>
-      </c>
       <c r="L1" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="10" t="s">
+      <c r="S1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="R1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="T1" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="U1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="V1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="X1" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Z1" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>86</v>
-      </c>
       <c r="AB1" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AC1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="AD1" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE1" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="AF1" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AH1" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AJ1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AL1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AR1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AW1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX1" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL1" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="AM1" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP1" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AQ1" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="AR1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS1" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AT1" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="AU1" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="AV1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX1" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="AY1" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="AZ1" s="12" t="s">
-        <v>37</v>
-      </c>
       <c r="BA1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BB1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="BC1" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="BB1" s="11" t="s">
+      <c r="BD1" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="BC1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="BD1" s="12" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
       <c r="E2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
       <c r="I2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="6"/>
       <c r="M2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W2" s="5"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
       <c r="AC2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM2" s="5"/>
       <c r="AN2" s="6"/>
       <c r="AO2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AP2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AQ2" s="5"/>
       <c r="AR2" s="6"/>
       <c r="AS2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AT2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AU2" s="5"/>
       <c r="AV2" s="6"/>
       <c r="AW2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AX2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AY2" s="5"/>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="BC2" s="5"/>
       <c r="BD2" s="6"/>
     </row>
     <row r="3" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
       <c r="I3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="6"/>
       <c r="M3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="W3" s="5"/>
       <c r="X3" s="6"/>
       <c r="Y3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="AA3" s="5"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="AE3" s="5"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
       <c r="AK3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="6"/>
       <c r="AO3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="AP3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="6"/>
       <c r="AS3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="AT3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="AU3" s="5"/>
       <c r="AV3" s="6"/>
       <c r="AW3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="AX3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="BB3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="BC3" s="5"/>
       <c r="BD3" s="6"/>
     </row>
     <row r="4" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
       <c r="I4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="6"/>
       <c r="M4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="6"/>
       <c r="U4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="W4" s="5"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AE4" s="5"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="6"/>
       <c r="AK4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AL4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AM4" s="5"/>
       <c r="AN4" s="6"/>
       <c r="AO4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AP4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="6"/>
       <c r="AS4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AU4" s="5"/>
       <c r="AV4" s="6"/>
       <c r="AW4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AX4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AY4" s="5"/>
       <c r="AZ4" s="6"/>
       <c r="BA4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="BB4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BC4" s="5"/>
       <c r="BD4" s="6"/>
     </row>
     <row r="5" spans="1:56" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T5" s="5"/>
       <c r="U5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="X5" s="6"/>
       <c r="Y5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB5" s="6"/>
       <c r="AC5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AF5" s="6"/>
       <c r="AG5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AH5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AI5" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AN5" s="6"/>
       <c r="AO5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AP5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AQ5" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AR5" s="6"/>
       <c r="AS5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AU5" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AV5" s="6"/>
       <c r="AW5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AX5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AY5" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AZ5" s="6"/>
       <c r="BA5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="BB5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="BC5" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BD5" s="6"/>
     </row>
@@ -1856,505 +1856,502 @@
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB6" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AC6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="AD6" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AF6" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AG6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="AH6" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AK6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM6" s="8"/>
       <c r="AN6" s="9"/>
       <c r="AO6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AP6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AS6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="AT6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AW6" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AX6" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA6" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="BB6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="V7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Z7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AD7" s="13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AG7" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AI7" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AK7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="AL7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM7" s="8"/>
       <c r="AN7" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ7" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AO7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ7" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="AS7" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AT7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AU7" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AW7" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AX7" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA7" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="BB7" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB8" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC8" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AD8" s="13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AG8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AH8" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AK8" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AL8" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AM8" s="8"/>
       <c r="AN8" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AO8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AP8" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AS8" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AT8" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AV8" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AW8" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AX8" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA8" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="BB8" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="U9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="V9" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC9" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Z9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB9" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC9" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AD9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG9" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="AH9" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AK9" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AL9" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM9" s="8"/>
       <c r="AN9" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AO9" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AP9" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AW9" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AX9" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA9" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="BB9" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="I10" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>163</v>
+        <v>70</v>
       </c>
       <c r="Y10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Z10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB10" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC10" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="AD10" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE10" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AH10" s="8"/>
       <c r="AK10" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AL10" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM10" s="8"/>
       <c r="AN10" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AW10" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AX10" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AY10" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BA10" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="BB10" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>70</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
       <c r="Y11" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Z11" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB11" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AD11" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AK11" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AL11" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM11" s="8"/>
       <c r="AN11" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="BA11" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="BB11" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="BC11" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:56" ht="72" x14ac:dyDescent="0.3">
@@ -2362,42 +2359,39 @@
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
-      <c r="M12" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>72</v>
-      </c>
+      <c r="M12" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="20"/>
       <c r="Y12" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AB12" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AC12" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AD12" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AK12" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AL12" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM12" s="8"/>
       <c r="AN12" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
@@ -2405,57 +2399,51 @@
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
-      <c r="M13" s="18" t="s">
+      <c r="M13" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="20"/>
       <c r="Y13" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB13" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AK13" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AL13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM13" s="8"/>
       <c r="AN13" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="M14" s="18" t="s">
+      <c r="M14" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="20"/>
       <c r="Y14" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB14" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AK14" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AL14" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM14" s="8"/>
       <c r="AN14" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2463,110 +2451,104 @@
         <v>166</v>
       </c>
       <c r="Y15" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Z15" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB15" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AK15" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AL15" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM15" s="8"/>
       <c r="AN15" s="9"/>
     </row>
     <row r="16" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M16" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="Y16" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Z16" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AK16" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AL16" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM16" s="19"/>
       <c r="AN16" s="9"/>
     </row>
     <row r="17" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="M17" s="7" t="s">
-        <v>168</v>
-      </c>
       <c r="Y17" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Z17" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB17" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AK17" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AL17" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM17" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AN17" s="9"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="Y18" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z18" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="20"/>
       <c r="AK18" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AL18" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AM18" s="19"/>
       <c r="AN18" s="9"/>
     </row>
-    <row r="19" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="Y19" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Z19" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA19" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB19" s="20"/>
       <c r="AK19" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AL19" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AM19" s="19"/>
       <c r="AN19" s="9"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="Y20" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z20" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AA20" s="19"/>
       <c r="AB20" s="20"/>
@@ -2577,95 +2559,95 @@
     </row>
     <row r="21" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Y21" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z21" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AA21" s="19"/>
       <c r="AB21" s="20"/>
     </row>
     <row r="22" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="37"/>
       <c r="I22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J22" s="36"/>
       <c r="K22" s="36"/>
       <c r="L22" s="37"/>
       <c r="M22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
       <c r="P22" s="37"/>
       <c r="Q22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="R22" s="36"/>
       <c r="S22" s="36"/>
       <c r="T22" s="37"/>
       <c r="U22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V22" s="36"/>
       <c r="W22" s="36"/>
       <c r="X22" s="37"/>
       <c r="Y22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Z22" s="36"/>
       <c r="AA22" s="36"/>
       <c r="AB22" s="37"/>
       <c r="AC22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AD22" s="36"/>
       <c r="AE22" s="36"/>
       <c r="AF22" s="37"/>
       <c r="AG22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AH22" s="36"/>
       <c r="AI22" s="36"/>
       <c r="AJ22" s="37"/>
       <c r="AK22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AL22" s="36"/>
       <c r="AM22" s="36"/>
       <c r="AN22" s="37"/>
       <c r="AO22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AP22" s="36"/>
       <c r="AQ22" s="36"/>
       <c r="AR22" s="37"/>
       <c r="AS22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AT22" s="36"/>
       <c r="AU22" s="36"/>
       <c r="AV22" s="37"/>
       <c r="AW22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AX22" s="36"/>
       <c r="AY22" s="36"/>
       <c r="AZ22" s="37"/>
       <c r="BA22" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BB22" s="36"/>
       <c r="BC22" s="36"/>
@@ -2673,172 +2655,172 @@
     </row>
     <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="D23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="H23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="K23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="J23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="L23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="O23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="N23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="O23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="P23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="S23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="R23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="S23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="T23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="U23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="V23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="W23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="V23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="W23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="X23" s="22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Y23" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="Z23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="AB23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="AD23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AE23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="AF23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AG23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="AH23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="AJ23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AK23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AL23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AM23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="AL23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="AN23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AO23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AQ23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="AP23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AQ23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="AR23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AS23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AT23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="AT23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AU23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="AV23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AW23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AY23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="AX23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AY23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="AZ23" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="BA23" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="BB23" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BB23" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="BC23" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="BD23" s="22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
@@ -2846,482 +2828,482 @@
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="S24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="T24" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="V24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="W24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X24" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Y24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Z24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB24" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AC24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AD24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AF24" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AG24" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AH24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AI24" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AJ24" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AK24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AL24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM24" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN24" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AO24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AP24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ24" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AR24" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AS24" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AT24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AU24" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AV24" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AW24" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AX24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY24" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ24" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="BA24" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="BB24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC24" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BD24" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="N25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="O25" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q25" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="R25" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="T25" s="9"/>
       <c r="U25" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V25" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="W25" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Z25" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA25" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AD25" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE25" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AG25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AH25" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AI25" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AL25" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM25" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN25" s="6"/>
       <c r="AO25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AP25" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ25" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AR25" s="6"/>
       <c r="AS25" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AT25" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AU25" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AV25" s="6"/>
       <c r="AW25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AX25" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY25" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ25" s="6"/>
       <c r="BA25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="BB25" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC25" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BD25" s="6"/>
     </row>
     <row r="26" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q26" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="U26" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="W26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AD26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE26" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AG26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AH26" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AI26" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AJ26" s="6"/>
       <c r="AK26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AL26" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM26" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN26" s="6"/>
       <c r="AO26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AP26" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ26" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AR26" s="6"/>
       <c r="AS26" s="24" t="s">
         <v>0</v>
       </c>
       <c r="AT26" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AU26" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AV26" s="6"/>
       <c r="AW26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AX26" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY26" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ26" s="6"/>
       <c r="BA26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="BB26" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC26" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BD26" s="6"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M27" s="24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q27" s="24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="S27" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y27" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Z27" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA27" s="8">
         <v>1</v>
@@ -3330,7 +3312,7 @@
         <v>0</v>
       </c>
       <c r="AD27" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE27" s="8">
         <v>1</v>
@@ -3339,7 +3321,7 @@
         <v>0</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AI27" s="5">
         <v>1</v>
@@ -3349,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="AL27" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM27" s="5">
         <v>1</v>
@@ -3359,27 +3341,27 @@
         <v>0</v>
       </c>
       <c r="AP27" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ27" s="5">
         <v>1</v>
       </c>
       <c r="AR27" s="6"/>
       <c r="AS27" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AT27" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AU27" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AV27" s="6"/>
       <c r="AW27" s="5" t="s">
         <v>0</v>
       </c>
       <c r="AX27" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY27" s="5">
         <v>1</v>
@@ -3389,7 +3371,7 @@
         <v>0</v>
       </c>
       <c r="BB27" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC27" s="5">
         <v>1</v>
@@ -3398,116 +3380,116 @@
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y28" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA28" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC28" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y28" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC28" s="24" t="s">
-        <v>12</v>
-      </c>
       <c r="AD28" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE28" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AG28" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AH28" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AI28" s="5">
         <v>1</v>
       </c>
       <c r="AJ28" s="6"/>
       <c r="AK28" s="34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AL28" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM28" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN28" s="25"/>
       <c r="AO28" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AP28" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ28" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AR28" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AS28" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AT28" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AU28" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AV28" s="26"/>
       <c r="AW28" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AX28" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY28" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AZ28" s="26"/>
       <c r="BA28" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BB28" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC28" s="5">
         <v>1</v>
@@ -3516,88 +3498,88 @@
     </row>
     <row r="29" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M29" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M29" s="24" t="s">
-        <v>17</v>
-      </c>
       <c r="N29" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y29" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Z29" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA29" s="8">
         <v>1</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AD29" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE29" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH29" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI29" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="AG29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH29" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI29" s="5" t="s">
-        <v>149</v>
-      </c>
       <c r="AJ29" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AK29" s="34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AL29" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM29" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN29" s="25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AO29" s="24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AP29" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ29" s="5">
         <v>1</v>
@@ -3608,20 +3590,20 @@
       <c r="AU29" s="5"/>
       <c r="AV29" s="6"/>
       <c r="AW29" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AX29" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY29" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AZ29" s="26"/>
       <c r="BA29" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="BB29" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC29" s="5">
         <v>1</v>
@@ -3630,268 +3612,268 @@
     </row>
     <row r="30" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="F30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M30" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y30" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA30" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC30" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE30" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M30" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y30" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA30" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC30" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AE30" s="8" t="s">
-        <v>149</v>
       </c>
       <c r="AG30" s="4"/>
       <c r="AH30" s="28"/>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AL30" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM30" s="5">
         <v>1</v>
       </c>
       <c r="AN30" s="6"/>
       <c r="AO30" s="24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AP30" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ30" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AR30" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AS30" s="4"/>
       <c r="AT30" s="5"/>
       <c r="AU30" s="5"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AX30" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY30" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AZ30" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="BA30" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="BB30" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC30" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="BD30" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M31" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M31" s="24" t="s">
-        <v>18</v>
-      </c>
       <c r="N31" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y31" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Z31" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB31" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AC31" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AD31" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE31" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AG31" s="4"/>
       <c r="AH31" s="28"/>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="6"/>
       <c r="AK31" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AL31" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM31" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN31" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AO31" s="27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AP31" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ31" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AR31" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AS31" s="4"/>
       <c r="AT31" s="5"/>
       <c r="AU31" s="5"/>
       <c r="AV31" s="6"/>
       <c r="AW31" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AX31" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AY31" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ31" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="BA31" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="BB31" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC31" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BD31" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y32" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Z32" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA32" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB32" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AC32" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AD32" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE32" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AF32" s="20"/>
       <c r="AG32" s="4"/>
@@ -3899,28 +3881,28 @@
       <c r="AI32" s="5"/>
       <c r="AJ32" s="6"/>
       <c r="AK32" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AL32" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM32" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN32" s="25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AO32" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AP32" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AQ32" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AR32" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AS32" s="4"/>
       <c r="AT32" s="5"/>
@@ -3931,61 +3913,61 @@
       <c r="AY32" s="5"/>
       <c r="AZ32" s="6"/>
       <c r="BA32" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="BB32" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="BC32" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BD32" s="26"/>
     </row>
     <row r="33" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y33" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Z33" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA33" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC33" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AD33" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AE33" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AF33" s="20"/>
       <c r="AG33" s="4"/>
@@ -3993,16 +3975,16 @@
       <c r="AI33" s="5"/>
       <c r="AJ33" s="6"/>
       <c r="AK33" s="27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AL33" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM33" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN33" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AO33" s="4"/>
       <c r="AP33" s="5"/>
@@ -4023,31 +4005,31 @@
     </row>
     <row r="34" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y34" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z34" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB34" s="20"/>
       <c r="AG34" s="4"/>
@@ -4055,16 +4037,16 @@
       <c r="AI34" s="5"/>
       <c r="AJ34" s="6"/>
       <c r="AK34" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AL34" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AM34" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AN34" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AO34" s="4"/>
       <c r="AP34" s="5"/>
@@ -4085,13 +4067,13 @@
     </row>
     <row r="35" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="Y35" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z35" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA35" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB35" s="20"/>
       <c r="AG35" s="4"/>
@@ -4173,10 +4155,10 @@
     </row>
     <row r="38" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AC38" s="8"/>
       <c r="AG38" s="4"/>
@@ -4206,29 +4188,37 @@
     </row>
     <row r="39" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AO39" s="15"/>
     </row>
     <row r="40" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AK40" s="8"/>
       <c r="AO40" s="8"/>
     </row>
-    <row r="41" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="30" t="s">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="C41" s="31" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ADD] regulatory interaction connections; [FIX] other connections
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1590" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03714790-5F39-492A-9FF1-472BE1686FAB}"/>
+  <xr:revisionPtr revIDLastSave="1597" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A453DA6-4A3C-4625-9924-30CA87573A51}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -574,7 +574,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,13 +605,6 @@
     <font>
       <sz val="11"/>
       <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -734,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -824,6 +817,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -832,36 +852,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,7 +1171,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BA31" activeCellId="6" sqref="BA24 BA27 BA28 BA29 BA30 BA32 BA31"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1330,7 +1320,7 @@
       <c r="AB1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="46" t="s">
+      <c r="AC1" s="43" t="s">
         <v>89</v>
       </c>
       <c r="AD1" s="11" t="s">
@@ -1416,14 +1406,14 @@
       </c>
     </row>
     <row r="2" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
+      <c r="B2" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="4" t="s">
         <v>50</v>
       </c>
@@ -1432,39 +1422,39 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="38" t="s">
+      <c r="J2" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="38" t="s">
+      <c r="N2" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="41"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="38" t="s">
+      <c r="R2" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="44"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="39" t="s">
+      <c r="V2" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="41"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="36" t="s">
         <v>50</v>
       </c>
       <c r="Z2" s="5" t="s">
@@ -1472,7 +1462,7 @@
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="38" t="s">
+      <c r="AC2" s="35" t="s">
         <v>50</v>
       </c>
       <c r="AD2" s="5" t="s">
@@ -1488,7 +1478,7 @@
       </c>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="6"/>
-      <c r="AK2" s="38" t="s">
+      <c r="AK2" s="35" t="s">
         <v>50</v>
       </c>
       <c r="AL2" s="5" t="s">
@@ -1496,7 +1486,7 @@
       </c>
       <c r="AM2" s="5"/>
       <c r="AN2" s="6"/>
-      <c r="AO2" s="38" t="s">
+      <c r="AO2" s="35" t="s">
         <v>50</v>
       </c>
       <c r="AP2" s="5" t="s">
@@ -1504,7 +1494,7 @@
       </c>
       <c r="AQ2" s="5"/>
       <c r="AR2" s="6"/>
-      <c r="AS2" s="38" t="s">
+      <c r="AS2" s="35" t="s">
         <v>50</v>
       </c>
       <c r="AT2" s="5" t="s">
@@ -1520,7 +1510,7 @@
       </c>
       <c r="AY2" s="5"/>
       <c r="AZ2" s="6"/>
-      <c r="BA2" s="38" t="s">
+      <c r="BA2" s="35" t="s">
         <v>50</v>
       </c>
       <c r="BB2" s="5" t="s">
@@ -1530,14 +1520,14 @@
       <c r="BD2" s="6"/>
     </row>
     <row r="3" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="4" t="s">
         <v>51</v>
       </c>
@@ -1546,39 +1536,39 @@
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="44"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="38" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="44"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="38" t="s">
+      <c r="O3" s="41"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="44" t="s">
+      <c r="R3" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="38" t="s">
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="44" t="s">
+      <c r="V3" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="W3" s="44"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="39" t="s">
+      <c r="W3" s="41"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="36" t="s">
         <v>51</v>
       </c>
       <c r="Z3" s="5" t="s">
@@ -1586,7 +1576,7 @@
       </c>
       <c r="AA3" s="5"/>
       <c r="AB3" s="6"/>
-      <c r="AC3" s="38" t="s">
+      <c r="AC3" s="35" t="s">
         <v>51</v>
       </c>
       <c r="AD3" s="5" t="s">
@@ -1602,7 +1592,7 @@
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
-      <c r="AK3" s="38" t="s">
+      <c r="AK3" s="35" t="s">
         <v>51</v>
       </c>
       <c r="AL3" s="5" t="s">
@@ -1610,7 +1600,7 @@
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="6"/>
-      <c r="AO3" s="38" t="s">
+      <c r="AO3" s="35" t="s">
         <v>51</v>
       </c>
       <c r="AP3" s="5" t="s">
@@ -1618,7 +1608,7 @@
       </c>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="6"/>
-      <c r="AS3" s="38" t="s">
+      <c r="AS3" s="35" t="s">
         <v>51</v>
       </c>
       <c r="AT3" s="5" t="s">
@@ -1634,7 +1624,7 @@
       </c>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="6"/>
-      <c r="BA3" s="38" t="s">
+      <c r="BA3" s="35" t="s">
         <v>51</v>
       </c>
       <c r="BB3" s="5" t="s">
@@ -1644,14 +1634,14 @@
       <c r="BD3" s="6"/>
     </row>
     <row r="4" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="4" t="s">
         <v>148</v>
       </c>
@@ -1660,39 +1650,39 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="38" t="s">
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="N4" s="44" t="s">
+      <c r="N4" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="44"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="38" t="s">
+      <c r="O4" s="41"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="R4" s="44" t="s">
+      <c r="R4" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="44"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="38" t="s">
+      <c r="S4" s="41"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="V4" s="44" t="s">
+      <c r="V4" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="W4" s="44"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="38" t="s">
+      <c r="W4" s="41"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="35" t="s">
         <v>148</v>
       </c>
       <c r="Z4" s="5" t="s">
@@ -1700,7 +1690,7 @@
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="38" t="s">
+      <c r="AC4" s="35" t="s">
         <v>148</v>
       </c>
       <c r="AD4" s="5" t="s">
@@ -1716,7 +1706,7 @@
       </c>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="6"/>
-      <c r="AK4" s="38" t="s">
+      <c r="AK4" s="35" t="s">
         <v>148</v>
       </c>
       <c r="AL4" s="5" t="s">
@@ -1724,7 +1714,7 @@
       </c>
       <c r="AM4" s="5"/>
       <c r="AN4" s="6"/>
-      <c r="AO4" s="38" t="s">
+      <c r="AO4" s="35" t="s">
         <v>148</v>
       </c>
       <c r="AP4" s="5" t="s">
@@ -1732,7 +1722,7 @@
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="6"/>
-      <c r="AS4" s="38" t="s">
+      <c r="AS4" s="35" t="s">
         <v>148</v>
       </c>
       <c r="AT4" s="5" t="s">
@@ -1748,7 +1738,7 @@
       </c>
       <c r="AY4" s="5"/>
       <c r="AZ4" s="6"/>
-      <c r="BA4" s="38" t="s">
+      <c r="BA4" s="35" t="s">
         <v>148</v>
       </c>
       <c r="BB4" s="5" t="s">
@@ -1758,16 +1748,16 @@
       <c r="BD4" s="6"/>
     </row>
     <row r="5" spans="1:56" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="44" t="s">
+      <c r="B5" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="4" t="s">
         <v>54</v>
       </c>
@@ -1778,47 +1768,47 @@
         <v>114</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" s="44" t="s">
+      <c r="J5" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="L5" s="45"/>
-      <c r="M5" s="38" t="s">
+      <c r="L5" s="42"/>
+      <c r="M5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="N5" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="44" t="s">
+      <c r="N5" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="38" t="s">
+      <c r="P5" s="42"/>
+      <c r="Q5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="R5" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" s="44" t="s">
+      <c r="R5" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="T5" s="44"/>
-      <c r="U5" s="38" t="s">
+      <c r="T5" s="41"/>
+      <c r="U5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="V5" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="W5" s="44" t="s">
+      <c r="V5" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="W5" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="39" t="s">
+      <c r="X5" s="42"/>
+      <c r="Y5" s="36" t="s">
         <v>54</v>
       </c>
       <c r="Z5" s="5" t="s">
@@ -1828,7 +1818,7 @@
         <v>130</v>
       </c>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="38" t="s">
+      <c r="AC5" s="35" t="s">
         <v>54</v>
       </c>
       <c r="AD5" s="5" t="s">
@@ -1848,7 +1838,7 @@
         <v>97</v>
       </c>
       <c r="AJ5" s="6"/>
-      <c r="AK5" s="38" t="s">
+      <c r="AK5" s="35" t="s">
         <v>54</v>
       </c>
       <c r="AL5" s="5" t="s">
@@ -1858,7 +1848,7 @@
         <v>101</v>
       </c>
       <c r="AN5" s="6"/>
-      <c r="AO5" s="38" t="s">
+      <c r="AO5" s="35" t="s">
         <v>54</v>
       </c>
       <c r="AP5" s="5" t="s">
@@ -1868,7 +1858,7 @@
         <v>108</v>
       </c>
       <c r="AR5" s="6"/>
-      <c r="AS5" s="38" t="s">
+      <c r="AS5" s="35" t="s">
         <v>54</v>
       </c>
       <c r="AT5" s="5" t="s">
@@ -1888,7 +1878,7 @@
         <v>156</v>
       </c>
       <c r="AZ5" s="6"/>
-      <c r="BA5" s="38" t="s">
+      <c r="BA5" s="35" t="s">
         <v>54</v>
       </c>
       <c r="BB5" s="5" t="s">
@@ -1900,59 +1890,59 @@
       <c r="BD5" s="6"/>
     </row>
     <row r="6" spans="1:56" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
+      <c r="B6" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
       <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="44"/>
-      <c r="L6" s="45" t="s">
+      <c r="J6" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6" s="44"/>
-      <c r="P6" s="45" t="s">
+      <c r="N6" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="41"/>
+      <c r="P6" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="Q6" s="38" t="s">
+      <c r="Q6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="R6" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="38" t="s">
+      <c r="R6" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="W6" s="44" t="s">
+      <c r="V6" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="W6" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="39" t="s">
+      <c r="X6" s="42"/>
+      <c r="Y6" s="36" t="s">
         <v>21</v>
       </c>
       <c r="Z6" s="8" t="s">
@@ -1961,7 +1951,7 @@
       <c r="AB6" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="AC6" s="38" t="s">
+      <c r="AC6" s="35" t="s">
         <v>1</v>
       </c>
       <c r="AD6" s="13" t="s">
@@ -1976,7 +1966,7 @@
       <c r="AH6" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AK6" s="38" t="s">
+      <c r="AK6" s="35" t="s">
         <v>21</v>
       </c>
       <c r="AL6" s="8" t="s">
@@ -1984,13 +1974,13 @@
       </c>
       <c r="AM6" s="8"/>
       <c r="AN6" s="9"/>
-      <c r="AO6" s="38" t="s">
+      <c r="AO6" s="35" t="s">
         <v>26</v>
       </c>
       <c r="AP6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AS6" s="38" t="s">
+      <c r="AS6" s="35" t="s">
         <v>1</v>
       </c>
       <c r="AT6" s="8" t="s">
@@ -2002,7 +1992,7 @@
       <c r="AX6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA6" s="38" t="s">
+      <c r="BA6" s="35" t="s">
         <v>46</v>
       </c>
       <c r="BB6" s="8" t="s">
@@ -2010,59 +2000,59 @@
       </c>
     </row>
     <row r="7" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="44" t="s">
+      <c r="B7" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="45"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="38" t="s">
+      <c r="J7" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="45" t="s">
+      <c r="N7" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="41"/>
+      <c r="P7" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="Q7" s="38" t="s">
+      <c r="Q7" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="R7" s="44" t="s">
+      <c r="R7" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="44"/>
-      <c r="T7" s="44" t="s">
+      <c r="S7" s="41"/>
+      <c r="T7" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="U7" s="38" t="s">
+      <c r="U7" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="V7" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="W7" s="44"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="39" t="s">
+      <c r="V7" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="W7" s="41"/>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="36" t="s">
         <v>22</v>
       </c>
       <c r="Z7" s="8" t="s">
@@ -2086,7 +2076,7 @@
       <c r="AI7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AK7" s="38" t="s">
+      <c r="AK7" s="35" t="s">
         <v>1</v>
       </c>
       <c r="AL7" s="8" t="s">
@@ -2096,7 +2086,7 @@
       <c r="AN7" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="AO7" s="38" t="s">
+      <c r="AO7" s="35" t="s">
         <v>27</v>
       </c>
       <c r="AP7" s="8" t="s">
@@ -2105,7 +2095,7 @@
       <c r="AQ7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AS7" s="38" t="s">
+      <c r="AS7" s="35" t="s">
         <v>11</v>
       </c>
       <c r="AT7" s="8" t="s">
@@ -2120,7 +2110,7 @@
       <c r="AX7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA7" s="38" t="s">
+      <c r="BA7" s="35" t="s">
         <v>47</v>
       </c>
       <c r="BB7" s="8" t="s">
@@ -2128,43 +2118,43 @@
       </c>
     </row>
     <row r="8" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="I8" s="38" t="s">
+      <c r="B8" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="I8" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="44"/>
-      <c r="L8" s="45" t="s">
+      <c r="J8" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="44"/>
-      <c r="P8" s="45" t="s">
+      <c r="N8" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="41"/>
+      <c r="P8" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="U8" s="38" t="s">
+      <c r="U8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="W8" s="44"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="39" t="s">
+      <c r="V8" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="W8" s="41"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="36" t="s">
         <v>1</v>
       </c>
       <c r="Z8" s="8" t="s">
@@ -2173,7 +2163,7 @@
       <c r="AB8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="AC8" s="38" t="s">
+      <c r="AC8" s="35" t="s">
         <v>48</v>
       </c>
       <c r="AD8" s="13" t="s">
@@ -2185,7 +2175,7 @@
       <c r="AH8" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="AK8" s="38" t="s">
+      <c r="AK8" s="35" t="s">
         <v>24</v>
       </c>
       <c r="AL8" s="8" t="s">
@@ -2195,13 +2185,13 @@
       <c r="AN8" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AO8" s="38" t="s">
+      <c r="AO8" s="35" t="s">
         <v>176</v>
       </c>
       <c r="AP8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AS8" s="38" t="s">
+      <c r="AS8" s="35" t="s">
         <v>165</v>
       </c>
       <c r="AT8" s="8" t="s">
@@ -2216,7 +2206,7 @@
       <c r="AX8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA8" s="38" t="s">
+      <c r="BA8" s="35" t="s">
         <v>48</v>
       </c>
       <c r="BB8" s="8" t="s">
@@ -2224,43 +2214,43 @@
       </c>
     </row>
     <row r="9" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="45"/>
-      <c r="I9" s="38" t="s">
+      <c r="B9" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="I9" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="44"/>
-      <c r="L9" s="45" t="s">
+      <c r="J9" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="N9" s="44" t="s">
+      <c r="N9" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="O9" s="44"/>
-      <c r="P9" s="45" t="s">
+      <c r="O9" s="41"/>
+      <c r="P9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="U9" s="38" t="s">
+      <c r="U9" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="V9" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="W9" s="44"/>
-      <c r="X9" s="45"/>
-      <c r="Y9" s="39" t="s">
+      <c r="V9" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" s="41"/>
+      <c r="X9" s="42"/>
+      <c r="Y9" s="36" t="s">
         <v>24</v>
       </c>
       <c r="Z9" s="8" t="s">
@@ -2269,7 +2259,7 @@
       <c r="AB9" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AC9" s="38" t="s">
+      <c r="AC9" s="35" t="s">
         <v>147</v>
       </c>
       <c r="AD9" s="13" t="s">
@@ -2281,7 +2271,7 @@
       <c r="AH9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AK9" s="38" t="s">
+      <c r="AK9" s="35" t="s">
         <v>25</v>
       </c>
       <c r="AL9" s="8" t="s">
@@ -2291,7 +2281,7 @@
       <c r="AN9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AO9" s="38" t="s">
+      <c r="AO9" s="35" t="s">
         <v>177</v>
       </c>
       <c r="AP9" s="8" t="s">
@@ -2303,7 +2293,7 @@
       <c r="AX9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA9" s="38" t="s">
+      <c r="BA9" s="35" t="s">
         <v>147</v>
       </c>
       <c r="BB9" s="8" t="s">
@@ -2311,35 +2301,35 @@
       </c>
     </row>
     <row r="10" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="45"/>
-      <c r="I10" s="38" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="I10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="44"/>
-      <c r="L10" s="45" t="s">
+      <c r="J10" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="M10" s="38" t="s">
+      <c r="M10" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="O10" s="44"/>
-      <c r="P10" s="45" t="s">
+      <c r="N10" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="41"/>
+      <c r="P10" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="Y10" s="39" t="s">
+      <c r="Y10" s="36" t="s">
         <v>25</v>
       </c>
       <c r="Z10" s="8" t="s">
@@ -2348,7 +2338,7 @@
       <c r="AB10" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AC10" s="38" t="s">
+      <c r="AC10" s="35" t="s">
         <v>27</v>
       </c>
       <c r="AD10" s="8" t="s">
@@ -2358,7 +2348,7 @@
         <v>85</v>
       </c>
       <c r="AH10" s="8"/>
-      <c r="AK10" s="38" t="s">
+      <c r="AK10" s="35" t="s">
         <v>6</v>
       </c>
       <c r="AL10" s="8" t="s">
@@ -2377,7 +2367,7 @@
       <c r="AY10" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="BA10" s="38" t="s">
+      <c r="BA10" s="35" t="s">
         <v>136</v>
       </c>
       <c r="BB10" s="8" t="s">
@@ -2385,21 +2375,21 @@
       </c>
     </row>
     <row r="11" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="M11" s="41" t="s">
+      <c r="B11" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="M11" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="43"/>
-      <c r="Y11" s="39" t="s">
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="40"/>
+      <c r="Y11" s="36" t="s">
         <v>6</v>
       </c>
       <c r="Z11" s="8" t="s">
@@ -2408,13 +2398,13 @@
       <c r="AB11" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AC11" s="38" t="s">
+      <c r="AC11" s="35" t="s">
         <v>176</v>
       </c>
       <c r="AD11" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AK11" s="39" t="s">
+      <c r="AK11" s="36" t="s">
         <v>152</v>
       </c>
       <c r="AL11" s="8" t="s">
@@ -2424,7 +2414,7 @@
       <c r="AN11" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="BA11" s="38" t="s">
+      <c r="BA11" s="35" t="s">
         <v>155</v>
       </c>
       <c r="BB11" s="8" t="s">
@@ -2439,13 +2429,13 @@
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
-      <c r="M12" s="41" t="s">
+      <c r="M12" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="43"/>
-      <c r="Y12" s="39" t="s">
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="40"/>
+      <c r="Y12" s="36" t="s">
         <v>11</v>
       </c>
       <c r="Z12" s="8" t="s">
@@ -2457,13 +2447,13 @@
       <c r="AB12" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AC12" s="38" t="s">
+      <c r="AC12" s="35" t="s">
         <v>177</v>
       </c>
       <c r="AD12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AK12" s="39" t="s">
+      <c r="AK12" s="36" t="s">
         <v>153</v>
       </c>
       <c r="AL12" s="8" t="s">
@@ -2479,13 +2469,13 @@
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
-      <c r="M13" s="38" t="s">
+      <c r="M13" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="40"/>
-      <c r="Y13" s="39" t="s">
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="37"/>
+      <c r="Y13" s="36" t="s">
         <v>152</v>
       </c>
       <c r="Z13" s="8" t="s">
@@ -2494,7 +2484,7 @@
       <c r="AB13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AK13" s="39" t="s">
+      <c r="AK13" s="36" t="s">
         <v>160</v>
       </c>
       <c r="AL13" s="8" t="s">
@@ -2506,13 +2496,13 @@
       </c>
     </row>
     <row r="14" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="M14" s="38" t="s">
+      <c r="M14" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="40"/>
-      <c r="Y14" s="39" t="s">
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="37"/>
+      <c r="Y14" s="36" t="s">
         <v>153</v>
       </c>
       <c r="Z14" s="8" t="s">
@@ -2521,7 +2511,7 @@
       <c r="AB14" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AK14" s="39" t="s">
+      <c r="AK14" s="36" t="s">
         <v>150</v>
       </c>
       <c r="AL14" s="8" t="s">
@@ -2533,13 +2523,13 @@
       </c>
     </row>
     <row r="15" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="40"/>
-      <c r="Y15" s="39" t="s">
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="37"/>
+      <c r="Y15" s="36" t="s">
         <v>160</v>
       </c>
       <c r="Z15" s="8" t="s">
@@ -2548,7 +2538,7 @@
       <c r="AB15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AK15" s="39" t="s">
+      <c r="AK15" s="36" t="s">
         <v>23</v>
       </c>
       <c r="AL15" s="8" t="s">
@@ -2558,13 +2548,13 @@
       <c r="AN15" s="9"/>
     </row>
     <row r="16" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y16" s="39" t="s">
+      <c r="Y16" s="36" t="s">
         <v>150</v>
       </c>
       <c r="Z16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AK16" s="42" t="s">
+      <c r="AK16" s="39" t="s">
         <v>26</v>
       </c>
       <c r="AL16" s="19" t="s">
@@ -2574,7 +2564,7 @@
       <c r="AN16" s="9"/>
     </row>
     <row r="17" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y17" s="39" t="s">
+      <c r="Y17" s="36" t="s">
         <v>23</v>
       </c>
       <c r="Z17" s="8" t="s">
@@ -2583,7 +2573,7 @@
       <c r="AB17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AK17" s="42" t="s">
+      <c r="AK17" s="39" t="s">
         <v>27</v>
       </c>
       <c r="AL17" s="19" t="s">
@@ -2595,7 +2585,7 @@
       <c r="AN17" s="9"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y18" s="42" t="s">
+      <c r="Y18" s="39" t="s">
         <v>26</v>
       </c>
       <c r="Z18" s="19" t="s">
@@ -2603,7 +2593,7 @@
       </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="20"/>
-      <c r="AK18" s="42" t="s">
+      <c r="AK18" s="39" t="s">
         <v>176</v>
       </c>
       <c r="AL18" s="19" t="s">
@@ -2613,7 +2603,7 @@
       <c r="AN18" s="9"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y19" s="42" t="s">
+      <c r="Y19" s="39" t="s">
         <v>27</v>
       </c>
       <c r="Z19" s="19" t="s">
@@ -2623,7 +2613,7 @@
         <v>85</v>
       </c>
       <c r="AB19" s="20"/>
-      <c r="AK19" s="42" t="s">
+      <c r="AK19" s="39" t="s">
         <v>177</v>
       </c>
       <c r="AL19" s="19" t="s">
@@ -2633,7 +2623,7 @@
       <c r="AN19" s="9"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y20" s="42" t="s">
+      <c r="Y20" s="39" t="s">
         <v>176</v>
       </c>
       <c r="Z20" s="19" t="s">
@@ -2647,7 +2637,7 @@
       <c r="AN20" s="9"/>
     </row>
     <row r="21" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="Y21" s="42" t="s">
+      <c r="Y21" s="39" t="s">
         <v>177</v>
       </c>
       <c r="Z21" s="19" t="s">
@@ -2657,90 +2647,90 @@
       <c r="AB21" s="20"/>
     </row>
     <row r="22" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="35" t="s">
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="35" t="s">
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="35" t="s">
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="35" t="s">
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="35" t="s">
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="V22" s="36"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="35" t="s">
+      <c r="V22" s="45"/>
+      <c r="W22" s="45"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="Z22" s="36"/>
-      <c r="AA22" s="36"/>
-      <c r="AB22" s="37"/>
-      <c r="AC22" s="35" t="s">
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="45"/>
+      <c r="AB22" s="46"/>
+      <c r="AC22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="AD22" s="36"/>
-      <c r="AE22" s="36"/>
-      <c r="AF22" s="37"/>
-      <c r="AG22" s="35" t="s">
+      <c r="AD22" s="45"/>
+      <c r="AE22" s="45"/>
+      <c r="AF22" s="46"/>
+      <c r="AG22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="AH22" s="36"/>
-      <c r="AI22" s="36"/>
-      <c r="AJ22" s="37"/>
-      <c r="AK22" s="35" t="s">
+      <c r="AH22" s="45"/>
+      <c r="AI22" s="45"/>
+      <c r="AJ22" s="46"/>
+      <c r="AK22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="AL22" s="36"/>
-      <c r="AM22" s="36"/>
-      <c r="AN22" s="37"/>
-      <c r="AO22" s="35" t="s">
+      <c r="AL22" s="45"/>
+      <c r="AM22" s="45"/>
+      <c r="AN22" s="46"/>
+      <c r="AO22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="AP22" s="36"/>
-      <c r="AQ22" s="36"/>
-      <c r="AR22" s="37"/>
-      <c r="AS22" s="35" t="s">
+      <c r="AP22" s="45"/>
+      <c r="AQ22" s="45"/>
+      <c r="AR22" s="46"/>
+      <c r="AS22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="AT22" s="36"/>
-      <c r="AU22" s="36"/>
-      <c r="AV22" s="37"/>
-      <c r="AW22" s="35" t="s">
+      <c r="AT22" s="45"/>
+      <c r="AU22" s="45"/>
+      <c r="AV22" s="46"/>
+      <c r="AW22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="AX22" s="36"/>
-      <c r="AY22" s="36"/>
-      <c r="AZ22" s="37"/>
-      <c r="BA22" s="35" t="s">
+      <c r="AX22" s="45"/>
+      <c r="AY22" s="45"/>
+      <c r="AZ22" s="46"/>
+      <c r="BA22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="BB22" s="36"/>
-      <c r="BC22" s="36"/>
-      <c r="BD22" s="37"/>
+      <c r="BB22" s="45"/>
+      <c r="BC22" s="45"/>
+      <c r="BD22" s="46"/>
     </row>
     <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
@@ -3060,7 +3050,7 @@
       <c r="AZ24" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="BA24" s="47" t="s">
+      <c r="BA24" s="24" t="s">
         <v>19</v>
       </c>
       <c r="BB24" s="5" t="s">
@@ -3456,7 +3446,7 @@
         <v>1</v>
       </c>
       <c r="AZ27" s="6"/>
-      <c r="BA27" s="47" t="s">
+      <c r="BA27" s="24" t="s">
         <v>0</v>
       </c>
       <c r="BB27" s="5" t="s">
@@ -3574,7 +3564,7 @@
         <v>144</v>
       </c>
       <c r="AZ28" s="26"/>
-      <c r="BA28" s="47" t="s">
+      <c r="BA28" s="24" t="s">
         <v>10</v>
       </c>
       <c r="BB28" s="5" t="s">
@@ -3688,7 +3678,7 @@
         <v>144</v>
       </c>
       <c r="AZ29" s="26"/>
-      <c r="BA29" s="47" t="s">
+      <c r="BA29" s="24" t="s">
         <v>8</v>
       </c>
       <c r="BB29" s="5" t="s">
@@ -3796,7 +3786,7 @@
       <c r="AZ30" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BA30" s="47" t="s">
+      <c r="BA30" s="24" t="s">
         <v>15</v>
       </c>
       <c r="BB30" s="5" t="s">
@@ -3902,7 +3892,7 @@
       <c r="AZ31" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BA31" s="47" t="s">
+      <c r="BA31" s="24" t="s">
         <v>14</v>
       </c>
       <c r="BB31" s="5" t="s">
@@ -4001,7 +3991,7 @@
       <c r="AX32" s="5"/>
       <c r="AY32" s="5"/>
       <c r="AZ32" s="6"/>
-      <c r="BA32" s="47" t="s">
+      <c r="BA32" s="24" t="s">
         <v>16</v>
       </c>
       <c r="BB32" s="5" t="s">

</xml_diff>

<commit_message>
[FIX] connectors and status
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1597" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A453DA6-4A3C-4625-9924-30CA87573A51}"/>
+  <xr:revisionPtr revIDLastSave="1602" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{465E2173-E5DA-4276-9DFD-282CA60B94D7}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="178">
   <si>
     <t>Organism</t>
   </si>
@@ -120,9 +120,6 @@
     <t>strand</t>
   </si>
   <si>
-    <t>position_left</t>
-  </si>
-  <si>
     <t>Operon Comments</t>
   </si>
   <si>
@@ -568,13 +565,16 @@
   </si>
   <si>
     <t>stop</t>
+  </si>
+  <si>
+    <t>length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,13 +598,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -727,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -792,18 +785,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -816,23 +803,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -841,7 +827,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,6 +839,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,8 +1157,8 @@
   <dimension ref="A1:BD42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1237,832 +1224,832 @@
   <sheetData>
     <row r="1" spans="1:56" s="2" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="N1" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="T1" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="W1" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="X1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AA1" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="AB1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="43" t="s">
+      <c r="AC1" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AE1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="AE1" s="11" t="s">
-        <v>91</v>
-      </c>
       <c r="AF1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH1" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI1" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AK1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AR1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AS1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AW1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AL1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AM1" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AN1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO1" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP1" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AQ1" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="AR1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AT1" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU1" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AV1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW1" s="10" t="s">
+      <c r="AX1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AY1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AX1" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="AY1" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ1" s="12" t="s">
-        <v>32</v>
-      </c>
       <c r="BA1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="BB1" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="BB1" s="11" t="s">
+      <c r="BC1" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="BC1" s="11" t="s">
+      <c r="BD1" s="12" t="s">
         <v>133</v>
-      </c>
-      <c r="BD1" s="12" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="41" t="s">
+      <c r="A2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="B2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="41" t="s">
+      <c r="J2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="41" t="s">
+      <c r="N2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="41" t="s">
+      <c r="R2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="36" t="s">
-        <v>50</v>
+      <c r="V2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="38"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="33" t="s">
+        <v>49</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="35" t="s">
-        <v>50</v>
+      <c r="AC2" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="6"/>
-      <c r="AK2" s="35" t="s">
-        <v>50</v>
+      <c r="AK2" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM2" s="5"/>
       <c r="AN2" s="6"/>
-      <c r="AO2" s="35" t="s">
-        <v>50</v>
+      <c r="AO2" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="AP2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AQ2" s="5"/>
       <c r="AR2" s="6"/>
-      <c r="AS2" s="35" t="s">
-        <v>50</v>
+      <c r="AS2" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="AT2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AU2" s="5"/>
       <c r="AV2" s="6"/>
       <c r="AW2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AX2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AY2" s="5"/>
       <c r="AZ2" s="6"/>
-      <c r="BA2" s="35" t="s">
-        <v>50</v>
+      <c r="BA2" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC2" s="5"/>
       <c r="BD2" s="6"/>
     </row>
     <row r="3" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
+      <c r="A3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" s="41"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="R3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" s="41"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="36" t="s">
-        <v>51</v>
+      <c r="I3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="38"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="38"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="38"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA3" s="5"/>
       <c r="AB3" s="6"/>
-      <c r="AC3" s="35" t="s">
-        <v>51</v>
+      <c r="AC3" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE3" s="5"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
-      <c r="AK3" s="35" t="s">
-        <v>51</v>
+      <c r="AK3" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="6"/>
-      <c r="AO3" s="35" t="s">
-        <v>51</v>
+      <c r="AO3" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="AP3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="6"/>
-      <c r="AS3" s="35" t="s">
-        <v>51</v>
+      <c r="AS3" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="AT3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AU3" s="5"/>
       <c r="AV3" s="6"/>
       <c r="AW3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AX3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="6"/>
-      <c r="BA3" s="35" t="s">
-        <v>51</v>
+      <c r="BA3" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="BB3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BC3" s="5"/>
       <c r="BD3" s="6"/>
     </row>
     <row r="4" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
+      <c r="A4" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="J4" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="41"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="N4" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="O4" s="41"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="R4" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="S4" s="41"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="V4" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="W4" s="41"/>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="35" t="s">
-        <v>148</v>
+      <c r="I4" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="38"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="38"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="R4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="38"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="V4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" s="38"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="35" t="s">
-        <v>148</v>
+      <c r="AC4" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE4" s="5"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="6"/>
-      <c r="AK4" s="35" t="s">
-        <v>148</v>
+      <c r="AK4" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="AL4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AM4" s="5"/>
       <c r="AN4" s="6"/>
-      <c r="AO4" s="35" t="s">
-        <v>148</v>
+      <c r="AO4" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="AP4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="6"/>
-      <c r="AS4" s="35" t="s">
-        <v>148</v>
+      <c r="AS4" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AU4" s="5"/>
       <c r="AV4" s="6"/>
       <c r="AW4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AX4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AY4" s="5"/>
       <c r="AZ4" s="6"/>
-      <c r="BA4" s="35" t="s">
-        <v>148</v>
+      <c r="BA4" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="BB4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BC4" s="5"/>
       <c r="BD4" s="6"/>
     </row>
     <row r="5" spans="1:56" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="41" t="s">
+      <c r="A5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="39"/>
+      <c r="M5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="R5" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="T5" s="41"/>
-      <c r="U5" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="V5" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="W5" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="36" t="s">
-        <v>54</v>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" s="38"/>
+      <c r="U5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="W5" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="35" t="s">
-        <v>54</v>
+      <c r="AC5" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AF5" s="6"/>
       <c r="AG5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AH5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI5" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AJ5" s="6"/>
-      <c r="AK5" s="35" t="s">
-        <v>54</v>
+      <c r="AK5" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN5" s="6"/>
-      <c r="AO5" s="35" t="s">
-        <v>54</v>
+      <c r="AO5" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="AP5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AQ5" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AR5" s="6"/>
-      <c r="AS5" s="35" t="s">
-        <v>54</v>
+      <c r="AS5" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AU5" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AV5" s="6"/>
       <c r="AW5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AX5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AY5" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AZ5" s="6"/>
-      <c r="BA5" s="35" t="s">
-        <v>54</v>
+      <c r="BA5" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="BB5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC5" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BD5" s="6"/>
     </row>
     <row r="6" spans="1:56" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
+      <c r="B6" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="M6" s="35" t="s">
+      <c r="J6" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="38"/>
+      <c r="L6" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="M6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6" s="41"/>
-      <c r="P6" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q6" s="35" t="s">
+      <c r="N6" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="38"/>
+      <c r="P6" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R6" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="35" t="s">
+      <c r="R6" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="W6" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="36" t="s">
+      <c r="V6" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="W6" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="33" t="s">
         <v>21</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB6" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC6" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC6" s="32" t="s">
         <v>1</v>
       </c>
       <c r="AD6" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AF6" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AG6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="AH6" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK6" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK6" s="32" t="s">
         <v>21</v>
       </c>
       <c r="AL6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM6" s="8"/>
       <c r="AN6" s="9"/>
-      <c r="AO6" s="35" t="s">
+      <c r="AO6" s="32" t="s">
         <v>26</v>
       </c>
       <c r="AP6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS6" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS6" s="32" t="s">
         <v>1</v>
       </c>
       <c r="AT6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AW6" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AX6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA6" s="35" t="s">
-        <v>46</v>
+      <c r="BA6" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="BB6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="42"/>
+      <c r="A7" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="39"/>
       <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q7" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="R7" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="38"/>
+      <c r="P7" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="R7" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="U7" s="35" t="s">
+      <c r="S7" s="38"/>
+      <c r="T7" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="U7" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="V7" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="W7" s="41"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="36" t="s">
+      <c r="V7" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="W7" s="38"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="33" t="s">
         <v>22</v>
       </c>
       <c r="Z7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AD7" s="13" t="s">
         <v>7</v>
@@ -2071,111 +2058,111 @@
         <v>27</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK7" s="32" t="s">
         <v>1</v>
       </c>
       <c r="AL7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM7" s="8"/>
       <c r="AN7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO7" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO7" s="32" t="s">
         <v>27</v>
       </c>
       <c r="AP7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AQ7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS7" s="32" t="s">
         <v>11</v>
       </c>
       <c r="AT7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AU7" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW7" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AX7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA7" s="35" t="s">
-        <v>47</v>
+      <c r="BA7" s="32" t="s">
+        <v>46</v>
       </c>
       <c r="BB7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="I8" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="M8" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="U8" s="35" t="s">
+      <c r="B8" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="I8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="38"/>
+      <c r="P8" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="U8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="W8" s="41"/>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="36" t="s">
+      <c r="V8" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="W8" s="38"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="33" t="s">
         <v>1</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB8" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC8" s="35" t="s">
-        <v>48</v>
+        <v>82</v>
+      </c>
+      <c r="AC8" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="AD8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="AG8" s="7" t="s">
-        <v>28</v>
+        <v>175</v>
       </c>
       <c r="AH8" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK8" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK8" s="32" t="s">
         <v>24</v>
       </c>
       <c r="AL8" s="8" t="s">
@@ -2183,84 +2170,84 @@
       </c>
       <c r="AM8" s="8"/>
       <c r="AN8" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO8" s="35" t="s">
-        <v>176</v>
+        <v>101</v>
+      </c>
+      <c r="AO8" s="32" t="s">
+        <v>175</v>
       </c>
       <c r="AP8" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS8" s="35" t="s">
-        <v>165</v>
+        <v>65</v>
+      </c>
+      <c r="AS8" s="32" t="s">
+        <v>164</v>
       </c>
       <c r="AT8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="AV8" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AW8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AX8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA8" s="35" t="s">
-        <v>48</v>
+      <c r="BA8" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="BB8" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="I9" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="41"/>
-      <c r="L9" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="M9" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="N9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="O9" s="41"/>
-      <c r="P9" s="42" t="s">
+      <c r="B9" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="I9" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="38"/>
+      <c r="L9" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="N9" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="U9" s="35" t="s">
+      <c r="O9" s="38"/>
+      <c r="P9" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="V9" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="W9" s="41"/>
-      <c r="X9" s="42"/>
-      <c r="Y9" s="36" t="s">
+      <c r="V9" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="W9" s="38"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="33" t="s">
         <v>24</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC9" s="35" t="s">
-        <v>147</v>
+        <v>102</v>
+      </c>
+      <c r="AC9" s="32" t="s">
+        <v>146</v>
       </c>
       <c r="AD9" s="13" t="s">
         <v>7</v>
@@ -2269,159 +2256,165 @@
         <v>26</v>
       </c>
       <c r="AH9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK9" s="32" t="s">
         <v>25</v>
       </c>
       <c r="AL9" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM9" s="8"/>
       <c r="AN9" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO9" s="35" t="s">
-        <v>177</v>
+        <v>101</v>
+      </c>
+      <c r="AO9" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="AP9" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AW9" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AX9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA9" s="35" t="s">
-        <v>147</v>
+      <c r="BA9" s="32" t="s">
+        <v>146</v>
       </c>
       <c r="BB9" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="I10" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="M10" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="N10" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="O10" s="41"/>
-      <c r="P10" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y10" s="36" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="39"/>
+      <c r="I10" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="38"/>
+      <c r="P10" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y10" s="33" t="s">
         <v>25</v>
       </c>
       <c r="Z10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB10" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC10" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC10" s="32" t="s">
         <v>27</v>
       </c>
       <c r="AD10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH10" s="8"/>
-      <c r="AK10" s="35" t="s">
+      <c r="AK10" s="32" t="s">
         <v>6</v>
       </c>
       <c r="AL10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM10" s="8"/>
       <c r="AN10" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="AO10" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP10" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="AW10" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AX10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AY10" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="BA10" s="35" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="BA10" s="32" t="s">
+        <v>135</v>
       </c>
       <c r="BB10" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="M11" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="40"/>
-      <c r="Y11" s="36" t="s">
+      <c r="B11" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="M11" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="37"/>
+      <c r="Y11" s="33" t="s">
         <v>6</v>
       </c>
       <c r="Z11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB11" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC11" s="35" t="s">
-        <v>176</v>
+        <v>103</v>
+      </c>
+      <c r="AC11" s="32" t="s">
+        <v>175</v>
       </c>
       <c r="AD11" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK11" s="36" t="s">
-        <v>152</v>
+        <v>65</v>
+      </c>
+      <c r="AK11" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="AL11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM11" s="8"/>
       <c r="AN11" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="BA11" s="35" t="s">
-        <v>155</v>
+        <v>85</v>
+      </c>
+      <c r="BA11" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="BB11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC11" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:56" ht="72" x14ac:dyDescent="0.3">
@@ -2429,39 +2422,39 @@
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
-      <c r="M12" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="40"/>
-      <c r="Y12" s="36" t="s">
+      <c r="M12" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="37"/>
+      <c r="Y12" s="33" t="s">
         <v>11</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB12" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC12" s="35" t="s">
-        <v>177</v>
+        <v>83</v>
+      </c>
+      <c r="AC12" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="AD12" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK12" s="36" t="s">
-        <v>153</v>
+        <v>65</v>
+      </c>
+      <c r="AK12" s="33" t="s">
+        <v>152</v>
       </c>
       <c r="AL12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM12" s="8"/>
       <c r="AN12" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
@@ -2469,165 +2462,165 @@
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
-      <c r="M13" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="37"/>
-      <c r="Y13" s="36" t="s">
-        <v>152</v>
+      <c r="M13" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="34"/>
+      <c r="Y13" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB13" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK13" s="36" t="s">
-        <v>160</v>
+        <v>85</v>
+      </c>
+      <c r="AK13" s="33" t="s">
+        <v>159</v>
       </c>
       <c r="AL13" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM13" s="8"/>
       <c r="AN13" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="M14" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="37"/>
-      <c r="Y14" s="36" t="s">
-        <v>153</v>
+      <c r="M14" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="34"/>
+      <c r="Y14" s="33" t="s">
+        <v>152</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB14" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK14" s="36" t="s">
-        <v>150</v>
+        <v>86</v>
+      </c>
+      <c r="AK14" s="33" t="s">
+        <v>149</v>
       </c>
       <c r="AL14" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM14" s="8"/>
       <c r="AN14" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M15" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="37"/>
-      <c r="Y15" s="36" t="s">
-        <v>160</v>
+      <c r="M15" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="34"/>
+      <c r="Y15" s="33" t="s">
+        <v>159</v>
       </c>
       <c r="Z15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB15" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK15" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK15" s="33" t="s">
         <v>23</v>
       </c>
       <c r="AL15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM15" s="8"/>
       <c r="AN15" s="9"/>
     </row>
     <row r="16" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y16" s="36" t="s">
-        <v>150</v>
+      <c r="Y16" s="33" t="s">
+        <v>149</v>
       </c>
       <c r="Z16" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK16" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK16" s="36" t="s">
         <v>26</v>
       </c>
       <c r="AL16" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM16" s="19"/>
       <c r="AN16" s="9"/>
     </row>
     <row r="17" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y17" s="36" t="s">
+      <c r="Y17" s="33" t="s">
         <v>23</v>
       </c>
       <c r="Z17" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB17" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK17" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK17" s="36" t="s">
         <v>27</v>
       </c>
       <c r="AL17" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM17" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN17" s="9"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y18" s="39" t="s">
+      <c r="Y18" s="36" t="s">
         <v>26</v>
       </c>
       <c r="Z18" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="20"/>
-      <c r="AK18" s="39" t="s">
-        <v>176</v>
+      <c r="AK18" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="AL18" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AM18" s="19"/>
       <c r="AN18" s="9"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y19" s="39" t="s">
+      <c r="Y19" s="36" t="s">
         <v>27</v>
       </c>
       <c r="Z19" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA19" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB19" s="20"/>
-      <c r="AK19" s="39" t="s">
-        <v>177</v>
+      <c r="AK19" s="36" t="s">
+        <v>176</v>
       </c>
       <c r="AL19" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AM19" s="19"/>
       <c r="AN19" s="9"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y20" s="39" t="s">
-        <v>176</v>
+      <c r="Y20" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="Z20" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA20" s="19"/>
       <c r="AB20" s="20"/>
@@ -2637,761 +2630,761 @@
       <c r="AN20" s="9"/>
     </row>
     <row r="21" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="Y21" s="39" t="s">
-        <v>177</v>
+      <c r="Y21" s="36" t="s">
+        <v>176</v>
       </c>
       <c r="Z21" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA21" s="19"/>
       <c r="AB21" s="20"/>
     </row>
     <row r="22" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="46"/>
-      <c r="U22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="V22" s="45"/>
-      <c r="W22" s="45"/>
-      <c r="X22" s="46"/>
-      <c r="Y22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z22" s="45"/>
-      <c r="AA22" s="45"/>
-      <c r="AB22" s="46"/>
-      <c r="AC22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD22" s="45"/>
-      <c r="AE22" s="45"/>
-      <c r="AF22" s="46"/>
-      <c r="AG22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="AH22" s="45"/>
-      <c r="AI22" s="45"/>
-      <c r="AJ22" s="46"/>
-      <c r="AK22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="AL22" s="45"/>
-      <c r="AM22" s="45"/>
-      <c r="AN22" s="46"/>
-      <c r="AO22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="AP22" s="45"/>
-      <c r="AQ22" s="45"/>
-      <c r="AR22" s="46"/>
-      <c r="AS22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="AT22" s="45"/>
-      <c r="AU22" s="45"/>
-      <c r="AV22" s="46"/>
-      <c r="AW22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="AX22" s="45"/>
-      <c r="AY22" s="45"/>
-      <c r="AZ22" s="46"/>
-      <c r="BA22" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="BB22" s="45"/>
-      <c r="BC22" s="45"/>
-      <c r="BD22" s="46"/>
+      <c r="A22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="42"/>
+      <c r="AB22" s="43"/>
+      <c r="AC22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD22" s="42"/>
+      <c r="AE22" s="42"/>
+      <c r="AF22" s="43"/>
+      <c r="AG22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH22" s="42"/>
+      <c r="AI22" s="42"/>
+      <c r="AJ22" s="43"/>
+      <c r="AK22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL22" s="42"/>
+      <c r="AM22" s="42"/>
+      <c r="AN22" s="43"/>
+      <c r="AO22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP22" s="42"/>
+      <c r="AQ22" s="42"/>
+      <c r="AR22" s="43"/>
+      <c r="AS22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT22" s="42"/>
+      <c r="AU22" s="42"/>
+      <c r="AV22" s="43"/>
+      <c r="AW22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX22" s="42"/>
+      <c r="AY22" s="42"/>
+      <c r="AZ22" s="43"/>
+      <c r="BA22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="BB22" s="42"/>
+      <c r="BC22" s="42"/>
+      <c r="BD22" s="43"/>
     </row>
     <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="D23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="G23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="G23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="H23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="J23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="K23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="K23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="L23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="N23" s="17" t="s">
+      <c r="O23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="O23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="P23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="R23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="R23" s="17" t="s">
+      <c r="S23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="S23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="T23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="V23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="V23" s="17" t="s">
+      <c r="W23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="W23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="X23" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Y23" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="Z23" s="17" t="s">
+      <c r="AA23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="AA23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="AB23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AC23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="AD23" s="17" t="s">
+      <c r="AE23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="AE23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="AF23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AG23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AH23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="AH23" s="17" t="s">
+      <c r="AI23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="AI23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="AJ23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="AL23" s="17" t="s">
+      <c r="AM23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="AM23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="AN23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AO23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="AP23" s="17" t="s">
+      <c r="AQ23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="AQ23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="AR23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AS23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AT23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="AT23" s="17" t="s">
+      <c r="AU23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="AU23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="AV23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AW23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AX23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="AX23" s="17" t="s">
+      <c r="AY23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="AY23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="AZ23" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BA23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB23" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="BB23" s="17" t="s">
+      <c r="BC23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="BC23" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="BD23" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M24" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="R24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T24" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="U24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="U24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="V24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X24" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="Z24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AB24" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="AC24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="AD24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF24" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG24" s="23" t="s">
         <v>19</v>
       </c>
       <c r="AH24" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI24" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AJ24" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="AK24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="AK24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="AL24" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM24" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AN24" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="AO24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="AP24" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ24" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AR24" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="AS24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="AT24" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AU24" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AV24" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="AX24" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY24" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AZ24" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="BA24" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="BA24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="BB24" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC24" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BD24" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="32" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T25" s="9"/>
-      <c r="U25" s="24" t="s">
+      <c r="U25" s="32" t="s">
         <v>20</v>
       </c>
       <c r="V25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AC25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AD25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AG25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AH25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI25" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AL25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM25" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AN25" s="6"/>
       <c r="AO25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AP25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ25" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AR25" s="6"/>
       <c r="AS25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AT25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AU25" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AV25" s="6"/>
       <c r="AW25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AX25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY25" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AZ25" s="6"/>
       <c r="BA25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BB25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC25" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BD25" s="6"/>
     </row>
     <row r="26" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
-        <v>37</v>
+      <c r="A26" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>37</v>
+        <v>141</v>
+      </c>
+      <c r="I26" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M26" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M26" s="32" t="s">
         <v>10</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q26" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q26" s="32" t="s">
         <v>10</v>
       </c>
       <c r="R26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="U26" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="U26" s="32" t="s">
         <v>10</v>
       </c>
       <c r="V26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W26" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Z26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA26" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AC26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AD26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE26" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AG26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AH26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AJ26" s="6"/>
       <c r="AK26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AL26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AN26" s="6"/>
       <c r="AO26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AP26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AR26" s="6"/>
-      <c r="AS26" s="24" t="s">
+      <c r="AS26" s="32" t="s">
         <v>0</v>
       </c>
       <c r="AT26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AU26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AV26" s="6"/>
       <c r="AW26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AX26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AZ26" s="6"/>
       <c r="BA26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="BB26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BD26" s="6"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M27" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M27" s="32" t="s">
         <v>8</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q27" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q27" s="32" t="s">
         <v>15</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S27" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y27" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y27" s="33" t="s">
         <v>0</v>
       </c>
       <c r="Z27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA27" s="8">
         <v>1</v>
       </c>
-      <c r="AC27" s="29" t="s">
+      <c r="AC27" s="33" t="s">
         <v>0</v>
       </c>
       <c r="AD27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE27" s="8">
         <v>1</v>
@@ -3400,57 +3393,57 @@
         <v>0</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI27" s="5">
         <v>1</v>
       </c>
       <c r="AJ27" s="6"/>
-      <c r="AK27" s="29" t="s">
+      <c r="AK27" s="33" t="s">
         <v>0</v>
       </c>
       <c r="AL27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM27" s="5">
         <v>1</v>
       </c>
       <c r="AN27" s="6"/>
-      <c r="AO27" s="29" t="s">
+      <c r="AO27" s="33" t="s">
         <v>0</v>
       </c>
       <c r="AP27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ27" s="5">
         <v>1</v>
       </c>
       <c r="AR27" s="6"/>
-      <c r="AS27" s="24" t="s">
+      <c r="AS27" s="32" t="s">
         <v>10</v>
       </c>
       <c r="AT27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AU27" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AV27" s="6"/>
       <c r="AW27" s="5" t="s">
         <v>0</v>
       </c>
       <c r="AX27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY27" s="5">
         <v>1</v>
       </c>
       <c r="AZ27" s="6"/>
-      <c r="BA27" s="24" t="s">
+      <c r="BA27" s="32" t="s">
         <v>0</v>
       </c>
       <c r="BB27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC27" s="5">
         <v>1</v>
@@ -3458,165 +3451,165 @@
       <c r="BD27" s="6"/>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y28" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y28" s="33" t="s">
         <v>18</v>
       </c>
       <c r="Z28" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA28" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC28" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC28" s="32" t="s">
         <v>10</v>
       </c>
       <c r="AD28" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE28" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AG28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AH28" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI28" s="5">
         <v>1</v>
       </c>
       <c r="AJ28" s="6"/>
-      <c r="AK28" s="34" t="s">
+      <c r="AK28" s="44" t="s">
         <v>18</v>
       </c>
       <c r="AL28" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM28" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN28" s="25"/>
-      <c r="AO28" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN28" s="24"/>
+      <c r="AO28" s="32" t="s">
         <v>10</v>
       </c>
       <c r="AP28" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ28" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AR28" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AS28" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS28" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AT28" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AU28" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AV28" s="26"/>
+        <v>141</v>
+      </c>
+      <c r="AV28" s="25"/>
       <c r="AW28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AX28" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY28" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AZ28" s="26"/>
-      <c r="BA28" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="AZ28" s="25"/>
+      <c r="BA28" s="32" t="s">
         <v>10</v>
       </c>
       <c r="BB28" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC28" s="5">
         <v>1</v>
       </c>
-      <c r="BD28" s="26"/>
+      <c r="BD28" s="25"/>
     </row>
     <row r="29" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M29" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M29" s="32" t="s">
         <v>15</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y29" s="29" t="s">
-        <v>37</v>
+        <v>141</v>
+      </c>
+      <c r="Y29" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="Z29" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA29" s="8">
         <v>1</v>
@@ -3625,40 +3618,40 @@
         <v>9</v>
       </c>
       <c r="AD29" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE29" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AG29" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AH29" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI29" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AJ29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK29" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK29" s="44" t="s">
         <v>10</v>
       </c>
       <c r="AL29" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM29" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN29" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO29" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN29" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO29" s="32" t="s">
         <v>8</v>
       </c>
       <c r="AP29" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ29" s="5">
         <v>1</v>
@@ -3672,103 +3665,103 @@
         <v>8</v>
       </c>
       <c r="AX29" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY29" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AZ29" s="26"/>
-      <c r="BA29" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="AZ29" s="25"/>
+      <c r="BA29" s="32" t="s">
         <v>8</v>
       </c>
       <c r="BB29" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC29" s="5">
         <v>1</v>
       </c>
-      <c r="BD29" s="26"/>
+      <c r="BD29" s="25"/>
     </row>
     <row r="30" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M30" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M30" s="32" t="s">
         <v>14</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y30" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y30" s="33" t="s">
         <v>8</v>
       </c>
       <c r="Z30" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA30" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC30" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC30" s="33" t="s">
         <v>15</v>
       </c>
       <c r="AD30" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE30" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AG30" s="4"/>
-      <c r="AH30" s="28"/>
+      <c r="AH30" s="27"/>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="6"/>
-      <c r="AK30" s="24" t="s">
+      <c r="AK30" s="32" t="s">
         <v>8</v>
       </c>
       <c r="AL30" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM30" s="5">
         <v>1</v>
       </c>
       <c r="AN30" s="6"/>
-      <c r="AO30" s="24" t="s">
+      <c r="AO30" s="32" t="s">
         <v>15</v>
       </c>
       <c r="AP30" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ30" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AR30" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AS30" s="4"/>
       <c r="AT30" s="5"/>
@@ -3778,103 +3771,103 @@
         <v>15</v>
       </c>
       <c r="AX30" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY30" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AZ30" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="BA30" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="AZ30" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA30" s="32" t="s">
         <v>15</v>
       </c>
       <c r="BB30" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC30" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="BD30" s="26" t="s">
-        <v>47</v>
+        <v>143</v>
+      </c>
+      <c r="BD30" s="25" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M31" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M31" s="32" t="s">
         <v>16</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y31" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y31" s="33" t="s">
         <v>15</v>
       </c>
       <c r="Z31" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AB31" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC31" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC31" s="33" t="s">
         <v>14</v>
       </c>
       <c r="AD31" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE31" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AG31" s="4"/>
-      <c r="AH31" s="28"/>
+      <c r="AH31" s="27"/>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="6"/>
       <c r="AK31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="AL31" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM31" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AN31" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO31" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO31" s="26" t="s">
         <v>13</v>
       </c>
       <c r="AP31" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ31" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AR31" s="26" t="s">
-        <v>47</v>
+        <v>141</v>
+      </c>
+      <c r="AR31" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="AS31" s="4"/>
       <c r="AT31" s="5"/>
@@ -3884,104 +3877,104 @@
         <v>14</v>
       </c>
       <c r="AX31" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AY31" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AZ31" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="BA31" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ31" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA31" s="32" t="s">
         <v>14</v>
       </c>
       <c r="BB31" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC31" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="BD31" s="26" t="s">
-        <v>47</v>
+        <v>141</v>
+      </c>
+      <c r="BD31" s="25" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="32" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y32" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y32" s="33" t="s">
         <v>14</v>
       </c>
       <c r="Z32" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA32" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AB32" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AC32" s="5" t="s">
         <v>13</v>
       </c>
       <c r="AD32" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE32" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF32" s="20"/>
       <c r="AG32" s="4"/>
-      <c r="AH32" s="28"/>
+      <c r="AH32" s="27"/>
       <c r="AI32" s="5"/>
       <c r="AJ32" s="6"/>
-      <c r="AK32" s="34" t="s">
+      <c r="AK32" s="44" t="s">
         <v>14</v>
       </c>
       <c r="AL32" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM32" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN32" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO32" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN32" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO32" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AP32" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ32" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AR32" s="26" t="s">
-        <v>47</v>
+        <v>141</v>
+      </c>
+      <c r="AR32" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="AS32" s="4"/>
       <c r="AT32" s="5"/>
@@ -3991,79 +3984,79 @@
       <c r="AX32" s="5"/>
       <c r="AY32" s="5"/>
       <c r="AZ32" s="6"/>
-      <c r="BA32" s="24" t="s">
+      <c r="BA32" s="32" t="s">
         <v>16</v>
       </c>
       <c r="BB32" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC32" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="BD32" s="26"/>
+        <v>141</v>
+      </c>
+      <c r="BD32" s="25"/>
     </row>
     <row r="33" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>17</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y33" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y33" s="33" t="s">
         <v>16</v>
       </c>
       <c r="Z33" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA33" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AC33" s="5" t="s">
         <v>17</v>
       </c>
       <c r="AD33" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE33" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF33" s="20"/>
       <c r="AG33" s="4"/>
-      <c r="AH33" s="28"/>
+      <c r="AH33" s="27"/>
       <c r="AI33" s="5"/>
       <c r="AJ33" s="6"/>
-      <c r="AK33" s="27" t="s">
+      <c r="AK33" s="26" t="s">
         <v>13</v>
       </c>
       <c r="AL33" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM33" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN33" s="26" t="s">
-        <v>47</v>
+        <v>141</v>
+      </c>
+      <c r="AN33" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="AO33" s="4"/>
       <c r="AP33" s="5"/>
@@ -4087,45 +4080,45 @@
         <v>17</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y34" s="5" t="s">
         <v>13</v>
       </c>
       <c r="Z34" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AB34" s="20"/>
       <c r="AG34" s="4"/>
-      <c r="AH34" s="28"/>
+      <c r="AH34" s="27"/>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="6"/>
-      <c r="AK34" s="27" t="s">
+      <c r="AK34" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AL34" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM34" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN34" s="26" t="s">
-        <v>47</v>
+        <v>141</v>
+      </c>
+      <c r="AN34" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="AO34" s="4"/>
       <c r="AP34" s="5"/>
@@ -4149,20 +4142,20 @@
         <v>17</v>
       </c>
       <c r="Z35" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA35" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AB35" s="20"/>
       <c r="AG35" s="4"/>
-      <c r="AH35" s="28"/>
+      <c r="AH35" s="27"/>
       <c r="AI35" s="5"/>
       <c r="AJ35" s="6"/>
-      <c r="AK35" s="27"/>
-      <c r="AL35" s="28"/>
-      <c r="AM35" s="28"/>
-      <c r="AN35" s="25"/>
+      <c r="AK35" s="26"/>
+      <c r="AL35" s="27"/>
+      <c r="AM35" s="27"/>
+      <c r="AN35" s="24"/>
       <c r="AO35" s="4"/>
       <c r="AP35" s="5"/>
       <c r="AQ35" s="5"/>
@@ -4182,13 +4175,13 @@
     </row>
     <row r="36" spans="1:56" x14ac:dyDescent="0.3">
       <c r="AG36" s="4"/>
-      <c r="AH36" s="28"/>
+      <c r="AH36" s="27"/>
       <c r="AI36" s="5"/>
       <c r="AJ36" s="6"/>
-      <c r="AK36" s="27"/>
-      <c r="AL36" s="28"/>
-      <c r="AM36" s="28"/>
-      <c r="AN36" s="25"/>
+      <c r="AK36" s="26"/>
+      <c r="AL36" s="27"/>
+      <c r="AM36" s="27"/>
+      <c r="AN36" s="24"/>
       <c r="AO36" s="4"/>
       <c r="AP36" s="5"/>
       <c r="AQ36" s="5"/>
@@ -4208,13 +4201,13 @@
     </row>
     <row r="37" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AG37" s="4"/>
-      <c r="AH37" s="28"/>
+      <c r="AH37" s="27"/>
       <c r="AI37" s="5"/>
       <c r="AJ37" s="6"/>
-      <c r="AK37" s="27"/>
-      <c r="AL37" s="28"/>
-      <c r="AM37" s="28"/>
-      <c r="AN37" s="25"/>
+      <c r="AK37" s="26"/>
+      <c r="AL37" s="27"/>
+      <c r="AM37" s="27"/>
+      <c r="AN37" s="24"/>
       <c r="AO37" s="4"/>
       <c r="AP37" s="5"/>
       <c r="AQ37" s="5"/>
@@ -4233,21 +4226,21 @@
       <c r="BD37" s="6"/>
     </row>
     <row r="38" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="31" t="s">
         <v>166</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>167</v>
       </c>
       <c r="AC38" s="8"/>
       <c r="AG38" s="4"/>
-      <c r="AH38" s="28"/>
+      <c r="AH38" s="27"/>
       <c r="AI38" s="5"/>
       <c r="AJ38" s="6"/>
       <c r="AK38" s="5"/>
-      <c r="AL38" s="28"/>
-      <c r="AM38" s="28"/>
-      <c r="AN38" s="25"/>
+      <c r="AL38" s="27"/>
+      <c r="AM38" s="27"/>
+      <c r="AN38" s="24"/>
       <c r="AO38" s="5"/>
       <c r="AP38" s="5"/>
       <c r="AQ38" s="5"/>
@@ -4267,37 +4260,37 @@
     </row>
     <row r="39" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="AO39" s="15"/>
     </row>
     <row r="40" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="AK40" s="8"/>
       <c r="AO40" s="8"/>
     </row>
     <row r="41" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>174</v>
+      <c r="B42" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] loaders and more
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1602" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{465E2173-E5DA-4276-9DFD-282CA60B94D7}"/>
+  <xr:revisionPtr revIDLastSave="1610" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A81682C-342F-4157-875B-2D5AC7527FAD}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="179">
   <si>
     <t>Organism</t>
   </si>
@@ -568,6 +568,9 @@
   </si>
   <si>
     <t>length</t>
+  </si>
+  <si>
+    <t>site_hash</t>
   </si>
 </sst>
 </file>
@@ -830,6 +833,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -839,7 +843,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,9 +1159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:BD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG9" sqref="AG9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2379,7 +2382,9 @@
       <c r="M11" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="N11" s="36"/>
+      <c r="N11" s="38" t="s">
+        <v>48</v>
+      </c>
       <c r="O11" s="36"/>
       <c r="P11" s="37"/>
       <c r="Y11" s="33" t="s">
@@ -2401,11 +2406,17 @@
         <v>151</v>
       </c>
       <c r="AL11" s="8" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="AM11" s="8"/>
       <c r="AN11" s="9" t="s">
         <v>85</v>
+      </c>
+      <c r="AO11" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="AP11" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="BA11" s="32" t="s">
         <v>154</v>
@@ -2425,7 +2436,9 @@
       <c r="M12" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="N12" s="36"/>
+      <c r="N12" s="38" t="s">
+        <v>48</v>
+      </c>
       <c r="O12" s="36"/>
       <c r="P12" s="37"/>
       <c r="Y12" s="33" t="s">
@@ -2450,7 +2463,7 @@
         <v>152</v>
       </c>
       <c r="AL12" s="8" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="AM12" s="8"/>
       <c r="AN12" s="9" t="s">
@@ -2465,14 +2478,16 @@
       <c r="M13" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="N13" s="33"/>
+      <c r="N13" s="38" t="s">
+        <v>48</v>
+      </c>
       <c r="O13" s="33"/>
       <c r="P13" s="34"/>
       <c r="Y13" s="33" t="s">
         <v>151</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="AB13" s="9" t="s">
         <v>85</v>
@@ -2492,14 +2507,16 @@
       <c r="M14" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="N14" s="33"/>
+      <c r="N14" s="38" t="s">
+        <v>65</v>
+      </c>
       <c r="O14" s="33"/>
       <c r="P14" s="34"/>
       <c r="Y14" s="33" t="s">
         <v>152</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="AB14" s="9" t="s">
         <v>86</v>
@@ -2519,7 +2536,9 @@
       <c r="M15" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="N15" s="33"/>
+      <c r="N15" s="38" t="s">
+        <v>48</v>
+      </c>
       <c r="O15" s="33"/>
       <c r="P15" s="34"/>
       <c r="Y15" s="33" t="s">
@@ -2640,90 +2659,90 @@
       <c r="AB21" s="20"/>
     </row>
     <row r="22" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="41" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="41" t="s">
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="41" t="s">
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="41" t="s">
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="44"/>
+      <c r="Q22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="43"/>
-      <c r="U22" s="41" t="s">
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="V22" s="42"/>
-      <c r="W22" s="42"/>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="41" t="s">
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="44"/>
+      <c r="Y22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="Z22" s="42"/>
-      <c r="AA22" s="42"/>
-      <c r="AB22" s="43"/>
-      <c r="AC22" s="41" t="s">
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="43"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="AD22" s="42"/>
-      <c r="AE22" s="42"/>
-      <c r="AF22" s="43"/>
-      <c r="AG22" s="41" t="s">
+      <c r="AD22" s="43"/>
+      <c r="AE22" s="43"/>
+      <c r="AF22" s="44"/>
+      <c r="AG22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="AH22" s="42"/>
-      <c r="AI22" s="42"/>
-      <c r="AJ22" s="43"/>
-      <c r="AK22" s="41" t="s">
+      <c r="AH22" s="43"/>
+      <c r="AI22" s="43"/>
+      <c r="AJ22" s="44"/>
+      <c r="AK22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="AL22" s="42"/>
-      <c r="AM22" s="42"/>
-      <c r="AN22" s="43"/>
-      <c r="AO22" s="41" t="s">
+      <c r="AL22" s="43"/>
+      <c r="AM22" s="43"/>
+      <c r="AN22" s="44"/>
+      <c r="AO22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="AP22" s="42"/>
-      <c r="AQ22" s="42"/>
-      <c r="AR22" s="43"/>
-      <c r="AS22" s="41" t="s">
+      <c r="AP22" s="43"/>
+      <c r="AQ22" s="43"/>
+      <c r="AR22" s="44"/>
+      <c r="AS22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="AT22" s="42"/>
-      <c r="AU22" s="42"/>
-      <c r="AV22" s="43"/>
-      <c r="AW22" s="41" t="s">
+      <c r="AT22" s="43"/>
+      <c r="AU22" s="43"/>
+      <c r="AV22" s="44"/>
+      <c r="AW22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="AX22" s="42"/>
-      <c r="AY22" s="42"/>
-      <c r="AZ22" s="43"/>
-      <c r="BA22" s="41" t="s">
+      <c r="AX22" s="43"/>
+      <c r="AY22" s="43"/>
+      <c r="AZ22" s="44"/>
+      <c r="BA22" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="BB22" s="42"/>
-      <c r="BC22" s="42"/>
-      <c r="BD22" s="43"/>
+      <c r="BB22" s="43"/>
+      <c r="BC22" s="43"/>
+      <c r="BD22" s="44"/>
     </row>
     <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
@@ -3515,7 +3534,7 @@
         <v>1</v>
       </c>
       <c r="AJ28" s="6"/>
-      <c r="AK28" s="44" t="s">
+      <c r="AK28" s="41" t="s">
         <v>18</v>
       </c>
       <c r="AL28" s="13" t="s">
@@ -3635,7 +3654,7 @@
       <c r="AJ29" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AK29" s="44" t="s">
+      <c r="AK29" s="41" t="s">
         <v>10</v>
       </c>
       <c r="AL29" s="13" t="s">
@@ -3952,7 +3971,7 @@
       <c r="AH32" s="27"/>
       <c r="AI32" s="5"/>
       <c r="AJ32" s="6"/>
-      <c r="AK32" s="44" t="s">
+      <c r="AK32" s="41" t="s">
         <v>14</v>
       </c>
       <c r="AL32" s="13" t="s">

</xml_diff>

<commit_message>
[ADD] collectf transformer annotation
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\OneDrive - Universidade do Minho\PhD\Protrend\main\protrend-database\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1610" documentId="8_{B89A609F-9AEF-497E-8FA4-82AB64538E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A81682C-342F-4157-875B-2D5AC7527FAD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBC6D18-32D0-49D8-980E-DEA7177D7E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,6 +615,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -723,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -806,16 +820,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,7 +841,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -842,6 +863,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,9 +1186,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:BD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK2" sqref="AK2:AK19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,7 +1337,7 @@
       <c r="AB1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="40" t="s">
+      <c r="AC1" s="38" t="s">
         <v>88</v>
       </c>
       <c r="AD1" s="11" t="s">
@@ -1396,15 +1423,15 @@
       </c>
     </row>
     <row r="2" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="4" t="s">
+      <c r="B2" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="43" t="s">
         <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1412,39 +1439,39 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="32" t="s">
+      <c r="J2" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="36"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="32" t="s">
+      <c r="N2" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="32" t="s">
+      <c r="R2" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="38"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="33" t="s">
+      <c r="V2" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="36"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="48" t="s">
         <v>49</v>
       </c>
       <c r="Z2" s="5" t="s">
@@ -1452,7 +1479,7 @@
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="32" t="s">
+      <c r="AC2" s="39" t="s">
         <v>49</v>
       </c>
       <c r="AD2" s="5" t="s">
@@ -1468,7 +1495,7 @@
       </c>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="6"/>
-      <c r="AK2" s="32" t="s">
+      <c r="AK2" s="43" t="s">
         <v>49</v>
       </c>
       <c r="AL2" s="5" t="s">
@@ -1476,7 +1503,7 @@
       </c>
       <c r="AM2" s="5"/>
       <c r="AN2" s="6"/>
-      <c r="AO2" s="32" t="s">
+      <c r="AO2" s="39" t="s">
         <v>49</v>
       </c>
       <c r="AP2" s="5" t="s">
@@ -1484,7 +1511,7 @@
       </c>
       <c r="AQ2" s="5"/>
       <c r="AR2" s="6"/>
-      <c r="AS2" s="32" t="s">
+      <c r="AS2" s="23" t="s">
         <v>49</v>
       </c>
       <c r="AT2" s="5" t="s">
@@ -1500,7 +1527,7 @@
       </c>
       <c r="AY2" s="5"/>
       <c r="AZ2" s="6"/>
-      <c r="BA2" s="32" t="s">
+      <c r="BA2" s="39" t="s">
         <v>49</v>
       </c>
       <c r="BB2" s="5" t="s">
@@ -1510,15 +1537,15 @@
       <c r="BD2" s="6"/>
     </row>
     <row r="3" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="43" t="s">
         <v>50</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1526,39 +1553,39 @@
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="32" t="s">
+      <c r="K3" s="36"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="32" t="s">
+      <c r="O3" s="36"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="R3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="32" t="s">
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="V3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="38"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="33" t="s">
+      <c r="W3" s="36"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="48" t="s">
         <v>50</v>
       </c>
       <c r="Z3" s="5" t="s">
@@ -1566,7 +1593,7 @@
       </c>
       <c r="AA3" s="5"/>
       <c r="AB3" s="6"/>
-      <c r="AC3" s="32" t="s">
+      <c r="AC3" s="39" t="s">
         <v>50</v>
       </c>
       <c r="AD3" s="5" t="s">
@@ -1582,7 +1609,7 @@
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="6"/>
-      <c r="AK3" s="32" t="s">
+      <c r="AK3" s="43" t="s">
         <v>50</v>
       </c>
       <c r="AL3" s="5" t="s">
@@ -1590,7 +1617,7 @@
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="6"/>
-      <c r="AO3" s="32" t="s">
+      <c r="AO3" s="39" t="s">
         <v>50</v>
       </c>
       <c r="AP3" s="5" t="s">
@@ -1598,7 +1625,7 @@
       </c>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="6"/>
-      <c r="AS3" s="32" t="s">
+      <c r="AS3" s="23" t="s">
         <v>50</v>
       </c>
       <c r="AT3" s="5" t="s">
@@ -1614,7 +1641,7 @@
       </c>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="6"/>
-      <c r="BA3" s="32" t="s">
+      <c r="BA3" s="39" t="s">
         <v>50</v>
       </c>
       <c r="BB3" s="5" t="s">
@@ -1624,15 +1651,15 @@
       <c r="BD3" s="6"/>
     </row>
     <row r="4" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1640,39 +1667,39 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="32" t="s">
+      <c r="K4" s="36"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="38"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="32" t="s">
+      <c r="O4" s="36"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="R4" s="38" t="s">
+      <c r="R4" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="38"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="32" t="s">
+      <c r="S4" s="36"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="V4" s="38" t="s">
+      <c r="V4" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="W4" s="38"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="32" t="s">
+      <c r="W4" s="36"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="Z4" s="5" t="s">
@@ -1680,7 +1707,7 @@
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="32" t="s">
+      <c r="AC4" s="39" t="s">
         <v>147</v>
       </c>
       <c r="AD4" s="5" t="s">
@@ -1696,7 +1723,7 @@
       </c>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="6"/>
-      <c r="AK4" s="32" t="s">
+      <c r="AK4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="AL4" s="5" t="s">
@@ -1704,7 +1731,7 @@
       </c>
       <c r="AM4" s="5"/>
       <c r="AN4" s="6"/>
-      <c r="AO4" s="32" t="s">
+      <c r="AO4" s="39" t="s">
         <v>147</v>
       </c>
       <c r="AP4" s="5" t="s">
@@ -1712,7 +1739,7 @@
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="6"/>
-      <c r="AS4" s="32" t="s">
+      <c r="AS4" s="23" t="s">
         <v>147</v>
       </c>
       <c r="AT4" s="5" t="s">
@@ -1728,7 +1755,7 @@
       </c>
       <c r="AY4" s="5"/>
       <c r="AZ4" s="6"/>
-      <c r="BA4" s="32" t="s">
+      <c r="BA4" s="39" t="s">
         <v>147</v>
       </c>
       <c r="BB4" s="5" t="s">
@@ -1738,17 +1765,17 @@
       <c r="BD4" s="6"/>
     </row>
     <row r="5" spans="1:56" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="37"/>
+      <c r="E5" s="43" t="s">
         <v>53</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1758,47 +1785,47 @@
         <v>113</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="38" t="s">
+      <c r="J5" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="32" t="s">
+      <c r="L5" s="37"/>
+      <c r="M5" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O5" s="38" t="s">
+      <c r="N5" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="32" t="s">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="R5" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="S5" s="38" t="s">
+      <c r="R5" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="T5" s="38"/>
-      <c r="U5" s="32" t="s">
+      <c r="T5" s="36"/>
+      <c r="U5" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="V5" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="W5" s="38" t="s">
+      <c r="V5" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W5" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="33" t="s">
+      <c r="X5" s="37"/>
+      <c r="Y5" s="48" t="s">
         <v>53</v>
       </c>
       <c r="Z5" s="5" t="s">
@@ -1808,7 +1835,7 @@
         <v>129</v>
       </c>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="32" t="s">
+      <c r="AC5" s="39" t="s">
         <v>53</v>
       </c>
       <c r="AD5" s="5" t="s">
@@ -1828,7 +1855,7 @@
         <v>96</v>
       </c>
       <c r="AJ5" s="6"/>
-      <c r="AK5" s="32" t="s">
+      <c r="AK5" s="43" t="s">
         <v>53</v>
       </c>
       <c r="AL5" s="5" t="s">
@@ -1838,7 +1865,7 @@
         <v>100</v>
       </c>
       <c r="AN5" s="6"/>
-      <c r="AO5" s="32" t="s">
+      <c r="AO5" s="39" t="s">
         <v>53</v>
       </c>
       <c r="AP5" s="5" t="s">
@@ -1848,7 +1875,7 @@
         <v>107</v>
       </c>
       <c r="AR5" s="6"/>
-      <c r="AS5" s="32" t="s">
+      <c r="AS5" s="23" t="s">
         <v>53</v>
       </c>
       <c r="AT5" s="5" t="s">
@@ -1868,7 +1895,7 @@
         <v>155</v>
       </c>
       <c r="AZ5" s="6"/>
-      <c r="BA5" s="32" t="s">
+      <c r="BA5" s="39" t="s">
         <v>53</v>
       </c>
       <c r="BB5" s="5" t="s">
@@ -1880,59 +1907,59 @@
       <c r="BD5" s="6"/>
     </row>
     <row r="6" spans="1:56" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="7" t="s">
+      <c r="B6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="43" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="39" t="s">
+      <c r="J6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" s="38"/>
-      <c r="P6" s="39" t="s">
+      <c r="N6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="R6" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="32" t="s">
+      <c r="R6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="W6" s="38" t="s">
+      <c r="V6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W6" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="33" t="s">
+      <c r="X6" s="37"/>
+      <c r="Y6" s="48" t="s">
         <v>21</v>
       </c>
       <c r="Z6" s="8" t="s">
@@ -1941,7 +1968,7 @@
       <c r="AB6" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="AC6" s="32" t="s">
+      <c r="AC6" s="39" t="s">
         <v>1</v>
       </c>
       <c r="AD6" s="13" t="s">
@@ -1956,7 +1983,7 @@
       <c r="AH6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AK6" s="32" t="s">
+      <c r="AK6" s="43" t="s">
         <v>21</v>
       </c>
       <c r="AL6" s="8" t="s">
@@ -1964,13 +1991,13 @@
       </c>
       <c r="AM6" s="8"/>
       <c r="AN6" s="9"/>
-      <c r="AO6" s="32" t="s">
+      <c r="AO6" s="39" t="s">
         <v>26</v>
       </c>
       <c r="AP6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AS6" s="32" t="s">
+      <c r="AS6" s="23" t="s">
         <v>1</v>
       </c>
       <c r="AT6" s="8" t="s">
@@ -1982,7 +2009,7 @@
       <c r="AX6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA6" s="32" t="s">
+      <c r="BA6" s="39" t="s">
         <v>45</v>
       </c>
       <c r="BB6" s="8" t="s">
@@ -1990,59 +2017,59 @@
       </c>
     </row>
     <row r="7" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="38" t="s">
+      <c r="B7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="37"/>
+      <c r="E7" s="43" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="32" t="s">
+      <c r="J7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="36"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" s="38"/>
-      <c r="P7" s="39" t="s">
+      <c r="N7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="36"/>
+      <c r="P7" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="Q7" s="32" t="s">
+      <c r="Q7" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="R7" s="38" t="s">
+      <c r="R7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38" t="s">
+      <c r="S7" s="36"/>
+      <c r="T7" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="U7" s="32" t="s">
+      <c r="U7" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="V7" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="W7" s="38"/>
-      <c r="X7" s="39"/>
-      <c r="Y7" s="33" t="s">
+      <c r="V7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W7" s="36"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="36" t="s">
         <v>22</v>
       </c>
       <c r="Z7" s="8" t="s">
@@ -2051,7 +2078,7 @@
       <c r="AB7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AC7" s="7" t="s">
+      <c r="AC7" s="39" t="s">
         <v>144</v>
       </c>
       <c r="AD7" s="13" t="s">
@@ -2066,7 +2093,7 @@
       <c r="AI7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AK7" s="32" t="s">
+      <c r="AK7" s="43" t="s">
         <v>1</v>
       </c>
       <c r="AL7" s="8" t="s">
@@ -2076,7 +2103,7 @@
       <c r="AN7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="AO7" s="32" t="s">
+      <c r="AO7" s="39" t="s">
         <v>27</v>
       </c>
       <c r="AP7" s="8" t="s">
@@ -2085,7 +2112,7 @@
       <c r="AQ7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AS7" s="32" t="s">
+      <c r="AS7" s="23" t="s">
         <v>11</v>
       </c>
       <c r="AT7" s="8" t="s">
@@ -2100,7 +2127,7 @@
       <c r="AX7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA7" s="32" t="s">
+      <c r="BA7" s="39" t="s">
         <v>46</v>
       </c>
       <c r="BB7" s="8" t="s">
@@ -2108,43 +2135,43 @@
       </c>
     </row>
     <row r="8" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
-      <c r="I8" s="32" t="s">
+      <c r="B8" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="I8" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39" t="s">
+      <c r="J8" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="36"/>
+      <c r="L8" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="39" t="s">
+      <c r="N8" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="36"/>
+      <c r="P8" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="U8" s="32" t="s">
+      <c r="U8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="W8" s="38"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="33" t="s">
+      <c r="V8" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W8" s="36"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="48" t="s">
         <v>1</v>
       </c>
       <c r="Z8" s="8" t="s">
@@ -2153,7 +2180,7 @@
       <c r="AB8" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="AC8" s="32" t="s">
+      <c r="AC8" s="39" t="s">
         <v>47</v>
       </c>
       <c r="AD8" s="13" t="s">
@@ -2165,7 +2192,7 @@
       <c r="AH8" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AK8" s="32" t="s">
+      <c r="AK8" s="43" t="s">
         <v>24</v>
       </c>
       <c r="AL8" s="8" t="s">
@@ -2175,13 +2202,13 @@
       <c r="AN8" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AO8" s="32" t="s">
+      <c r="AO8" s="39" t="s">
         <v>175</v>
       </c>
       <c r="AP8" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AS8" s="32" t="s">
+      <c r="AS8" s="23" t="s">
         <v>164</v>
       </c>
       <c r="AT8" s="8" t="s">
@@ -2196,7 +2223,7 @@
       <c r="AX8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA8" s="32" t="s">
+      <c r="BA8" s="39" t="s">
         <v>47</v>
       </c>
       <c r="BB8" s="8" t="s">
@@ -2204,43 +2231,43 @@
       </c>
     </row>
     <row r="9" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="I9" s="32" t="s">
+      <c r="B9" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="I9" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39" t="s">
+      <c r="J9" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="36"/>
+      <c r="L9" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="N9" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="O9" s="38"/>
-      <c r="P9" s="39" t="s">
+      <c r="O9" s="36"/>
+      <c r="P9" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="U9" s="32" t="s">
+      <c r="U9" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="V9" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="W9" s="38"/>
-      <c r="X9" s="39"/>
-      <c r="Y9" s="33" t="s">
+      <c r="V9" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W9" s="36"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="48" t="s">
         <v>24</v>
       </c>
       <c r="Z9" s="8" t="s">
@@ -2249,7 +2276,7 @@
       <c r="AB9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AC9" s="32" t="s">
+      <c r="AC9" s="39" t="s">
         <v>146</v>
       </c>
       <c r="AD9" s="13" t="s">
@@ -2261,7 +2288,7 @@
       <c r="AH9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AK9" s="32" t="s">
+      <c r="AK9" s="43" t="s">
         <v>25</v>
       </c>
       <c r="AL9" s="8" t="s">
@@ -2271,7 +2298,7 @@
       <c r="AN9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AO9" s="32" t="s">
+      <c r="AO9" s="39" t="s">
         <v>176</v>
       </c>
       <c r="AP9" s="8" t="s">
@@ -2283,7 +2310,7 @@
       <c r="AX9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA9" s="32" t="s">
+      <c r="BA9" s="39" t="s">
         <v>146</v>
       </c>
       <c r="BB9" s="8" t="s">
@@ -2291,35 +2318,35 @@
       </c>
     </row>
     <row r="10" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-      <c r="I10" s="32" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="I10" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39" t="s">
+      <c r="J10" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="36"/>
+      <c r="L10" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N10" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="38"/>
-      <c r="P10" s="39" t="s">
+      <c r="N10" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="36"/>
+      <c r="P10" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Y10" s="33" t="s">
+      <c r="Y10" s="48" t="s">
         <v>25</v>
       </c>
       <c r="Z10" s="8" t="s">
@@ -2328,7 +2355,7 @@
       <c r="AB10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AC10" s="32" t="s">
+      <c r="AC10" s="39" t="s">
         <v>27</v>
       </c>
       <c r="AD10" s="8" t="s">
@@ -2338,7 +2365,7 @@
         <v>84</v>
       </c>
       <c r="AH10" s="8"/>
-      <c r="AK10" s="32" t="s">
+      <c r="AK10" s="43" t="s">
         <v>6</v>
       </c>
       <c r="AL10" s="8" t="s">
@@ -2348,7 +2375,7 @@
       <c r="AN10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AO10" s="32" t="s">
+      <c r="AO10" s="39" t="s">
         <v>177</v>
       </c>
       <c r="AP10" s="8" t="s">
@@ -2363,7 +2390,7 @@
       <c r="AY10" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="BA10" s="32" t="s">
+      <c r="BA10" s="39" t="s">
         <v>135</v>
       </c>
       <c r="BB10" s="8" t="s">
@@ -2371,23 +2398,23 @@
       </c>
     </row>
     <row r="11" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="M11" s="35" t="s">
+      <c r="B11" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="M11" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="N11" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" s="36"/>
-      <c r="P11" s="37"/>
-      <c r="Y11" s="33" t="s">
+      <c r="N11" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="34"/>
+      <c r="P11" s="35"/>
+      <c r="Y11" s="48" t="s">
         <v>6</v>
       </c>
       <c r="Z11" s="8" t="s">
@@ -2396,13 +2423,13 @@
       <c r="AB11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AC11" s="32" t="s">
+      <c r="AC11" s="39" t="s">
         <v>175</v>
       </c>
       <c r="AD11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AK11" s="33" t="s">
+      <c r="AK11" s="48" t="s">
         <v>151</v>
       </c>
       <c r="AL11" s="8" t="s">
@@ -2412,13 +2439,13 @@
       <c r="AN11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AO11" s="7" t="s">
+      <c r="AO11" s="39" t="s">
         <v>178</v>
       </c>
       <c r="AP11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="BA11" s="32" t="s">
+      <c r="BA11" s="39" t="s">
         <v>154</v>
       </c>
       <c r="BB11" s="8" t="s">
@@ -2433,15 +2460,15 @@
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
-      <c r="M12" s="35" t="s">
+      <c r="M12" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="N12" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="36"/>
-      <c r="P12" s="37"/>
-      <c r="Y12" s="33" t="s">
+      <c r="N12" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="34"/>
+      <c r="P12" s="35"/>
+      <c r="Y12" s="48" t="s">
         <v>11</v>
       </c>
       <c r="Z12" s="8" t="s">
@@ -2453,13 +2480,13 @@
       <c r="AB12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="AC12" s="32" t="s">
+      <c r="AC12" s="39" t="s">
         <v>176</v>
       </c>
       <c r="AD12" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AK12" s="33" t="s">
+      <c r="AK12" s="48" t="s">
         <v>152</v>
       </c>
       <c r="AL12" s="8" t="s">
@@ -2475,15 +2502,15 @@
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
-      <c r="M13" s="32" t="s">
+      <c r="M13" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="N13" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O13" s="33"/>
-      <c r="P13" s="34"/>
-      <c r="Y13" s="33" t="s">
+      <c r="N13" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="32"/>
+      <c r="P13" s="33"/>
+      <c r="Y13" s="48" t="s">
         <v>151</v>
       </c>
       <c r="Z13" s="8" t="s">
@@ -2492,7 +2519,7 @@
       <c r="AB13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AK13" s="33" t="s">
+      <c r="AK13" s="48" t="s">
         <v>159</v>
       </c>
       <c r="AL13" s="8" t="s">
@@ -2504,15 +2531,15 @@
       </c>
     </row>
     <row r="14" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="M14" s="32" t="s">
+      <c r="M14" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="N14" s="38" t="s">
+      <c r="N14" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="O14" s="33"/>
-      <c r="P14" s="34"/>
-      <c r="Y14" s="33" t="s">
+      <c r="O14" s="32"/>
+      <c r="P14" s="33"/>
+      <c r="Y14" s="48" t="s">
         <v>152</v>
       </c>
       <c r="Z14" s="8" t="s">
@@ -2521,7 +2548,7 @@
       <c r="AB14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AK14" s="33" t="s">
+      <c r="AK14" s="48" t="s">
         <v>149</v>
       </c>
       <c r="AL14" s="8" t="s">
@@ -2533,15 +2560,15 @@
       </c>
     </row>
     <row r="15" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M15" s="32" t="s">
+      <c r="M15" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="N15" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="O15" s="33"/>
-      <c r="P15" s="34"/>
-      <c r="Y15" s="33" t="s">
+      <c r="N15" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15" s="32"/>
+      <c r="P15" s="33"/>
+      <c r="Y15" s="48" t="s">
         <v>159</v>
       </c>
       <c r="Z15" s="8" t="s">
@@ -2550,7 +2577,7 @@
       <c r="AB15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AK15" s="33" t="s">
+      <c r="AK15" s="48" t="s">
         <v>23</v>
       </c>
       <c r="AL15" s="8" t="s">
@@ -2560,13 +2587,13 @@
       <c r="AN15" s="9"/>
     </row>
     <row r="16" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y16" s="33" t="s">
+      <c r="Y16" s="48" t="s">
         <v>149</v>
       </c>
       <c r="Z16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AK16" s="36" t="s">
+      <c r="AK16" s="49" t="s">
         <v>26</v>
       </c>
       <c r="AL16" s="19" t="s">
@@ -2576,7 +2603,7 @@
       <c r="AN16" s="9"/>
     </row>
     <row r="17" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y17" s="33" t="s">
+      <c r="Y17" s="48" t="s">
         <v>23</v>
       </c>
       <c r="Z17" s="8" t="s">
@@ -2585,7 +2612,7 @@
       <c r="AB17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AK17" s="36" t="s">
+      <c r="AK17" s="49" t="s">
         <v>27</v>
       </c>
       <c r="AL17" s="19" t="s">
@@ -2597,7 +2624,7 @@
       <c r="AN17" s="9"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y18" s="36" t="s">
+      <c r="Y18" s="49" t="s">
         <v>26</v>
       </c>
       <c r="Z18" s="19" t="s">
@@ -2605,7 +2632,7 @@
       </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="20"/>
-      <c r="AK18" s="36" t="s">
+      <c r="AK18" s="49" t="s">
         <v>175</v>
       </c>
       <c r="AL18" s="19" t="s">
@@ -2615,7 +2642,7 @@
       <c r="AN18" s="9"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y19" s="36" t="s">
+      <c r="Y19" s="49" t="s">
         <v>27</v>
       </c>
       <c r="Z19" s="19" t="s">
@@ -2625,7 +2652,7 @@
         <v>84</v>
       </c>
       <c r="AB19" s="20"/>
-      <c r="AK19" s="36" t="s">
+      <c r="AK19" s="49" t="s">
         <v>176</v>
       </c>
       <c r="AL19" s="19" t="s">
@@ -2635,7 +2662,7 @@
       <c r="AN19" s="9"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y20" s="36" t="s">
+      <c r="Y20" s="49" t="s">
         <v>175</v>
       </c>
       <c r="Z20" s="19" t="s">
@@ -2649,7 +2676,7 @@
       <c r="AN20" s="9"/>
     </row>
     <row r="21" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="Y21" s="36" t="s">
+      <c r="Y21" s="49" t="s">
         <v>176</v>
       </c>
       <c r="Z21" s="19" t="s">
@@ -2659,90 +2686,90 @@
       <c r="AB21" s="20"/>
     </row>
     <row r="22" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="42" t="s">
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="42" t="s">
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="42" t="s">
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="42" t="s">
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="R22" s="43"/>
-      <c r="S22" s="43"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="42" t="s">
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="V22" s="43"/>
-      <c r="W22" s="43"/>
-      <c r="X22" s="44"/>
-      <c r="Y22" s="42" t="s">
+      <c r="V22" s="46"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="47"/>
+      <c r="Y22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="43"/>
-      <c r="AB22" s="44"/>
-      <c r="AC22" s="42" t="s">
+      <c r="Z22" s="46"/>
+      <c r="AA22" s="46"/>
+      <c r="AB22" s="47"/>
+      <c r="AC22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="AD22" s="43"/>
-      <c r="AE22" s="43"/>
-      <c r="AF22" s="44"/>
-      <c r="AG22" s="42" t="s">
+      <c r="AD22" s="46"/>
+      <c r="AE22" s="46"/>
+      <c r="AF22" s="47"/>
+      <c r="AG22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="AH22" s="43"/>
-      <c r="AI22" s="43"/>
-      <c r="AJ22" s="44"/>
-      <c r="AK22" s="42" t="s">
+      <c r="AH22" s="46"/>
+      <c r="AI22" s="46"/>
+      <c r="AJ22" s="47"/>
+      <c r="AK22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="AL22" s="43"/>
-      <c r="AM22" s="43"/>
-      <c r="AN22" s="44"/>
-      <c r="AO22" s="42" t="s">
+      <c r="AL22" s="46"/>
+      <c r="AM22" s="46"/>
+      <c r="AN22" s="47"/>
+      <c r="AO22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="AP22" s="43"/>
-      <c r="AQ22" s="43"/>
-      <c r="AR22" s="44"/>
-      <c r="AS22" s="42" t="s">
+      <c r="AP22" s="46"/>
+      <c r="AQ22" s="46"/>
+      <c r="AR22" s="47"/>
+      <c r="AS22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="AT22" s="43"/>
-      <c r="AU22" s="43"/>
-      <c r="AV22" s="44"/>
-      <c r="AW22" s="42" t="s">
+      <c r="AT22" s="46"/>
+      <c r="AU22" s="46"/>
+      <c r="AV22" s="47"/>
+      <c r="AW22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="AX22" s="43"/>
-      <c r="AY22" s="43"/>
-      <c r="AZ22" s="44"/>
-      <c r="BA22" s="42" t="s">
+      <c r="AX22" s="46"/>
+      <c r="AY22" s="46"/>
+      <c r="AZ22" s="47"/>
+      <c r="BA22" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="BB22" s="43"/>
-      <c r="BC22" s="43"/>
-      <c r="BD22" s="44"/>
+      <c r="BB22" s="46"/>
+      <c r="BC22" s="46"/>
+      <c r="BD22" s="47"/>
     </row>
     <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
@@ -2915,7 +2942,7 @@
       </c>
     </row>
     <row r="24" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -2924,7 +2951,7 @@
       <c r="C24" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="39" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2933,7 +2960,7 @@
       <c r="G24" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="39" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="8" t="s">
@@ -2942,7 +2969,7 @@
       <c r="K24" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M24" s="32" t="s">
+      <c r="M24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="N24" s="8" t="s">
@@ -2954,7 +2981,7 @@
       <c r="P24" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="Q24" s="32" t="s">
+      <c r="Q24" s="23" t="s">
         <v>19</v>
       </c>
       <c r="R24" s="8" t="s">
@@ -2966,7 +2993,7 @@
       <c r="T24" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="U24" s="32" t="s">
+      <c r="U24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="V24" s="8" t="s">
@@ -2978,7 +3005,7 @@
       <c r="X24" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="Y24" s="32" t="s">
+      <c r="Y24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="Z24" s="8" t="s">
@@ -2990,7 +3017,7 @@
       <c r="AB24" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AC24" s="32" t="s">
+      <c r="AC24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="AD24" s="8" t="s">
@@ -3014,7 +3041,7 @@
       <c r="AJ24" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="AK24" s="32" t="s">
+      <c r="AK24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="AL24" s="5" t="s">
@@ -3026,7 +3053,7 @@
       <c r="AN24" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="AO24" s="32" t="s">
+      <c r="AO24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="AP24" s="5" t="s">
@@ -3038,7 +3065,7 @@
       <c r="AR24" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="AS24" s="32" t="s">
+      <c r="AS24" s="23" t="s">
         <v>19</v>
       </c>
       <c r="AT24" s="5" t="s">
@@ -3062,7 +3089,7 @@
       <c r="AZ24" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="BA24" s="32" t="s">
+      <c r="BA24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="BB24" s="5" t="s">
@@ -3076,7 +3103,7 @@
       </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -3085,7 +3112,7 @@
       <c r="C25" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="39" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -3122,7 +3149,7 @@
         <v>141</v>
       </c>
       <c r="T25" s="9"/>
-      <c r="U25" s="32" t="s">
+      <c r="U25" s="39" t="s">
         <v>20</v>
       </c>
       <c r="V25" s="8" t="s">
@@ -3131,7 +3158,7 @@
       <c r="W25" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y25" s="4" t="s">
+      <c r="Y25" s="39" t="s">
         <v>114</v>
       </c>
       <c r="Z25" s="8" t="s">
@@ -3140,7 +3167,7 @@
       <c r="AA25" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="AC25" s="4" t="s">
+      <c r="AC25" s="39" t="s">
         <v>114</v>
       </c>
       <c r="AD25" s="8" t="s">
@@ -3159,7 +3186,7 @@
         <v>141</v>
       </c>
       <c r="AJ25" s="6"/>
-      <c r="AK25" s="4" t="s">
+      <c r="AK25" s="39" t="s">
         <v>114</v>
       </c>
       <c r="AL25" s="5" t="s">
@@ -3169,7 +3196,7 @@
         <v>141</v>
       </c>
       <c r="AN25" s="6"/>
-      <c r="AO25" s="4" t="s">
+      <c r="AO25" s="39" t="s">
         <v>114</v>
       </c>
       <c r="AP25" s="5" t="s">
@@ -3179,7 +3206,7 @@
         <v>141</v>
       </c>
       <c r="AR25" s="6"/>
-      <c r="AS25" s="4" t="s">
+      <c r="AS25" s="23" t="s">
         <v>20</v>
       </c>
       <c r="AT25" s="5" t="s">
@@ -3199,7 +3226,7 @@
         <v>141</v>
       </c>
       <c r="AZ25" s="6"/>
-      <c r="BA25" s="4" t="s">
+      <c r="BA25" s="39" t="s">
         <v>114</v>
       </c>
       <c r="BB25" s="5" t="s">
@@ -3211,7 +3238,7 @@
       <c r="BD25" s="6"/>
     </row>
     <row r="26" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="39" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -3229,7 +3256,7 @@
       <c r="G26" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I26" s="32" t="s">
+      <c r="I26" s="39" t="s">
         <v>36</v>
       </c>
       <c r="J26" s="8" t="s">
@@ -3238,7 +3265,7 @@
       <c r="K26" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M26" s="32" t="s">
+      <c r="M26" s="39" t="s">
         <v>10</v>
       </c>
       <c r="N26" s="8" t="s">
@@ -3247,7 +3274,7 @@
       <c r="O26" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q26" s="32" t="s">
+      <c r="Q26" s="23" t="s">
         <v>10</v>
       </c>
       <c r="R26" s="8" t="s">
@@ -3256,7 +3283,7 @@
       <c r="S26" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="U26" s="32" t="s">
+      <c r="U26" s="39" t="s">
         <v>10</v>
       </c>
       <c r="V26" s="8" t="s">
@@ -3265,7 +3292,7 @@
       <c r="W26" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y26" s="4" t="s">
+      <c r="Y26" s="39" t="s">
         <v>20</v>
       </c>
       <c r="Z26" s="8" t="s">
@@ -3313,7 +3340,7 @@
         <v>141</v>
       </c>
       <c r="AR26" s="6"/>
-      <c r="AS26" s="32" t="s">
+      <c r="AS26" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AT26" s="5" t="s">
@@ -3333,7 +3360,7 @@
         <v>141</v>
       </c>
       <c r="AZ26" s="6"/>
-      <c r="BA26" s="4" t="s">
+      <c r="BA26" s="39" t="s">
         <v>20</v>
       </c>
       <c r="BB26" s="5" t="s">
@@ -3345,7 +3372,7 @@
       <c r="BD26" s="6"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3354,7 +3381,7 @@
       <c r="C27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="39" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -3363,7 +3390,7 @@
       <c r="G27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="39" t="s">
         <v>10</v>
       </c>
       <c r="J27" s="8" t="s">
@@ -3372,7 +3399,7 @@
       <c r="K27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M27" s="32" t="s">
+      <c r="M27" s="39" t="s">
         <v>8</v>
       </c>
       <c r="N27" s="8" t="s">
@@ -3381,7 +3408,7 @@
       <c r="O27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q27" s="32" t="s">
+      <c r="Q27" s="23" t="s">
         <v>15</v>
       </c>
       <c r="R27" s="8" t="s">
@@ -3390,7 +3417,7 @@
       <c r="S27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y27" s="33" t="s">
+      <c r="Y27" s="40" t="s">
         <v>0</v>
       </c>
       <c r="Z27" s="8" t="s">
@@ -3399,7 +3426,7 @@
       <c r="AA27" s="8">
         <v>1</v>
       </c>
-      <c r="AC27" s="33" t="s">
+      <c r="AC27" s="40" t="s">
         <v>0</v>
       </c>
       <c r="AD27" s="8" t="s">
@@ -3418,7 +3445,7 @@
         <v>1</v>
       </c>
       <c r="AJ27" s="6"/>
-      <c r="AK27" s="33" t="s">
+      <c r="AK27" s="40" t="s">
         <v>0</v>
       </c>
       <c r="AL27" s="5" t="s">
@@ -3428,7 +3455,7 @@
         <v>1</v>
       </c>
       <c r="AN27" s="6"/>
-      <c r="AO27" s="33" t="s">
+      <c r="AO27" s="40" t="s">
         <v>0</v>
       </c>
       <c r="AP27" s="5" t="s">
@@ -3438,7 +3465,7 @@
         <v>1</v>
       </c>
       <c r="AR27" s="6"/>
-      <c r="AS27" s="32" t="s">
+      <c r="AS27" s="23" t="s">
         <v>10</v>
       </c>
       <c r="AT27" s="5" t="s">
@@ -3458,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="AZ27" s="6"/>
-      <c r="BA27" s="32" t="s">
+      <c r="BA27" s="39" t="s">
         <v>0</v>
       </c>
       <c r="BB27" s="5" t="s">
@@ -3470,7 +3497,7 @@
       <c r="BD27" s="6"/>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -3479,7 +3506,7 @@
       <c r="C28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -3488,7 +3515,7 @@
       <c r="G28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="39" t="s">
         <v>8</v>
       </c>
       <c r="J28" s="8" t="s">
@@ -3506,7 +3533,7 @@
       <c r="O28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y28" s="33" t="s">
+      <c r="Y28" s="36" t="s">
         <v>18</v>
       </c>
       <c r="Z28" s="8" t="s">
@@ -3515,7 +3542,7 @@
       <c r="AA28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="AC28" s="32" t="s">
+      <c r="AC28" s="39" t="s">
         <v>10</v>
       </c>
       <c r="AD28" s="19" t="s">
@@ -3534,7 +3561,7 @@
         <v>1</v>
       </c>
       <c r="AJ28" s="6"/>
-      <c r="AK28" s="41" t="s">
+      <c r="AK28" s="42" t="s">
         <v>18</v>
       </c>
       <c r="AL28" s="13" t="s">
@@ -3544,7 +3571,7 @@
         <v>141</v>
       </c>
       <c r="AN28" s="24"/>
-      <c r="AO28" s="32" t="s">
+      <c r="AO28" s="39" t="s">
         <v>10</v>
       </c>
       <c r="AP28" s="5" t="s">
@@ -3556,7 +3583,7 @@
       <c r="AR28" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AS28" s="26" t="s">
+      <c r="AS28" s="42" t="s">
         <v>17</v>
       </c>
       <c r="AT28" s="13" t="s">
@@ -3576,7 +3603,7 @@
         <v>143</v>
       </c>
       <c r="AZ28" s="25"/>
-      <c r="BA28" s="32" t="s">
+      <c r="BA28" s="39" t="s">
         <v>10</v>
       </c>
       <c r="BB28" s="5" t="s">
@@ -3615,7 +3642,7 @@
       <c r="K29" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M29" s="32" t="s">
+      <c r="M29" s="39" t="s">
         <v>15</v>
       </c>
       <c r="N29" s="8" t="s">
@@ -3624,7 +3651,7 @@
       <c r="O29" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y29" s="33" t="s">
+      <c r="Y29" s="40" t="s">
         <v>36</v>
       </c>
       <c r="Z29" s="8" t="s">
@@ -3666,7 +3693,7 @@
       <c r="AN29" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AO29" s="32" t="s">
+      <c r="AO29" s="39" t="s">
         <v>8</v>
       </c>
       <c r="AP29" s="5" t="s">
@@ -3690,7 +3717,7 @@
         <v>143</v>
       </c>
       <c r="AZ29" s="25"/>
-      <c r="BA29" s="32" t="s">
+      <c r="BA29" s="39" t="s">
         <v>8</v>
       </c>
       <c r="BB29" s="5" t="s">
@@ -3702,7 +3729,7 @@
       <c r="BD29" s="25"/>
     </row>
     <row r="30" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -3711,7 +3738,7 @@
       <c r="C30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="39" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="8" t="s">
@@ -3720,7 +3747,7 @@
       <c r="G30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="39" t="s">
         <v>15</v>
       </c>
       <c r="J30" s="8" t="s">
@@ -3729,7 +3756,7 @@
       <c r="K30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M30" s="32" t="s">
+      <c r="M30" s="39" t="s">
         <v>14</v>
       </c>
       <c r="N30" s="8" t="s">
@@ -3738,7 +3765,7 @@
       <c r="O30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y30" s="33" t="s">
+      <c r="Y30" s="40" t="s">
         <v>8</v>
       </c>
       <c r="Z30" s="8" t="s">
@@ -3747,7 +3774,7 @@
       <c r="AA30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="AC30" s="33" t="s">
+      <c r="AC30" s="40" t="s">
         <v>15</v>
       </c>
       <c r="AD30" s="8" t="s">
@@ -3760,7 +3787,7 @@
       <c r="AH30" s="27"/>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="6"/>
-      <c r="AK30" s="32" t="s">
+      <c r="AK30" s="39" t="s">
         <v>8</v>
       </c>
       <c r="AL30" s="13" t="s">
@@ -3770,7 +3797,7 @@
         <v>1</v>
       </c>
       <c r="AN30" s="6"/>
-      <c r="AO30" s="32" t="s">
+      <c r="AO30" s="39" t="s">
         <v>15</v>
       </c>
       <c r="AP30" s="5" t="s">
@@ -3798,7 +3825,7 @@
       <c r="AZ30" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="BA30" s="32" t="s">
+      <c r="BA30" s="39" t="s">
         <v>15</v>
       </c>
       <c r="BB30" s="5" t="s">
@@ -3812,7 +3839,7 @@
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3821,7 +3848,7 @@
       <c r="C31" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="39" t="s">
         <v>14</v>
       </c>
       <c r="J31" s="8" t="s">
@@ -3830,7 +3857,7 @@
       <c r="K31" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M31" s="32" t="s">
+      <c r="M31" s="23" t="s">
         <v>16</v>
       </c>
       <c r="N31" s="8" t="s">
@@ -3839,7 +3866,7 @@
       <c r="O31" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y31" s="33" t="s">
+      <c r="Y31" s="40" t="s">
         <v>15</v>
       </c>
       <c r="Z31" s="8" t="s">
@@ -3851,7 +3878,7 @@
       <c r="AB31" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AC31" s="33" t="s">
+      <c r="AC31" s="40" t="s">
         <v>14</v>
       </c>
       <c r="AD31" s="8" t="s">
@@ -3904,7 +3931,7 @@
       <c r="AZ31" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="BA31" s="32" t="s">
+      <c r="BA31" s="39" t="s">
         <v>14</v>
       </c>
       <c r="BB31" s="5" t="s">
@@ -3918,7 +3945,7 @@
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -3945,7 +3972,7 @@
       <c r="O32" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y32" s="33" t="s">
+      <c r="Y32" s="40" t="s">
         <v>14</v>
       </c>
       <c r="Z32" s="8" t="s">
@@ -3983,7 +4010,7 @@
       <c r="AN32" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AO32" s="26" t="s">
+      <c r="AO32" s="41" t="s">
         <v>17</v>
       </c>
       <c r="AP32" s="13" t="s">
@@ -4003,7 +4030,7 @@
       <c r="AX32" s="5"/>
       <c r="AY32" s="5"/>
       <c r="AZ32" s="6"/>
-      <c r="BA32" s="32" t="s">
+      <c r="BA32" s="23" t="s">
         <v>16</v>
       </c>
       <c r="BB32" s="5" t="s">
@@ -4033,7 +4060,7 @@
       <c r="K33" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M33" s="4" t="s">
+      <c r="M33" s="39" t="s">
         <v>17</v>
       </c>
       <c r="N33" s="8" t="s">
@@ -4042,7 +4069,7 @@
       <c r="O33" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Y33" s="33" t="s">
+      <c r="Y33" s="36" t="s">
         <v>16</v>
       </c>
       <c r="Z33" s="8" t="s">
@@ -4051,7 +4078,7 @@
       <c r="AA33" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="AC33" s="5" t="s">
+      <c r="AC33" s="40" t="s">
         <v>17</v>
       </c>
       <c r="AD33" s="8" t="s">
@@ -4095,7 +4122,7 @@
       <c r="BD33" s="6"/>
     </row>
     <row r="34" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -4104,7 +4131,7 @@
       <c r="C34" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="39" t="s">
         <v>17</v>
       </c>
       <c r="J34" s="8" t="s">
@@ -4127,7 +4154,7 @@
       <c r="AH34" s="27"/>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="6"/>
-      <c r="AK34" s="26" t="s">
+      <c r="AK34" s="41" t="s">
         <v>17</v>
       </c>
       <c r="AL34" s="13" t="s">
@@ -4157,7 +4184,7 @@
       <c r="BD34" s="6"/>
     </row>
     <row r="35" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y35" s="5" t="s">
+      <c r="Y35" s="40" t="s">
         <v>17</v>
       </c>
       <c r="Z35" s="8" t="s">

</xml_diff>

<commit_message>
[ADD] update collectf annotation
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\OneDrive - Universidade do Minho\PhD\Protrend\main\protrend-database\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BiSBII\OneDrive - Universidade do Minho\PhD\Protrend\main\protrend-database\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBC6D18-32D0-49D8-980E-DEA7177D7E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0D040A-9A49-4F4A-B070-6375476B1ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -855,6 +855,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -863,12 +869,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,8 +1187,8 @@
   <dimension ref="A1:BD42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK2" sqref="AK2:AK19"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="W2" s="36"/>
       <c r="X2" s="37"/>
-      <c r="Y2" s="48" t="s">
+      <c r="Y2" s="45" t="s">
         <v>49</v>
       </c>
       <c r="Z2" s="5" t="s">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="39" t="s">
+      <c r="AC2" s="43" t="s">
         <v>49</v>
       </c>
       <c r="AD2" s="5" t="s">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="AM2" s="5"/>
       <c r="AN2" s="6"/>
-      <c r="AO2" s="39" t="s">
+      <c r="AO2" s="43" t="s">
         <v>49</v>
       </c>
       <c r="AP2" s="5" t="s">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="AY2" s="5"/>
       <c r="AZ2" s="6"/>
-      <c r="BA2" s="39" t="s">
+      <c r="BA2" s="43" t="s">
         <v>49</v>
       </c>
       <c r="BB2" s="5" t="s">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="W3" s="36"/>
       <c r="X3" s="37"/>
-      <c r="Y3" s="48" t="s">
+      <c r="Y3" s="45" t="s">
         <v>50</v>
       </c>
       <c r="Z3" s="5" t="s">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="AA3" s="5"/>
       <c r="AB3" s="6"/>
-      <c r="AC3" s="39" t="s">
+      <c r="AC3" s="43" t="s">
         <v>50</v>
       </c>
       <c r="AD3" s="5" t="s">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="AM3" s="5"/>
       <c r="AN3" s="6"/>
-      <c r="AO3" s="39" t="s">
+      <c r="AO3" s="43" t="s">
         <v>50</v>
       </c>
       <c r="AP3" s="5" t="s">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="6"/>
-      <c r="BA3" s="39" t="s">
+      <c r="BA3" s="43" t="s">
         <v>50</v>
       </c>
       <c r="BB3" s="5" t="s">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="39" t="s">
+      <c r="AC4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="AD4" s="5" t="s">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="AM4" s="5"/>
       <c r="AN4" s="6"/>
-      <c r="AO4" s="39" t="s">
+      <c r="AO4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="AP4" s="5" t="s">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="AY4" s="5"/>
       <c r="AZ4" s="6"/>
-      <c r="BA4" s="39" t="s">
+      <c r="BA4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="BB4" s="5" t="s">
@@ -1825,7 +1825,7 @@
         <v>76</v>
       </c>
       <c r="X5" s="37"/>
-      <c r="Y5" s="48" t="s">
+      <c r="Y5" s="45" t="s">
         <v>53</v>
       </c>
       <c r="Z5" s="5" t="s">
@@ -1835,7 +1835,7 @@
         <v>129</v>
       </c>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="39" t="s">
+      <c r="AC5" s="43" t="s">
         <v>53</v>
       </c>
       <c r="AD5" s="5" t="s">
@@ -1865,7 +1865,7 @@
         <v>100</v>
       </c>
       <c r="AN5" s="6"/>
-      <c r="AO5" s="39" t="s">
+      <c r="AO5" s="43" t="s">
         <v>53</v>
       </c>
       <c r="AP5" s="5" t="s">
@@ -1895,7 +1895,7 @@
         <v>155</v>
       </c>
       <c r="AZ5" s="6"/>
-      <c r="BA5" s="39" t="s">
+      <c r="BA5" s="43" t="s">
         <v>53</v>
       </c>
       <c r="BB5" s="5" t="s">
@@ -1959,7 +1959,7 @@
         <v>77</v>
       </c>
       <c r="X6" s="37"/>
-      <c r="Y6" s="48" t="s">
+      <c r="Y6" s="45" t="s">
         <v>21</v>
       </c>
       <c r="Z6" s="8" t="s">
@@ -1968,7 +1968,7 @@
       <c r="AB6" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="AC6" s="39" t="s">
+      <c r="AC6" s="43" t="s">
         <v>1</v>
       </c>
       <c r="AD6" s="13" t="s">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="AM6" s="8"/>
       <c r="AN6" s="9"/>
-      <c r="AO6" s="39" t="s">
+      <c r="AO6" s="43" t="s">
         <v>26</v>
       </c>
       <c r="AP6" s="8" t="s">
@@ -2009,7 +2009,7 @@
       <c r="AX6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA6" s="39" t="s">
+      <c r="BA6" s="43" t="s">
         <v>45</v>
       </c>
       <c r="BB6" s="8" t="s">
@@ -2078,7 +2078,7 @@
       <c r="AB7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AC7" s="39" t="s">
+      <c r="AC7" s="43" t="s">
         <v>144</v>
       </c>
       <c r="AD7" s="13" t="s">
@@ -2103,7 +2103,7 @@
       <c r="AN7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="AO7" s="39" t="s">
+      <c r="AO7" s="43" t="s">
         <v>27</v>
       </c>
       <c r="AP7" s="8" t="s">
@@ -2127,7 +2127,7 @@
       <c r="AX7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA7" s="39" t="s">
+      <c r="BA7" s="43" t="s">
         <v>46</v>
       </c>
       <c r="BB7" s="8" t="s">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="W8" s="36"/>
       <c r="X8" s="37"/>
-      <c r="Y8" s="48" t="s">
+      <c r="Y8" s="45" t="s">
         <v>1</v>
       </c>
       <c r="Z8" s="8" t="s">
@@ -2180,7 +2180,7 @@
       <c r="AB8" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="AC8" s="39" t="s">
+      <c r="AC8" s="43" t="s">
         <v>47</v>
       </c>
       <c r="AD8" s="13" t="s">
@@ -2202,7 +2202,7 @@
       <c r="AN8" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AO8" s="39" t="s">
+      <c r="AO8" s="43" t="s">
         <v>175</v>
       </c>
       <c r="AP8" s="8" t="s">
@@ -2223,7 +2223,7 @@
       <c r="AX8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA8" s="39" t="s">
+      <c r="BA8" s="43" t="s">
         <v>47</v>
       </c>
       <c r="BB8" s="8" t="s">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="W9" s="36"/>
       <c r="X9" s="37"/>
-      <c r="Y9" s="48" t="s">
+      <c r="Y9" s="45" t="s">
         <v>24</v>
       </c>
       <c r="Z9" s="8" t="s">
@@ -2276,7 +2276,7 @@
       <c r="AB9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AC9" s="39" t="s">
+      <c r="AC9" s="43" t="s">
         <v>146</v>
       </c>
       <c r="AD9" s="13" t="s">
@@ -2298,7 +2298,7 @@
       <c r="AN9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AO9" s="39" t="s">
+      <c r="AO9" s="43" t="s">
         <v>176</v>
       </c>
       <c r="AP9" s="8" t="s">
@@ -2310,7 +2310,7 @@
       <c r="AX9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="BA9" s="39" t="s">
+      <c r="BA9" s="43" t="s">
         <v>146</v>
       </c>
       <c r="BB9" s="8" t="s">
@@ -2346,7 +2346,7 @@
       <c r="P10" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Y10" s="48" t="s">
+      <c r="Y10" s="45" t="s">
         <v>25</v>
       </c>
       <c r="Z10" s="8" t="s">
@@ -2355,7 +2355,7 @@
       <c r="AB10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AC10" s="39" t="s">
+      <c r="AC10" s="43" t="s">
         <v>27</v>
       </c>
       <c r="AD10" s="8" t="s">
@@ -2375,7 +2375,7 @@
       <c r="AN10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AO10" s="39" t="s">
+      <c r="AO10" s="43" t="s">
         <v>177</v>
       </c>
       <c r="AP10" s="8" t="s">
@@ -2390,7 +2390,7 @@
       <c r="AY10" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="BA10" s="39" t="s">
+      <c r="BA10" s="43" t="s">
         <v>135</v>
       </c>
       <c r="BB10" s="8" t="s">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="O11" s="34"/>
       <c r="P11" s="35"/>
-      <c r="Y11" s="48" t="s">
+      <c r="Y11" s="45" t="s">
         <v>6</v>
       </c>
       <c r="Z11" s="8" t="s">
@@ -2423,13 +2423,13 @@
       <c r="AB11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AC11" s="39" t="s">
+      <c r="AC11" s="43" t="s">
         <v>175</v>
       </c>
       <c r="AD11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AK11" s="48" t="s">
+      <c r="AK11" s="45" t="s">
         <v>151</v>
       </c>
       <c r="AL11" s="8" t="s">
@@ -2439,13 +2439,13 @@
       <c r="AN11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AO11" s="39" t="s">
+      <c r="AO11" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AP11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="BA11" s="39" t="s">
+      <c r="BA11" s="43" t="s">
         <v>154</v>
       </c>
       <c r="BB11" s="8" t="s">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="O12" s="34"/>
       <c r="P12" s="35"/>
-      <c r="Y12" s="48" t="s">
+      <c r="Y12" s="45" t="s">
         <v>11</v>
       </c>
       <c r="Z12" s="8" t="s">
@@ -2480,13 +2480,13 @@
       <c r="AB12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="AC12" s="39" t="s">
+      <c r="AC12" s="43" t="s">
         <v>176</v>
       </c>
       <c r="AD12" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AK12" s="48" t="s">
+      <c r="AK12" s="45" t="s">
         <v>152</v>
       </c>
       <c r="AL12" s="8" t="s">
@@ -2510,7 +2510,7 @@
       </c>
       <c r="O13" s="32"/>
       <c r="P13" s="33"/>
-      <c r="Y13" s="48" t="s">
+      <c r="Y13" s="45" t="s">
         <v>151</v>
       </c>
       <c r="Z13" s="8" t="s">
@@ -2519,7 +2519,7 @@
       <c r="AB13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AK13" s="48" t="s">
+      <c r="AK13" s="45" t="s">
         <v>159</v>
       </c>
       <c r="AL13" s="8" t="s">
@@ -2539,7 +2539,7 @@
       </c>
       <c r="O14" s="32"/>
       <c r="P14" s="33"/>
-      <c r="Y14" s="48" t="s">
+      <c r="Y14" s="45" t="s">
         <v>152</v>
       </c>
       <c r="Z14" s="8" t="s">
@@ -2548,7 +2548,7 @@
       <c r="AB14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AK14" s="48" t="s">
+      <c r="AK14" s="45" t="s">
         <v>149</v>
       </c>
       <c r="AL14" s="8" t="s">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="O15" s="32"/>
       <c r="P15" s="33"/>
-      <c r="Y15" s="48" t="s">
+      <c r="Y15" s="45" t="s">
         <v>159</v>
       </c>
       <c r="Z15" s="8" t="s">
@@ -2577,7 +2577,7 @@
       <c r="AB15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AK15" s="48" t="s">
+      <c r="AK15" s="45" t="s">
         <v>23</v>
       </c>
       <c r="AL15" s="8" t="s">
@@ -2587,13 +2587,13 @@
       <c r="AN15" s="9"/>
     </row>
     <row r="16" spans="1:56" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y16" s="48" t="s">
+      <c r="Y16" s="45" t="s">
         <v>149</v>
       </c>
       <c r="Z16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AK16" s="49" t="s">
+      <c r="AK16" s="46" t="s">
         <v>26</v>
       </c>
       <c r="AL16" s="19" t="s">
@@ -2603,7 +2603,7 @@
       <c r="AN16" s="9"/>
     </row>
     <row r="17" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y17" s="48" t="s">
+      <c r="Y17" s="45" t="s">
         <v>23</v>
       </c>
       <c r="Z17" s="8" t="s">
@@ -2612,7 +2612,7 @@
       <c r="AB17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AK17" s="49" t="s">
+      <c r="AK17" s="46" t="s">
         <v>27</v>
       </c>
       <c r="AL17" s="19" t="s">
@@ -2624,7 +2624,7 @@
       <c r="AN17" s="9"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y18" s="49" t="s">
+      <c r="Y18" s="46" t="s">
         <v>26</v>
       </c>
       <c r="Z18" s="19" t="s">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="20"/>
-      <c r="AK18" s="49" t="s">
+      <c r="AK18" s="46" t="s">
         <v>175</v>
       </c>
       <c r="AL18" s="19" t="s">
@@ -2642,7 +2642,7 @@
       <c r="AN18" s="9"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y19" s="49" t="s">
+      <c r="Y19" s="46" t="s">
         <v>27</v>
       </c>
       <c r="Z19" s="19" t="s">
@@ -2652,7 +2652,7 @@
         <v>84</v>
       </c>
       <c r="AB19" s="20"/>
-      <c r="AK19" s="49" t="s">
+      <c r="AK19" s="46" t="s">
         <v>176</v>
       </c>
       <c r="AL19" s="19" t="s">
@@ -2662,7 +2662,7 @@
       <c r="AN19" s="9"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Y20" s="49" t="s">
+      <c r="Y20" s="46" t="s">
         <v>175</v>
       </c>
       <c r="Z20" s="19" t="s">
@@ -2676,7 +2676,7 @@
       <c r="AN20" s="9"/>
     </row>
     <row r="21" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="Y21" s="49" t="s">
+      <c r="Y21" s="46" t="s">
         <v>176</v>
       </c>
       <c r="Z21" s="19" t="s">
@@ -2686,90 +2686,90 @@
       <c r="AB21" s="20"/>
     </row>
     <row r="22" spans="1:56" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="45" t="s">
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="45" t="s">
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="45" t="s">
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="47"/>
-      <c r="Q22" s="45" t="s">
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="R22" s="46"/>
-      <c r="S22" s="46"/>
-      <c r="T22" s="47"/>
-      <c r="U22" s="45" t="s">
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="49"/>
+      <c r="U22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="V22" s="46"/>
-      <c r="W22" s="46"/>
-      <c r="X22" s="47"/>
-      <c r="Y22" s="45" t="s">
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="49"/>
+      <c r="Y22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="Z22" s="46"/>
-      <c r="AA22" s="46"/>
-      <c r="AB22" s="47"/>
-      <c r="AC22" s="45" t="s">
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="48"/>
+      <c r="AB22" s="49"/>
+      <c r="AC22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="AD22" s="46"/>
-      <c r="AE22" s="46"/>
-      <c r="AF22" s="47"/>
-      <c r="AG22" s="45" t="s">
+      <c r="AD22" s="48"/>
+      <c r="AE22" s="48"/>
+      <c r="AF22" s="49"/>
+      <c r="AG22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="AH22" s="46"/>
-      <c r="AI22" s="46"/>
-      <c r="AJ22" s="47"/>
-      <c r="AK22" s="45" t="s">
+      <c r="AH22" s="48"/>
+      <c r="AI22" s="48"/>
+      <c r="AJ22" s="49"/>
+      <c r="AK22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="AL22" s="46"/>
-      <c r="AM22" s="46"/>
-      <c r="AN22" s="47"/>
-      <c r="AO22" s="45" t="s">
+      <c r="AL22" s="48"/>
+      <c r="AM22" s="48"/>
+      <c r="AN22" s="49"/>
+      <c r="AO22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="AP22" s="46"/>
-      <c r="AQ22" s="46"/>
-      <c r="AR22" s="47"/>
-      <c r="AS22" s="45" t="s">
+      <c r="AP22" s="48"/>
+      <c r="AQ22" s="48"/>
+      <c r="AR22" s="49"/>
+      <c r="AS22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="AT22" s="46"/>
-      <c r="AU22" s="46"/>
-      <c r="AV22" s="47"/>
-      <c r="AW22" s="45" t="s">
+      <c r="AT22" s="48"/>
+      <c r="AU22" s="48"/>
+      <c r="AV22" s="49"/>
+      <c r="AW22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="AX22" s="46"/>
-      <c r="AY22" s="46"/>
-      <c r="AZ22" s="47"/>
-      <c r="BA22" s="45" t="s">
+      <c r="AX22" s="48"/>
+      <c r="AY22" s="48"/>
+      <c r="AZ22" s="49"/>
+      <c r="BA22" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="BB22" s="46"/>
-      <c r="BC22" s="46"/>
-      <c r="BD22" s="47"/>
+      <c r="BB22" s="48"/>
+      <c r="BC22" s="48"/>
+      <c r="BD22" s="49"/>
     </row>
     <row r="23" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
@@ -2942,7 +2942,7 @@
       </c>
     </row>
     <row r="24" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="43" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -2951,7 +2951,7 @@
       <c r="C24" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="43" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -3112,7 +3112,7 @@
       <c r="C25" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="43" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -3381,7 +3381,7 @@
       <c r="C27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="43" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -3506,7 +3506,7 @@
       <c r="C28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="43" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -3738,7 +3738,7 @@
       <c r="C30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="43" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="8" t="s">

</xml_diff>

<commit_message>
[ADD] model annotation for coryneregnet
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="13_ncr:1_{15E36B38-B12C-4BC5-84DF-7B470AA1660C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC1B7B9C-6FA8-4CFD-9E26-293AC9A1EC90}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:1_{15E36B38-B12C-4BC5-84DF-7B470AA1660C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0462DC2C-8D2C-41E6-9A2D-E8E2D86043AA}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -593,7 +593,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -770,15 +770,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -799,6 +790,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,7 +1118,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AW2" activeCellId="4" sqref="Y2:Y21 AC2:AC13 AK2:AK19 AO2:AO11 AW2:AW11"/>
+      <selection pane="bottomLeft" activeCell="AV13" sqref="AV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1131,7 @@
     <col min="6" max="6" width="10.109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="6" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="5" customWidth="1"/>
     <col min="10" max="10" width="10.88671875" style="6" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" style="6" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" style="7" customWidth="1"/>
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="2" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="16" t="s">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="17"/>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="J2" s="16" t="s">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="N2" s="16" t="s">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="W2" s="16"/>
       <c r="X2" s="17"/>
-      <c r="Y2" s="35" t="s">
+      <c r="Y2" s="32" t="s">
         <v>46</v>
       </c>
       <c r="Z2" s="16" t="s">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="AA2" s="16"/>
       <c r="AB2" s="17"/>
-      <c r="AC2" s="33" t="s">
+      <c r="AC2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="AD2" s="16" t="s">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="AI2" s="16"/>
       <c r="AJ2" s="17"/>
-      <c r="AK2" s="33" t="s">
+      <c r="AK2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="AL2" s="16" t="s">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="AM2" s="16"/>
       <c r="AN2" s="17"/>
-      <c r="AO2" s="33" t="s">
+      <c r="AO2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="AP2" s="16" t="s">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="AU2" s="16"/>
       <c r="AV2" s="17"/>
-      <c r="AW2" s="33" t="s">
+      <c r="AW2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="AX2" s="16" t="s">
@@ -1443,7 +1443,7 @@
       <c r="AZ2" s="17"/>
     </row>
     <row r="3" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="J3" s="16" t="s">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="17"/>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="N3" s="16" t="s">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="W3" s="16"/>
       <c r="X3" s="17"/>
-      <c r="Y3" s="35" t="s">
+      <c r="Y3" s="32" t="s">
         <v>47</v>
       </c>
       <c r="Z3" s="16" t="s">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="AA3" s="16"/>
       <c r="AB3" s="17"/>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="AD3" s="16" t="s">
@@ -1515,7 +1515,7 @@
       </c>
       <c r="AI3" s="16"/>
       <c r="AJ3" s="17"/>
-      <c r="AK3" s="33" t="s">
+      <c r="AK3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="AL3" s="16" t="s">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="AM3" s="16"/>
       <c r="AN3" s="17"/>
-      <c r="AO3" s="33" t="s">
+      <c r="AO3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="AP3" s="16" t="s">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="AU3" s="16"/>
       <c r="AV3" s="17"/>
-      <c r="AW3" s="33" t="s">
+      <c r="AW3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="AX3" s="16" t="s">
@@ -1549,7 +1549,7 @@
       <c r="AZ3" s="17"/>
     </row>
     <row r="4" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="B4" s="16" t="s">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="F4" s="16" t="s">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="J4" s="16" t="s">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="N4" s="16" t="s">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="W4" s="16"/>
       <c r="X4" s="17"/>
-      <c r="Y4" s="33" t="s">
+      <c r="Y4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="Z4" s="16" t="s">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="AA4" s="16"/>
       <c r="AB4" s="17"/>
-      <c r="AC4" s="33" t="s">
+      <c r="AC4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="AD4" s="16" t="s">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="AI4" s="16"/>
       <c r="AJ4" s="17"/>
-      <c r="AK4" s="33" t="s">
+      <c r="AK4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="AL4" s="16" t="s">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="AM4" s="16"/>
       <c r="AN4" s="17"/>
-      <c r="AO4" s="33" t="s">
+      <c r="AO4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="AP4" s="16" t="s">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="AU4" s="16"/>
       <c r="AV4" s="17"/>
-      <c r="AW4" s="33" t="s">
+      <c r="AW4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="AX4" s="16" t="s">
@@ -1655,7 +1655,7 @@
       <c r="AZ4" s="17"/>
     </row>
     <row r="5" spans="1:52" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -1665,7 +1665,7 @@
         <v>55</v>
       </c>
       <c r="D5" s="17"/>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="16" t="s">
@@ -1675,7 +1675,7 @@
         <v>110</v>
       </c>
       <c r="H5" s="17"/>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="J5" s="16" t="s">
@@ -1685,7 +1685,7 @@
         <v>119</v>
       </c>
       <c r="L5" s="17"/>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="N5" s="16" t="s">
@@ -1715,7 +1715,7 @@
         <v>73</v>
       </c>
       <c r="X5" s="17"/>
-      <c r="Y5" s="35" t="s">
+      <c r="Y5" s="32" t="s">
         <v>50</v>
       </c>
       <c r="Z5" s="16" t="s">
@@ -1725,7 +1725,7 @@
         <v>122</v>
       </c>
       <c r="AB5" s="17"/>
-      <c r="AC5" s="33" t="s">
+      <c r="AC5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="AD5" s="16" t="s">
@@ -1745,7 +1745,7 @@
         <v>93</v>
       </c>
       <c r="AJ5" s="17"/>
-      <c r="AK5" s="33" t="s">
+      <c r="AK5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="AL5" s="16" t="s">
@@ -1755,7 +1755,7 @@
         <v>97</v>
       </c>
       <c r="AN5" s="17"/>
-      <c r="AO5" s="33" t="s">
+      <c r="AO5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="AP5" s="16" t="s">
@@ -1775,7 +1775,7 @@
         <v>108</v>
       </c>
       <c r="AV5" s="17"/>
-      <c r="AW5" s="33" t="s">
+      <c r="AW5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="AX5" s="16" t="s">
@@ -1787,7 +1787,7 @@
       <c r="AZ5" s="17"/>
     </row>
     <row r="6" spans="1:52" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="16" t="s">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="30" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="16" t="s">
@@ -1813,7 +1813,7 @@
       <c r="L6" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="N6" s="16" t="s">
@@ -1841,7 +1841,7 @@
         <v>74</v>
       </c>
       <c r="X6" s="17"/>
-      <c r="Y6" s="35" t="s">
+      <c r="Y6" s="32" t="s">
         <v>20</v>
       </c>
       <c r="Z6" s="16" t="s">
@@ -1851,7 +1851,7 @@
       <c r="AB6" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="AC6" s="33" t="s">
+      <c r="AC6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="AD6" s="20" t="s">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="AI6" s="16"/>
       <c r="AJ6" s="17"/>
-      <c r="AK6" s="33" t="s">
+      <c r="AK6" s="30" t="s">
         <v>20</v>
       </c>
       <c r="AL6" s="16" t="s">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="AM6" s="16"/>
       <c r="AN6" s="17"/>
-      <c r="AO6" s="33" t="s">
+      <c r="AO6" s="30" t="s">
         <v>25</v>
       </c>
       <c r="AP6" s="16" t="s">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="AU6" s="16"/>
       <c r="AV6" s="17"/>
-      <c r="AW6" s="33" t="s">
+      <c r="AW6" s="30" t="s">
         <v>42</v>
       </c>
       <c r="AX6" s="16" t="s">
@@ -1903,7 +1903,7 @@
       <c r="AZ6" s="17"/>
     </row>
     <row r="7" spans="1:52" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1913,7 +1913,7 @@
         <v>52</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="30" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="16" t="s">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="30" t="s">
         <v>37</v>
       </c>
       <c r="J7" s="16" t="s">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="K7" s="16"/>
       <c r="L7" s="17"/>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="30" t="s">
         <v>57</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="W7" s="16"/>
       <c r="X7" s="17"/>
-      <c r="Y7" s="35" t="s">
+      <c r="Y7" s="32" t="s">
         <v>21</v>
       </c>
       <c r="Z7" s="16" t="s">
@@ -1967,7 +1967,7 @@
       <c r="AB7" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AC7" s="33" t="s">
+      <c r="AC7" s="30" t="s">
         <v>136</v>
       </c>
       <c r="AD7" s="20" t="s">
@@ -1985,7 +1985,7 @@
         <v>81</v>
       </c>
       <c r="AJ7" s="17"/>
-      <c r="AK7" s="33" t="s">
+      <c r="AK7" s="30" t="s">
         <v>1</v>
       </c>
       <c r="AL7" s="16" t="s">
@@ -1995,7 +1995,7 @@
       <c r="AN7" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="AO7" s="33" t="s">
+      <c r="AO7" s="30" t="s">
         <v>26</v>
       </c>
       <c r="AP7" s="16" t="s">
@@ -2015,7 +2015,7 @@
         <v>144</v>
       </c>
       <c r="AV7" s="17"/>
-      <c r="AW7" s="33" t="s">
+      <c r="AW7" s="30" t="s">
         <v>43</v>
       </c>
       <c r="AX7" s="16" t="s">
@@ -2025,7 +2025,7 @@
       <c r="AZ7" s="17"/>
     </row>
     <row r="8" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -2037,7 +2037,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="30" t="s">
         <v>38</v>
       </c>
       <c r="J8" s="16" t="s">
@@ -2047,7 +2047,7 @@
       <c r="L8" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="30" t="s">
         <v>58</v>
       </c>
       <c r="N8" s="16" t="s">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="W8" s="16"/>
       <c r="X8" s="17"/>
-      <c r="Y8" s="35" t="s">
+      <c r="Y8" s="32" t="s">
         <v>1</v>
       </c>
       <c r="Z8" s="16" t="s">
@@ -2079,7 +2079,7 @@
       <c r="AB8" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="AC8" s="33" t="s">
+      <c r="AC8" s="30" t="s">
         <v>44</v>
       </c>
       <c r="AD8" s="20" t="s">
@@ -2095,7 +2095,7 @@
       </c>
       <c r="AI8" s="16"/>
       <c r="AJ8" s="17"/>
-      <c r="AK8" s="33" t="s">
+      <c r="AK8" s="30" t="s">
         <v>23</v>
       </c>
       <c r="AL8" s="16" t="s">
@@ -2105,7 +2105,7 @@
       <c r="AN8" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="AO8" s="33" t="s">
+      <c r="AO8" s="30" t="s">
         <v>165</v>
       </c>
       <c r="AP8" s="16" t="s">
@@ -2123,7 +2123,7 @@
       <c r="AV8" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="AW8" s="33" t="s">
+      <c r="AW8" s="30" t="s">
         <v>44</v>
       </c>
       <c r="AX8" s="16" t="s">
@@ -2133,7 +2133,7 @@
       <c r="AZ8" s="17"/>
     </row>
     <row r="9" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -2145,7 +2145,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="30" t="s">
         <v>39</v>
       </c>
       <c r="J9" s="16" t="s">
@@ -2155,7 +2155,7 @@
       <c r="L9" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="30" t="s">
         <v>139</v>
       </c>
       <c r="N9" s="16" t="s">
@@ -2177,7 +2177,7 @@
       </c>
       <c r="W9" s="16"/>
       <c r="X9" s="17"/>
-      <c r="Y9" s="35" t="s">
+      <c r="Y9" s="32" t="s">
         <v>23</v>
       </c>
       <c r="Z9" s="16" t="s">
@@ -2187,7 +2187,7 @@
       <c r="AB9" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="AC9" s="33" t="s">
+      <c r="AC9" s="30" t="s">
         <v>137</v>
       </c>
       <c r="AD9" s="20" t="s">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="AI9" s="16"/>
       <c r="AJ9" s="17"/>
-      <c r="AK9" s="33" t="s">
+      <c r="AK9" s="30" t="s">
         <v>24</v>
       </c>
       <c r="AL9" s="16" t="s">
@@ -2213,7 +2213,7 @@
       <c r="AN9" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="AO9" s="33" t="s">
+      <c r="AO9" s="30" t="s">
         <v>166</v>
       </c>
       <c r="AP9" s="16" t="s">
@@ -2225,7 +2225,7 @@
       <c r="AT9" s="16"/>
       <c r="AU9" s="16"/>
       <c r="AV9" s="17"/>
-      <c r="AW9" s="33" t="s">
+      <c r="AW9" s="30" t="s">
         <v>137</v>
       </c>
       <c r="AX9" s="16" t="s">
@@ -2235,7 +2235,7 @@
       <c r="AZ9" s="17"/>
     </row>
     <row r="10" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -2247,7 +2247,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="30" t="s">
         <v>40</v>
       </c>
       <c r="J10" s="16" t="s">
@@ -2257,7 +2257,7 @@
       <c r="L10" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M10" s="30" t="s">
         <v>140</v>
       </c>
       <c r="N10" s="16" t="s">
@@ -2275,7 +2275,7 @@
       <c r="V10" s="16"/>
       <c r="W10" s="16"/>
       <c r="X10" s="17"/>
-      <c r="Y10" s="35" t="s">
+      <c r="Y10" s="32" t="s">
         <v>24</v>
       </c>
       <c r="Z10" s="16" t="s">
@@ -2285,7 +2285,7 @@
       <c r="AB10" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AC10" s="33" t="s">
+      <c r="AC10" s="30" t="s">
         <v>26</v>
       </c>
       <c r="AD10" s="16" t="s">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="AI10" s="16"/>
       <c r="AJ10" s="17"/>
-      <c r="AK10" s="33" t="s">
+      <c r="AK10" s="30" t="s">
         <v>6</v>
       </c>
       <c r="AL10" s="16" t="s">
@@ -2313,7 +2313,7 @@
       <c r="AN10" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="AO10" s="33" t="s">
+      <c r="AO10" s="30" t="s">
         <v>167</v>
       </c>
       <c r="AP10" s="16" t="s">
@@ -2325,7 +2325,7 @@
       <c r="AT10" s="16"/>
       <c r="AU10" s="16"/>
       <c r="AV10" s="17"/>
-      <c r="AW10" s="33" t="s">
+      <c r="AW10" s="30" t="s">
         <v>171</v>
       </c>
       <c r="AX10" s="16" t="s">
@@ -2335,7 +2335,7 @@
       <c r="AZ10" s="17"/>
     </row>
     <row r="11" spans="1:52" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -2351,7 +2351,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="34" t="s">
+      <c r="M11" s="31" t="s">
         <v>148</v>
       </c>
       <c r="N11" s="16" t="s">
@@ -2367,7 +2367,7 @@
       <c r="V11" s="16"/>
       <c r="W11" s="16"/>
       <c r="X11" s="17"/>
-      <c r="Y11" s="35" t="s">
+      <c r="Y11" s="32" t="s">
         <v>6</v>
       </c>
       <c r="Z11" s="16" t="s">
@@ -2377,7 +2377,7 @@
       <c r="AB11" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AC11" s="33" t="s">
+      <c r="AC11" s="30" t="s">
         <v>165</v>
       </c>
       <c r="AD11" s="16" t="s">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="AI11" s="16"/>
       <c r="AJ11" s="17"/>
-      <c r="AK11" s="35" t="s">
+      <c r="AK11" s="32" t="s">
         <v>142</v>
       </c>
       <c r="AL11" s="16" t="s">
@@ -2403,7 +2403,7 @@
       <c r="AN11" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="AO11" s="33" t="s">
+      <c r="AO11" s="30" t="s">
         <v>168</v>
       </c>
       <c r="AP11" s="16" t="s">
@@ -2415,7 +2415,7 @@
       <c r="AT11" s="16"/>
       <c r="AU11" s="16"/>
       <c r="AV11" s="17"/>
-      <c r="AW11" s="33" t="s">
+      <c r="AW11" s="30" t="s">
         <v>145</v>
       </c>
       <c r="AX11" s="16" t="s">
@@ -2439,7 +2439,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="34" t="s">
+      <c r="M12" s="31" t="s">
         <v>149</v>
       </c>
       <c r="N12" s="16" t="s">
@@ -2455,7 +2455,7 @@
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
       <c r="X12" s="17"/>
-      <c r="Y12" s="35" t="s">
+      <c r="Y12" s="32" t="s">
         <v>11</v>
       </c>
       <c r="Z12" s="16" t="s">
@@ -2467,7 +2467,7 @@
       <c r="AB12" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="AC12" s="33" t="s">
+      <c r="AC12" s="30" t="s">
         <v>166</v>
       </c>
       <c r="AD12" s="16" t="s">
@@ -2479,7 +2479,7 @@
       <c r="AH12" s="23"/>
       <c r="AI12" s="16"/>
       <c r="AJ12" s="17"/>
-      <c r="AK12" s="35" t="s">
+      <c r="AK12" s="32" t="s">
         <v>143</v>
       </c>
       <c r="AL12" s="16" t="s">
@@ -2515,7 +2515,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="17"/>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="30" t="s">
         <v>150</v>
       </c>
       <c r="N13" s="16" t="s">
@@ -2531,7 +2531,7 @@
       <c r="V13" s="16"/>
       <c r="W13" s="16"/>
       <c r="X13" s="17"/>
-      <c r="Y13" s="35" t="s">
+      <c r="Y13" s="32" t="s">
         <v>142</v>
       </c>
       <c r="Z13" s="16" t="s">
@@ -2541,7 +2541,7 @@
       <c r="AB13" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="AC13" s="33" t="s">
+      <c r="AC13" s="30" t="s">
         <v>170</v>
       </c>
       <c r="AD13" s="20" t="s">
@@ -2553,7 +2553,7 @@
       <c r="AH13" s="23"/>
       <c r="AI13" s="16"/>
       <c r="AJ13" s="17"/>
-      <c r="AK13" s="35" t="s">
+      <c r="AK13" s="32" t="s">
         <v>149</v>
       </c>
       <c r="AL13" s="16" t="s">
@@ -2589,7 +2589,7 @@
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="17"/>
-      <c r="M14" s="33" t="s">
+      <c r="M14" s="30" t="s">
         <v>151</v>
       </c>
       <c r="N14" s="16" t="s">
@@ -2605,7 +2605,7 @@
       <c r="V14" s="16"/>
       <c r="W14" s="16"/>
       <c r="X14" s="17"/>
-      <c r="Y14" s="35" t="s">
+      <c r="Y14" s="32" t="s">
         <v>143</v>
       </c>
       <c r="Z14" s="16" t="s">
@@ -2623,7 +2623,7 @@
       <c r="AH14" s="23"/>
       <c r="AI14" s="16"/>
       <c r="AJ14" s="17"/>
-      <c r="AK14" s="35" t="s">
+      <c r="AK14" s="32" t="s">
         <v>140</v>
       </c>
       <c r="AL14" s="16" t="s">
@@ -2659,7 +2659,7 @@
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="17"/>
-      <c r="M15" s="33" t="s">
+      <c r="M15" s="30" t="s">
         <v>152</v>
       </c>
       <c r="N15" s="16" t="s">
@@ -2675,7 +2675,7 @@
       <c r="V15" s="16"/>
       <c r="W15" s="16"/>
       <c r="X15" s="17"/>
-      <c r="Y15" s="35" t="s">
+      <c r="Y15" s="32" t="s">
         <v>149</v>
       </c>
       <c r="Z15" s="16" t="s">
@@ -2693,7 +2693,7 @@
       <c r="AH15" s="23"/>
       <c r="AI15" s="16"/>
       <c r="AJ15" s="17"/>
-      <c r="AK15" s="35" t="s">
+      <c r="AK15" s="32" t="s">
         <v>22</v>
       </c>
       <c r="AL15" s="16" t="s">
@@ -2739,7 +2739,7 @@
       <c r="V16" s="16"/>
       <c r="W16" s="16"/>
       <c r="X16" s="17"/>
-      <c r="Y16" s="35" t="s">
+      <c r="Y16" s="32" t="s">
         <v>140</v>
       </c>
       <c r="Z16" s="16" t="s">
@@ -2755,7 +2755,7 @@
       <c r="AH16" s="23"/>
       <c r="AI16" s="16"/>
       <c r="AJ16" s="17"/>
-      <c r="AK16" s="36" t="s">
+      <c r="AK16" s="33" t="s">
         <v>25</v>
       </c>
       <c r="AL16" s="20" t="s">
@@ -2801,7 +2801,7 @@
       <c r="V17" s="16"/>
       <c r="W17" s="16"/>
       <c r="X17" s="17"/>
-      <c r="Y17" s="35" t="s">
+      <c r="Y17" s="32" t="s">
         <v>22</v>
       </c>
       <c r="Z17" s="16" t="s">
@@ -2819,7 +2819,7 @@
       <c r="AH17" s="23"/>
       <c r="AI17" s="16"/>
       <c r="AJ17" s="17"/>
-      <c r="AK17" s="36" t="s">
+      <c r="AK17" s="33" t="s">
         <v>26</v>
       </c>
       <c r="AL17" s="20" t="s">
@@ -2867,7 +2867,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
       <c r="X18" s="17"/>
-      <c r="Y18" s="36" t="s">
+      <c r="Y18" s="33" t="s">
         <v>25</v>
       </c>
       <c r="Z18" s="20" t="s">
@@ -2883,7 +2883,7 @@
       <c r="AH18" s="23"/>
       <c r="AI18" s="16"/>
       <c r="AJ18" s="17"/>
-      <c r="AK18" s="36" t="s">
+      <c r="AK18" s="33" t="s">
         <v>165</v>
       </c>
       <c r="AL18" s="20" t="s">
@@ -2929,7 +2929,7 @@
       <c r="V19" s="16"/>
       <c r="W19" s="16"/>
       <c r="X19" s="17"/>
-      <c r="Y19" s="36" t="s">
+      <c r="Y19" s="33" t="s">
         <v>26</v>
       </c>
       <c r="Z19" s="20" t="s">
@@ -2947,7 +2947,7 @@
       <c r="AH19" s="23"/>
       <c r="AI19" s="16"/>
       <c r="AJ19" s="17"/>
-      <c r="AK19" s="36" t="s">
+      <c r="AK19" s="33" t="s">
         <v>166</v>
       </c>
       <c r="AL19" s="20" t="s">
@@ -2993,7 +2993,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="17"/>
-      <c r="Y20" s="36" t="s">
+      <c r="Y20" s="33" t="s">
         <v>165</v>
       </c>
       <c r="Z20" s="20" t="s">
@@ -3051,7 +3051,7 @@
       <c r="V21" s="16"/>
       <c r="W21" s="16"/>
       <c r="X21" s="17"/>
-      <c r="Y21" s="36" t="s">
+      <c r="Y21" s="33" t="s">
         <v>166</v>
       </c>
       <c r="Z21" s="20" t="s">
@@ -3085,240 +3085,240 @@
       <c r="AZ21" s="17"/>
     </row>
     <row r="22" spans="1:52" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="27" t="s">
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="27" t="s">
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="27" t="s">
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="27" t="s">
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="27" t="s">
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="29"/>
-      <c r="Y22" s="27" t="s">
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="29"/>
-      <c r="AC22" s="27" t="s">
+      <c r="Z22" s="35"/>
+      <c r="AA22" s="35"/>
+      <c r="AB22" s="36"/>
+      <c r="AC22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="29"/>
-      <c r="AG22" s="27" t="s">
+      <c r="AD22" s="35"/>
+      <c r="AE22" s="35"/>
+      <c r="AF22" s="36"/>
+      <c r="AG22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AH22" s="28"/>
-      <c r="AI22" s="28"/>
-      <c r="AJ22" s="29"/>
-      <c r="AK22" s="27" t="s">
+      <c r="AH22" s="35"/>
+      <c r="AI22" s="35"/>
+      <c r="AJ22" s="36"/>
+      <c r="AK22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AL22" s="28"/>
-      <c r="AM22" s="28"/>
-      <c r="AN22" s="29"/>
-      <c r="AO22" s="27" t="s">
+      <c r="AL22" s="35"/>
+      <c r="AM22" s="35"/>
+      <c r="AN22" s="36"/>
+      <c r="AO22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AP22" s="28"/>
-      <c r="AQ22" s="28"/>
-      <c r="AR22" s="29"/>
-      <c r="AS22" s="27" t="s">
+      <c r="AP22" s="35"/>
+      <c r="AQ22" s="35"/>
+      <c r="AR22" s="36"/>
+      <c r="AS22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AT22" s="28"/>
-      <c r="AU22" s="28"/>
-      <c r="AV22" s="29"/>
-      <c r="AW22" s="27" t="s">
+      <c r="AT22" s="35"/>
+      <c r="AU22" s="35"/>
+      <c r="AV22" s="36"/>
+      <c r="AW22" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AX22" s="28"/>
-      <c r="AY22" s="28"/>
-      <c r="AZ22" s="29"/>
+      <c r="AX22" s="35"/>
+      <c r="AY22" s="35"/>
+      <c r="AZ22" s="36"/>
     </row>
     <row r="23" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="J23" s="31" t="s">
+      <c r="J23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="K23" s="31" t="s">
+      <c r="K23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="L23" s="31" t="s">
+      <c r="L23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="M23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="N23" s="31" t="s">
+      <c r="N23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="O23" s="31" t="s">
+      <c r="O23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="P23" s="31" t="s">
+      <c r="P23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="Q23" s="30" t="s">
+      <c r="Q23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="R23" s="31" t="s">
+      <c r="R23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="S23" s="31" t="s">
+      <c r="S23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="T23" s="31" t="s">
+      <c r="T23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="U23" s="30" t="s">
+      <c r="U23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="V23" s="31" t="s">
+      <c r="V23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="W23" s="31" t="s">
+      <c r="W23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="X23" s="32" t="s">
+      <c r="X23" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="Y23" s="31" t="s">
+      <c r="Y23" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="Z23" s="31" t="s">
+      <c r="Z23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AA23" s="31" t="s">
+      <c r="AA23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AB23" s="31" t="s">
+      <c r="AB23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="AC23" s="30" t="s">
+      <c r="AC23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="AD23" s="31" t="s">
+      <c r="AD23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AE23" s="31" t="s">
+      <c r="AE23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AF23" s="31" t="s">
+      <c r="AF23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="AG23" s="30" t="s">
+      <c r="AG23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="AH23" s="31" t="s">
+      <c r="AH23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AI23" s="31" t="s">
+      <c r="AI23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AJ23" s="31" t="s">
+      <c r="AJ23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="AK23" s="30" t="s">
+      <c r="AK23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="AL23" s="31" t="s">
+      <c r="AL23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AM23" s="31" t="s">
+      <c r="AM23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AN23" s="31" t="s">
+      <c r="AN23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="AO23" s="30" t="s">
+      <c r="AO23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="AP23" s="31" t="s">
+      <c r="AP23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AQ23" s="31" t="s">
+      <c r="AQ23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AR23" s="31" t="s">
+      <c r="AR23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="AS23" s="30" t="s">
+      <c r="AS23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="AT23" s="31" t="s">
+      <c r="AT23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AU23" s="31" t="s">
+      <c r="AU23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AV23" s="31" t="s">
+      <c r="AV23" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="AW23" s="30" t="s">
+      <c r="AW23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="AX23" s="31" t="s">
+      <c r="AX23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AY23" s="31" t="s">
+      <c r="AY23" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AZ23" s="32" t="s">
+      <c r="AZ23" s="29" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADD] model abasy annotation
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BiSBII\OneDrive - Universidade do Minho\PhD\Protrend\main\protrend-database\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="13_ncr:1_{15E36B38-B12C-4BC5-84DF-7B470AA1660C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28E36497-B059-4813-B632-153007312D10}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D752E79-F96D-4DF4-B163-B2D5D1E09FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -747,15 +747,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -774,6 +765,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1090,9 +1091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:AZ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AW2" sqref="AW2:AW11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,10 +1150,10 @@
     <col min="50" max="50" width="11.109375" style="2" customWidth="1"/>
     <col min="51" max="51" width="12.109375" style="2" customWidth="1"/>
     <col min="52" max="52" width="11.44140625" style="3" customWidth="1"/>
-    <col min="53" max="16384" width="8.88671875" style="24"/>
+    <col min="53" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="23" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:52" s="20" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -2403,84 +2404,84 @@
       <c r="AB21" s="8"/>
     </row>
     <row r="22" spans="1:52" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="20" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="20" t="s">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="20" t="s">
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="20" t="s">
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="20" t="s">
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="22"/>
-      <c r="Y22" s="20" t="s">
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="28"/>
+      <c r="Y22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="22"/>
-      <c r="AC22" s="20" t="s">
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="28"/>
+      <c r="AC22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="22"/>
-      <c r="AG22" s="20" t="s">
+      <c r="AD22" s="27"/>
+      <c r="AE22" s="27"/>
+      <c r="AF22" s="28"/>
+      <c r="AG22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AH22" s="21"/>
-      <c r="AI22" s="21"/>
-      <c r="AJ22" s="22"/>
-      <c r="AK22" s="20" t="s">
+      <c r="AH22" s="27"/>
+      <c r="AI22" s="27"/>
+      <c r="AJ22" s="28"/>
+      <c r="AK22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AL22" s="21"/>
-      <c r="AM22" s="21"/>
-      <c r="AN22" s="22"/>
-      <c r="AO22" s="20" t="s">
+      <c r="AL22" s="27"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="28"/>
+      <c r="AO22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AP22" s="21"/>
-      <c r="AQ22" s="21"/>
-      <c r="AR22" s="22"/>
-      <c r="AS22" s="20" t="s">
+      <c r="AP22" s="27"/>
+      <c r="AQ22" s="27"/>
+      <c r="AR22" s="28"/>
+      <c r="AS22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AT22" s="21"/>
-      <c r="AU22" s="21"/>
-      <c r="AV22" s="22"/>
-      <c r="AW22" s="20" t="s">
+      <c r="AT22" s="27"/>
+      <c r="AU22" s="27"/>
+      <c r="AV22" s="28"/>
+      <c r="AW22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AX22" s="21"/>
-      <c r="AY22" s="21"/>
-      <c r="AZ22" s="22"/>
+      <c r="AX22" s="27"/>
+      <c r="AY22" s="27"/>
+      <c r="AZ22" s="28"/>
     </row>
     <row r="23" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -2641,7 +2642,7 @@
       </c>
     </row>
     <row r="24" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2668,7 +2669,7 @@
       <c r="K24" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M24" s="16" t="s">
         <v>18</v>
       </c>
       <c r="N24" s="2" t="s">
@@ -2704,7 +2705,7 @@
       <c r="X24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="Y24" s="1" t="s">
+      <c r="Y24" s="16" t="s">
         <v>18</v>
       </c>
       <c r="Z24" s="2" t="s">
@@ -2716,7 +2717,7 @@
       <c r="AB24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AC24" s="1" t="s">
+      <c r="AC24" s="16" t="s">
         <v>18</v>
       </c>
       <c r="AD24" s="2" t="s">
@@ -2740,7 +2741,7 @@
       <c r="AJ24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AK24" s="1" t="s">
+      <c r="AK24" s="16" t="s">
         <v>18</v>
       </c>
       <c r="AL24" s="2" t="s">
@@ -2776,7 +2777,7 @@
       <c r="AV24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AW24" s="1" t="s">
+      <c r="AW24" s="16" t="s">
         <v>18</v>
       </c>
       <c r="AX24" s="2" t="s">
@@ -2938,7 +2939,7 @@
       <c r="K26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="M26" s="16" t="s">
         <v>10</v>
       </c>
       <c r="N26" s="2" t="s">
@@ -3031,7 +3032,7 @@
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3058,7 +3059,7 @@
       <c r="K27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M27" s="16" t="s">
         <v>8</v>
       </c>
       <c r="N27" s="2" t="s">
@@ -3076,7 +3077,7 @@
       <c r="S27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Y27" s="2" t="s">
+      <c r="Y27" s="18" t="s">
         <v>0</v>
       </c>
       <c r="Z27" s="2" t="s">
@@ -3085,7 +3086,7 @@
       <c r="AA27" s="2">
         <v>1</v>
       </c>
-      <c r="AC27" s="2" t="s">
+      <c r="AC27" s="18" t="s">
         <v>0</v>
       </c>
       <c r="AD27" s="2" t="s">
@@ -3103,7 +3104,7 @@
       <c r="AI27" s="2">
         <v>1</v>
       </c>
-      <c r="AK27" s="2" t="s">
+      <c r="AK27" s="18" t="s">
         <v>0</v>
       </c>
       <c r="AL27" s="2" t="s">
@@ -3131,7 +3132,7 @@
       <c r="AU27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AW27" s="1" t="s">
+      <c r="AW27" s="16" t="s">
         <v>0</v>
       </c>
       <c r="AX27" s="2" t="s">
@@ -3142,7 +3143,7 @@
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3187,7 +3188,7 @@
       <c r="AA28" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="AC28" s="1" t="s">
+      <c r="AC28" s="16" t="s">
         <v>10</v>
       </c>
       <c r="AD28" s="6" t="s">
@@ -3236,7 +3237,7 @@
         <v>133</v>
       </c>
       <c r="AV28" s="8"/>
-      <c r="AW28" s="1" t="s">
+      <c r="AW28" s="16" t="s">
         <v>10</v>
       </c>
       <c r="AX28" s="2" t="s">
@@ -3275,7 +3276,7 @@
       <c r="K29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M29" s="16" t="s">
         <v>14</v>
       </c>
       <c r="N29" s="2" t="s">
@@ -3314,7 +3315,7 @@
       <c r="AJ29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AK29" s="5" t="s">
+      <c r="AK29" s="29" t="s">
         <v>10</v>
       </c>
       <c r="AL29" s="6" t="s">
@@ -3335,7 +3336,7 @@
       <c r="AQ29" s="2">
         <v>1</v>
       </c>
-      <c r="AW29" s="1" t="s">
+      <c r="AW29" s="16" t="s">
         <v>8</v>
       </c>
       <c r="AX29" s="2" t="s">
@@ -3347,7 +3348,7 @@
       <c r="AZ29" s="8"/>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3374,7 +3375,7 @@
       <c r="O30" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Y30" s="2" t="s">
+      <c r="Y30" s="18" t="s">
         <v>8</v>
       </c>
       <c r="Z30" s="2" t="s">
@@ -3383,7 +3384,7 @@
       <c r="AA30" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="AC30" s="2" t="s">
+      <c r="AC30" s="18" t="s">
         <v>14</v>
       </c>
       <c r="AD30" s="2" t="s">
@@ -3392,7 +3393,7 @@
       <c r="AE30" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AK30" s="1" t="s">
+      <c r="AK30" s="16" t="s">
         <v>8</v>
       </c>
       <c r="AL30" s="6" t="s">
@@ -3414,7 +3415,7 @@
       <c r="AR30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AW30" s="1" t="s">
+      <c r="AW30" s="16" t="s">
         <v>14</v>
       </c>
       <c r="AX30" s="2" t="s">
@@ -3455,7 +3456,7 @@
       <c r="O31" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Y31" s="2" t="s">
+      <c r="Y31" s="18" t="s">
         <v>14</v>
       </c>
       <c r="Z31" s="2" t="s">
@@ -3532,7 +3533,7 @@
       <c r="K32" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="M32" s="16" t="s">
         <v>16</v>
       </c>
       <c r="N32" s="2" t="s">
@@ -3553,7 +3554,7 @@
       <c r="AB32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AC32" s="2" t="s">
+      <c r="AC32" s="18" t="s">
         <v>16</v>
       </c>
       <c r="AD32" s="2" t="s">
@@ -3587,7 +3588,7 @@
       <c r="AZ32" s="8"/>
     </row>
     <row r="33" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3614,7 +3615,7 @@
       <c r="AA33" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="AK33" s="5" t="s">
+      <c r="AK33" s="29" t="s">
         <v>16</v>
       </c>
       <c r="AL33" s="6" t="s">
@@ -3628,7 +3629,7 @@
       </c>
     </row>
     <row r="34" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y34" s="2" t="s">
+      <c r="Y34" s="18" t="s">
         <v>16</v>
       </c>
       <c r="Z34" s="2" t="s">
@@ -3641,10 +3642,10 @@
     </row>
     <row r="36" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="37" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="23" t="s">
         <v>156</v>
       </c>
       <c r="AC37" s="2"/>
@@ -3679,10 +3680,10 @@
       </c>
     </row>
     <row r="41" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="25" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] fix minor issues associated with database loading
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -765,6 +765,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -774,7 +775,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,9 +1091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:AZ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AW32" activeCellId="1" sqref="AW28:AW30 AW32"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2404,84 +2404,84 @@
       <c r="AB21" s="8"/>
     </row>
     <row r="22" spans="1:52" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="26" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="26" t="s">
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="26" t="s">
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="26" t="s">
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="26" t="s">
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="V22" s="27"/>
-      <c r="W22" s="27"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="26" t="s">
+      <c r="V22" s="28"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="Z22" s="27"/>
-      <c r="AA22" s="27"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="26" t="s">
+      <c r="Z22" s="28"/>
+      <c r="AA22" s="28"/>
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AD22" s="27"/>
-      <c r="AE22" s="27"/>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="26" t="s">
+      <c r="AD22" s="28"/>
+      <c r="AE22" s="28"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AH22" s="27"/>
-      <c r="AI22" s="27"/>
-      <c r="AJ22" s="28"/>
-      <c r="AK22" s="26" t="s">
+      <c r="AH22" s="28"/>
+      <c r="AI22" s="28"/>
+      <c r="AJ22" s="29"/>
+      <c r="AK22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AL22" s="27"/>
-      <c r="AM22" s="27"/>
-      <c r="AN22" s="28"/>
-      <c r="AO22" s="26" t="s">
+      <c r="AL22" s="28"/>
+      <c r="AM22" s="28"/>
+      <c r="AN22" s="29"/>
+      <c r="AO22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AP22" s="27"/>
-      <c r="AQ22" s="27"/>
-      <c r="AR22" s="28"/>
-      <c r="AS22" s="26" t="s">
+      <c r="AP22" s="28"/>
+      <c r="AQ22" s="28"/>
+      <c r="AR22" s="29"/>
+      <c r="AS22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AT22" s="27"/>
-      <c r="AU22" s="27"/>
-      <c r="AV22" s="28"/>
-      <c r="AW22" s="26" t="s">
+      <c r="AT22" s="28"/>
+      <c r="AU22" s="28"/>
+      <c r="AV22" s="29"/>
+      <c r="AW22" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AX22" s="27"/>
-      <c r="AY22" s="27"/>
-      <c r="AZ22" s="28"/>
+      <c r="AX22" s="28"/>
+      <c r="AY22" s="28"/>
+      <c r="AZ22" s="29"/>
     </row>
     <row r="23" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -3227,7 +3227,7 @@
       <c r="AR28" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AS28" s="29" t="s">
+      <c r="AS28" s="26" t="s">
         <v>16</v>
       </c>
       <c r="AT28" s="6" t="s">
@@ -3315,7 +3315,7 @@
       <c r="AJ29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AK29" s="29" t="s">
+      <c r="AK29" s="26" t="s">
         <v>10</v>
       </c>
       <c r="AL29" s="6" t="s">
@@ -3615,7 +3615,7 @@
       <c r="AA33" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="AK33" s="29" t="s">
+      <c r="AK33" s="26" t="s">
         <v>16</v>
       </c>
       <c r="AL33" s="6" t="s">

</xml_diff>

<commit_message>
[ADD] abasy connections using the create connection method
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="258" documentId="13_ncr:1_{0D752E79-F96D-4DF4-B163-B2D5D1E09FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A95CF64D-9FA5-4E1F-9037-C611EC4795F4}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -1043,9 +1043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89572100-23F8-4530-8FD2-7BD168F0C2AB}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA27" sqref="AA27"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS27" sqref="AS27:AS29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[UPDATE] model annotation update
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="13_ncr:1_{0D752E79-F96D-4DF4-B163-B2D5D1E09FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A95CF64D-9FA5-4E1F-9037-C611EC4795F4}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="13_ncr:1_{0D752E79-F96D-4DF4-B163-B2D5D1E09FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{198C16AA-309F-4D85-ACDC-6432D3ED35CC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="157">
   <si>
     <t>Organism</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>regulator</t>
-  </si>
-  <si>
-    <t>operon</t>
   </si>
   <si>
     <t>genes</t>
@@ -653,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -727,6 +724,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,8 +1042,8 @@
   <dimension ref="A1:AV41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS27" sqref="AS27:AS29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,15 +1056,15 @@
     <col min="6" max="6" width="10.109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.88671875" style="2" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" style="2" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.44140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.77734375" style="2" customWidth="1"/>
     <col min="15" max="15" width="12" style="2" customWidth="1"/>
     <col min="16" max="16" width="12.44140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.21875" style="1" customWidth="1"/>
     <col min="18" max="18" width="10.109375" style="2" customWidth="1"/>
     <col min="19" max="19" width="12.6640625" style="2" customWidth="1"/>
     <col min="20" max="20" width="17.109375" style="2" customWidth="1"/>
@@ -1086,7 +1084,7 @@
     <col min="34" max="34" width="9.6640625" style="9" customWidth="1"/>
     <col min="35" max="35" width="12.6640625" style="9" customWidth="1"/>
     <col min="36" max="36" width="11.77734375" style="7" customWidth="1"/>
-    <col min="37" max="37" width="11.5546875" style="1" customWidth="1"/>
+    <col min="37" max="37" width="18.109375" style="1" customWidth="1"/>
     <col min="38" max="38" width="11.77734375" style="2" customWidth="1"/>
     <col min="39" max="39" width="12.44140625" style="2" customWidth="1"/>
     <col min="40" max="40" width="11.21875" style="3" customWidth="1"/>
@@ -1103,488 +1101,488 @@
   <sheetData>
     <row r="1" spans="1:48" s="16" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>33</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>34</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="Q1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="T1" s="10" t="s">
         <v>29</v>
       </c>
       <c r="U1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="X1" s="11" t="s">
         <v>32</v>
       </c>
       <c r="Y1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="AB1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="AC1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="AF1" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AG1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="AI1" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="AJ1" s="11" t="s">
         <v>27</v>
       </c>
       <c r="AK1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AM1" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="AM1" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="AN1" s="11" t="s">
         <v>28</v>
       </c>
       <c r="AO1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AP1" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AQ1" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AR1" s="11" t="s">
         <v>30</v>
       </c>
       <c r="AS1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="AT1" s="10" t="s">
+      <c r="AU1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="AU1" s="10" t="s">
+      <c r="AV1" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="AV1" s="11" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="N2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="R2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="V2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="Z2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AD2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AH2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AO2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AP2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AT2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AT3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AT4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AP5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AT5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.3">
@@ -1592,107 +1590,110 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>4</v>
+        <v>149</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="M6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y6" s="23" t="s">
         <v>19</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AC6" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AD6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AG6" s="22" t="s">
         <v>19</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AK6" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN6" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN6" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="AO6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AR6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AS6" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AT6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="115.2" x14ac:dyDescent="0.3">
@@ -1700,107 +1701,104 @@
         <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>35</v>
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y7" s="23" t="s">
         <v>21</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG7" s="23" t="s">
         <v>21</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AL7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AO7" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="AR7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AS7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AT7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
@@ -1808,68 +1806,68 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AC8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AD8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AK8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AN8" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AS8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AT8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV8" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
@@ -1877,25 +1875,25 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y9" s="2" t="s">
         <v>22</v>
@@ -1904,16 +1902,16 @@
         <v>7</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AD9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AG9" s="1" t="s">
         <v>22</v>
@@ -1923,28 +1921,28 @@
       </c>
       <c r="AI9" s="2"/>
       <c r="AJ9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AK9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AM9" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AN9" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AS9" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AT9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV9" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:48" ht="72" x14ac:dyDescent="0.3">
@@ -1955,62 +1953,62 @@
         <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AC10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AK10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AN10" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AS10" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AT10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
@@ -2018,13 +2016,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="8"/>
@@ -2032,41 +2030,41 @@
         <v>23</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AS11" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AT11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:48" ht="57.6" x14ac:dyDescent="0.3">
@@ -2075,10 +2073,10 @@
       <c r="C12" s="6"/>
       <c r="D12" s="8"/>
       <c r="M12" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="8"/>
@@ -2086,47 +2084,47 @@
         <v>6</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AS12" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AT12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AV12" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
@@ -2135,98 +2133,98 @@
       <c r="C13" s="6"/>
       <c r="D13" s="8"/>
       <c r="M13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG13" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="Z13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG13" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="AH13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="M14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AD14" s="6"/>
       <c r="AG14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AH14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M15" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AG15" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AH15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Y16" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AH16" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="3"/>
@@ -2236,7 +2234,7 @@
         <v>24</v>
       </c>
       <c r="Z17" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA17" s="6"/>
       <c r="AB17" s="8"/>
@@ -2244,10 +2242,10 @@
         <v>25</v>
       </c>
       <c r="AH17" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI17" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AJ17" s="3"/>
     </row>
@@ -2256,45 +2254,45 @@
         <v>25</v>
       </c>
       <c r="Z18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA18" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB18" s="8"/>
       <c r="AG18" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AH18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI18" s="6"/>
       <c r="AJ18" s="3"/>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="Y19" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA19" s="6"/>
       <c r="AB19" s="8"/>
       <c r="AG19" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AH19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="3"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="Y20" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Z20" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA20" s="6"/>
       <c r="AB20" s="8"/>
@@ -2302,73 +2300,73 @@
     <row r="21" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:48" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
       <c r="E22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
       <c r="I22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
       <c r="L22" s="26"/>
       <c r="M22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="26"/>
       <c r="Q22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
       <c r="T22" s="26"/>
       <c r="U22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V22" s="25"/>
       <c r="W22" s="25"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z22" s="25"/>
       <c r="AA22" s="25"/>
       <c r="AB22" s="26"/>
       <c r="AC22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AD22" s="25"/>
       <c r="AE22" s="25"/>
       <c r="AF22" s="26"/>
       <c r="AG22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AH22" s="25"/>
       <c r="AI22" s="25"/>
       <c r="AJ22" s="26"/>
       <c r="AK22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AL22" s="25"/>
       <c r="AM22" s="25"/>
       <c r="AN22" s="26"/>
       <c r="AO22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AP22" s="25"/>
       <c r="AQ22" s="25"/>
       <c r="AR22" s="26"/>
       <c r="AS22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AT22" s="25"/>
       <c r="AU22" s="25"/>
@@ -2376,687 +2374,687 @@
     </row>
     <row r="23" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="C23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="D23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="G23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="H23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="K23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="K23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="L23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="N23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="N23" s="14" t="s">
+      <c r="O23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="O23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="P23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="R23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="R23" s="14" t="s">
+      <c r="S23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="S23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="T23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="V23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="V23" s="14" t="s">
+      <c r="W23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="W23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="X23" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y23" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="Z23" s="14" t="s">
+      <c r="AA23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AA23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="AB23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AD23" s="14" t="s">
+      <c r="AE23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AE23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="AF23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AG23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AH23" s="14" t="s">
+      <c r="AI23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AI23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="AJ23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AK23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AL23" s="14" t="s">
+      <c r="AM23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AM23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="AN23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AO23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AP23" s="14" t="s">
+      <c r="AQ23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AQ23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="AR23" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AS23" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT23" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AT23" s="14" t="s">
+      <c r="AU23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AU23" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="AV23" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>31</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="U24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AB24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE24" s="2">
         <v>1</v>
       </c>
       <c r="AF24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AG24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="AH24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AJ24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="AL24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AM24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AN24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AO24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="AP24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AQ24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AR24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AS24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="AT24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AV24" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="13" t="s">
         <v>9</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M25" s="13" t="s">
         <v>9</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q25" s="13" t="s">
         <v>9</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="U25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="U25" s="13" t="s">
         <v>18</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y25" s="1" t="s">
-        <v>99</v>
+        <v>119</v>
+      </c>
+      <c r="Y25" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>99</v>
+        <v>119</v>
+      </c>
+      <c r="AC25" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="AD25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE25" s="2">
         <v>1</v>
       </c>
-      <c r="AG25" s="1" t="s">
-        <v>99</v>
+      <c r="AG25" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="AH25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AJ25" s="3"/>
-      <c r="AK25" s="1" t="s">
-        <v>99</v>
+      <c r="AK25" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="AL25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AM25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO25" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AP25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AQ25" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS25" s="1" t="s">
-        <v>99</v>
+        <v>119</v>
+      </c>
+      <c r="AS25" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="AT25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26" s="13" t="s">
         <v>8</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M26" s="13" t="s">
         <v>8</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q26" s="13" t="s">
         <v>13</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="U26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="U26" s="13" t="s">
         <v>9</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="AH26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AJ26" s="3"/>
-      <c r="AK26" s="1" t="s">
+      <c r="AK26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="AL26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AM26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO26" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO26" s="27" t="s">
         <v>15</v>
       </c>
       <c r="AP26" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AQ26" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AR26" s="8"/>
-      <c r="AS26" s="1" t="s">
+      <c r="AS26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="AT26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M27" s="13" t="s">
         <v>13</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y27" s="14" t="s">
         <v>0</v>
       </c>
       <c r="Z27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA27" s="2">
         <v>1</v>
       </c>
-      <c r="AC27" s="2" t="s">
+      <c r="AC27" s="14" t="s">
         <v>0</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE27" s="2">
         <v>1</v>
       </c>
-      <c r="AG27" s="2" t="s">
+      <c r="AG27" s="14" t="s">
         <v>0</v>
       </c>
       <c r="AH27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI27" s="2">
         <v>1</v>
       </c>
       <c r="AJ27" s="3"/>
-      <c r="AK27" s="2" t="s">
+      <c r="AK27" s="14" t="s">
         <v>0</v>
       </c>
       <c r="AL27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AM27" s="2">
         <v>1</v>
       </c>
-      <c r="AS27" s="1" t="s">
+      <c r="AS27" s="13" t="s">
         <v>0</v>
       </c>
       <c r="AT27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU27" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I28" s="13" t="s">
         <v>12</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M28" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y28" s="14" t="s">
         <v>16</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC28" s="14" t="s">
         <v>13</v>
       </c>
       <c r="AD28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG28" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG28" s="27" t="s">
         <v>16</v>
       </c>
       <c r="AH28" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI28" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK28" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AL28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AM28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS28" s="13" t="s">
         <v>9</v>
       </c>
       <c r="AT28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU28" s="2">
         <v>1</v>
@@ -3064,69 +3062,69 @@
       <c r="AV28" s="8"/>
     </row>
     <row r="29" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I29" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M29" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M29" s="13" t="s">
         <v>15</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y29" s="14" t="s">
         <v>31</v>
       </c>
       <c r="Z29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA29" s="2">
         <v>1</v>
       </c>
       <c r="AD29" s="6"/>
-      <c r="AG29" s="5" t="s">
+      <c r="AG29" s="27" t="s">
         <v>9</v>
       </c>
       <c r="AH29" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI29" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK29" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK29" s="13" t="s">
         <v>13</v>
       </c>
       <c r="AL29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AM29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS29" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS29" s="13" t="s">
         <v>13</v>
       </c>
       <c r="AT29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU29" s="2">
         <v>1</v>
@@ -3134,52 +3132,52 @@
       <c r="AV29" s="8"/>
     </row>
     <row r="30" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y30" s="14" t="s">
         <v>13</v>
       </c>
       <c r="Z30" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA30" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG30" s="13" t="s">
         <v>8</v>
       </c>
       <c r="AH30" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI30" s="2">
         <v>1</v>
       </c>
       <c r="AJ30" s="3"/>
-      <c r="AK30" s="5" t="s">
+      <c r="AK30" s="27" t="s">
         <v>15</v>
       </c>
       <c r="AL30" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AM30" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AN30" s="8"/>
-      <c r="AS30" s="1" t="s">
+      <c r="AS30" s="13" t="s">
         <v>12</v>
       </c>
       <c r="AT30" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU30" s="2">
         <v>1</v>
@@ -3187,43 +3185,43 @@
       <c r="AV30" s="8"/>
     </row>
     <row r="31" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y31" s="14" t="s">
         <v>12</v>
       </c>
       <c r="Z31" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA31" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
-      <c r="AG31" s="5" t="s">
+      <c r="AG31" s="27" t="s">
         <v>12</v>
       </c>
       <c r="AH31" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI31" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS31" s="13" t="s">
         <v>14</v>
       </c>
       <c r="AT31" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU31" s="2">
         <v>1</v>
@@ -3231,62 +3229,60 @@
       <c r="AV31" s="8"/>
     </row>
     <row r="32" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y32" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y32" s="14" t="s">
         <v>14</v>
       </c>
       <c r="Z32" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
       <c r="AF32" s="8"/>
-      <c r="AG32" s="5" t="s">
+      <c r="AG32" s="27" t="s">
         <v>15</v>
       </c>
       <c r="AH32" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AI32" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ32" s="8" t="s">
-        <v>41</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="AJ32" s="8"/>
     </row>
     <row r="33" spans="2:37" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="Y33" s="2" t="s">
+      <c r="Y33" s="14" t="s">
         <v>15</v>
       </c>
       <c r="Z33" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA33" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AB33" s="8"/>
     </row>
     <row r="36" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="37" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>136</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>137</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AG37" s="2"/>
@@ -3294,37 +3290,37 @@
     </row>
     <row r="38" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="AK38" s="5"/>
     </row>
     <row r="39" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="AG39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
     <row r="40" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] changing gene-operon cardinality from one to zero or more
</commit_message>
<xml_diff>
--- a/annotation/model.xlsx
+++ b/annotation/model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/PhD/Protrend/main/protrend-database/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="13_ncr:1_{0D752E79-F96D-4DF4-B163-B2D5D1E09FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{198C16AA-309F-4D85-ACDC-6432D3ED35CC}"/>
+  <xr:revisionPtr revIDLastSave="348" documentId="13_ncr:1_{0D752E79-F96D-4DF4-B163-B2D5D1E09FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16F99A5E-0F3D-4FE1-AFE6-6B28A57364D7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0A134B7-604B-4CDA-82AD-3C97C1467F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="157">
   <si>
     <t>Organism</t>
   </si>
@@ -715,6 +715,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -724,7 +725,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1043,7 +1043,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="AI30" sqref="AI30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2299,78 +2299,78 @@
     </row>
     <row r="21" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:48" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="24" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="24" t="s">
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="24" t="s">
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="24" t="s">
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="24" t="s">
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="V22" s="25"/>
-      <c r="W22" s="25"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="24" t="s">
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="Z22" s="25"/>
-      <c r="AA22" s="25"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="24" t="s">
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="27"/>
+      <c r="AC22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="AD22" s="25"/>
-      <c r="AE22" s="25"/>
-      <c r="AF22" s="26"/>
-      <c r="AG22" s="24" t="s">
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="26"/>
+      <c r="AF22" s="27"/>
+      <c r="AG22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="AH22" s="25"/>
-      <c r="AI22" s="25"/>
-      <c r="AJ22" s="26"/>
-      <c r="AK22" s="24" t="s">
+      <c r="AH22" s="26"/>
+      <c r="AI22" s="26"/>
+      <c r="AJ22" s="27"/>
+      <c r="AK22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="AL22" s="25"/>
-      <c r="AM22" s="25"/>
-      <c r="AN22" s="26"/>
-      <c r="AO22" s="24" t="s">
+      <c r="AL22" s="26"/>
+      <c r="AM22" s="26"/>
+      <c r="AN22" s="27"/>
+      <c r="AO22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="AP22" s="25"/>
-      <c r="AQ22" s="25"/>
-      <c r="AR22" s="26"/>
-      <c r="AS22" s="24" t="s">
+      <c r="AP22" s="26"/>
+      <c r="AQ22" s="26"/>
+      <c r="AR22" s="27"/>
+      <c r="AS22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="AT22" s="25"/>
-      <c r="AU22" s="25"/>
-      <c r="AV22" s="26"/>
+      <c r="AT22" s="26"/>
+      <c r="AU22" s="26"/>
+      <c r="AV22" s="27"/>
     </row>
     <row r="23" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -2867,7 +2867,7 @@
       <c r="AM26" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AO26" s="27" t="s">
+      <c r="AO26" s="24" t="s">
         <v>15</v>
       </c>
       <c r="AP26" s="6" t="s">
@@ -3032,7 +3032,7 @@
       <c r="AE28" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AG28" s="27" t="s">
+      <c r="AG28" s="24" t="s">
         <v>16</v>
       </c>
       <c r="AH28" s="6" t="s">
@@ -3102,7 +3102,7 @@
         <v>1</v>
       </c>
       <c r="AD29" s="6"/>
-      <c r="AG29" s="27" t="s">
+      <c r="AG29" s="24" t="s">
         <v>9</v>
       </c>
       <c r="AH29" s="6" t="s">
@@ -3159,11 +3159,11 @@
       <c r="AH30" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="AI30" s="2">
-        <v>1</v>
+      <c r="AI30" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="AJ30" s="3"/>
-      <c r="AK30" s="27" t="s">
+      <c r="AK30" s="24" t="s">
         <v>15</v>
       </c>
       <c r="AL30" s="6" t="s">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
-      <c r="AG31" s="27" t="s">
+      <c r="AG31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="AH31" s="6" t="s">
@@ -3253,7 +3253,7 @@
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
       <c r="AF32" s="8"/>
-      <c r="AG32" s="27" t="s">
+      <c r="AG32" s="24" t="s">
         <v>15</v>
       </c>
       <c r="AH32" s="6" t="s">

</xml_diff>